<commit_message>
Changes to support new figures
In the future, it might be best to completely isolate figure generation from the other calculations.
</commit_message>
<xml_diff>
--- a/RunSummaries.xlsx
+++ b/RunSummaries.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>rcp60</t>
+  </si>
+  <si>
+    <t>rcp85</t>
   </si>
 </sst>
 </file>
@@ -443,10 +446,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:P13"/>
+      <selection activeCell="A23" sqref="A23:P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,6 +1104,506 @@
         <v>4.7156000000000002</v>
       </c>
     </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>42945.580775462964</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1000</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>10.197927302969147</v>
+      </c>
+      <c r="G14">
+        <v>9.615384615384615</v>
+      </c>
+      <c r="H14">
+        <v>0.3</v>
+      </c>
+      <c r="I14">
+        <v>0.1</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>0.36</v>
+      </c>
+      <c r="N14">
+        <v>1.5</v>
+      </c>
+      <c r="O14">
+        <v>0.46</v>
+      </c>
+      <c r="P14">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>42945.733703703707</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1000</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>19.929067068743567</v>
+      </c>
+      <c r="G15">
+        <v>9.615384615384615</v>
+      </c>
+      <c r="H15">
+        <v>0.3</v>
+      </c>
+      <c r="I15">
+        <v>0.1</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>0.36</v>
+      </c>
+      <c r="N15">
+        <v>1.5</v>
+      </c>
+      <c r="O15">
+        <v>0.46</v>
+      </c>
+      <c r="P15">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>42945.743715277778</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1000</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>5.336427200732647</v>
+      </c>
+      <c r="G16">
+        <v>9.615384615384615</v>
+      </c>
+      <c r="H16">
+        <v>0.3</v>
+      </c>
+      <c r="I16">
+        <v>0.1</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>0.36</v>
+      </c>
+      <c r="N16">
+        <v>1.5</v>
+      </c>
+      <c r="O16">
+        <v>0.46</v>
+      </c>
+      <c r="P16">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>42945.744398148148</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1000</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>5.0318168305917208</v>
+      </c>
+      <c r="G17">
+        <v>9.615384615384615</v>
+      </c>
+      <c r="H17">
+        <v>0.3</v>
+      </c>
+      <c r="I17">
+        <v>0.1</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>0.36</v>
+      </c>
+      <c r="N17">
+        <v>1.5</v>
+      </c>
+      <c r="O17">
+        <v>0.46</v>
+      </c>
+      <c r="P17">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>42945.752025462964</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1000</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>12.080413886628522</v>
+      </c>
+      <c r="G18">
+        <v>13.01775147928994</v>
+      </c>
+      <c r="H18">
+        <v>0.3</v>
+      </c>
+      <c r="I18">
+        <v>0.1</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>0.36</v>
+      </c>
+      <c r="N18">
+        <v>1.5</v>
+      </c>
+      <c r="O18">
+        <v>0.46</v>
+      </c>
+      <c r="P18">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>42945.752662037034</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1000</v>
+      </c>
+      <c r="E19">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>7.3886378930385428</v>
+      </c>
+      <c r="G19">
+        <v>13.01775147928994</v>
+      </c>
+      <c r="H19">
+        <v>0.3</v>
+      </c>
+      <c r="I19">
+        <v>0.1</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+      <c r="M19">
+        <v>0.36</v>
+      </c>
+      <c r="N19">
+        <v>1.5</v>
+      </c>
+      <c r="O19">
+        <v>0.46</v>
+      </c>
+      <c r="P19">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>42945.759548611109</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1000</v>
+      </c>
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>6.8727726762635646</v>
+      </c>
+      <c r="G20">
+        <v>11.834319526627219</v>
+      </c>
+      <c r="H20">
+        <v>0.3</v>
+      </c>
+      <c r="I20">
+        <v>0.1</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>0.36</v>
+      </c>
+      <c r="N20">
+        <v>1.5</v>
+      </c>
+      <c r="O20">
+        <v>0.46</v>
+      </c>
+      <c r="P20">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>42945.759872685187</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1000</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>6.5432937176231087</v>
+      </c>
+      <c r="G21">
+        <v>11.538461538461538</v>
+      </c>
+      <c r="H21">
+        <v>0.3</v>
+      </c>
+      <c r="I21">
+        <v>0.1</v>
+      </c>
+      <c r="J21">
+        <v>4</v>
+      </c>
+      <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21">
+        <v>0.36</v>
+      </c>
+      <c r="N21">
+        <v>1.5</v>
+      </c>
+      <c r="O21">
+        <v>0.46</v>
+      </c>
+      <c r="P21">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>42945.922500000001</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1000</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>24.113477714523054</v>
+      </c>
+      <c r="G22">
+        <v>11.538461538461538</v>
+      </c>
+      <c r="H22">
+        <v>0.3</v>
+      </c>
+      <c r="I22">
+        <v>0.1</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>0.36</v>
+      </c>
+      <c r="N22">
+        <v>1.5</v>
+      </c>
+      <c r="O22">
+        <v>0.46</v>
+      </c>
+      <c r="P22">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>42945.923935185187</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1000</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>5.4166161350635358</v>
+      </c>
+      <c r="G23">
+        <v>8.6538461538461533</v>
+      </c>
+      <c r="H23">
+        <v>0.3</v>
+      </c>
+      <c r="I23">
+        <v>0.1</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>0.36</v>
+      </c>
+      <c r="N23">
+        <v>1.5</v>
+      </c>
+      <c r="O23">
+        <v>0.46</v>
+      </c>
+      <c r="P23">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Stats update for Stress History
This changes the logic for which combinations of stress to massive and branching corals count as serious stress.  The other changes are mostly to plotting tools.
</commit_message>
<xml_diff>
--- a/RunSummaries.xlsx
+++ b/RunSummaries.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>rcp85</t>
+  </si>
+  <si>
+    <t>rcp26</t>
+  </si>
+  <si>
+    <t>rcp45</t>
   </si>
 </sst>
 </file>
@@ -446,10 +452,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:P23"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98:P98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,6 +1610,3756 @@
         <v>4.7156000000000002</v>
       </c>
     </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>42948.518310185187</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>10000</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>19.151348426459808</v>
+      </c>
+      <c r="G24">
+        <v>1.2820512820512822</v>
+      </c>
+      <c r="H24">
+        <v>0.3</v>
+      </c>
+      <c r="I24">
+        <v>0.1</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
+      </c>
+      <c r="M24">
+        <v>0.36</v>
+      </c>
+      <c r="N24">
+        <v>1.5</v>
+      </c>
+      <c r="O24">
+        <v>0.46</v>
+      </c>
+      <c r="P24">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>42948.520636574074</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>10000</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>5.6688680987121316</v>
+      </c>
+      <c r="G25">
+        <v>1.2820512820512822</v>
+      </c>
+      <c r="H25">
+        <v>0.3</v>
+      </c>
+      <c r="I25">
+        <v>0.1</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <v>2</v>
+      </c>
+      <c r="M25">
+        <v>0.36</v>
+      </c>
+      <c r="N25">
+        <v>1.5</v>
+      </c>
+      <c r="O25">
+        <v>0.46</v>
+      </c>
+      <c r="P25">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>42948.546724537038</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>10000</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>4.7194404507778502</v>
+      </c>
+      <c r="G26">
+        <v>1.2820512820512822</v>
+      </c>
+      <c r="H26">
+        <v>0.3</v>
+      </c>
+      <c r="I26">
+        <v>0.1</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+      <c r="K26">
+        <v>4</v>
+      </c>
+      <c r="L26">
+        <v>2</v>
+      </c>
+      <c r="M26">
+        <v>0.36</v>
+      </c>
+      <c r="N26">
+        <v>1.5</v>
+      </c>
+      <c r="O26">
+        <v>0.46</v>
+      </c>
+      <c r="P26">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>42948.547789351855</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>10000</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>4.5057123209689847</v>
+      </c>
+      <c r="G27">
+        <v>1.2820512820512822</v>
+      </c>
+      <c r="H27">
+        <v>0.3</v>
+      </c>
+      <c r="I27">
+        <v>0.1</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="M27">
+        <v>0.36</v>
+      </c>
+      <c r="N27">
+        <v>1.5</v>
+      </c>
+      <c r="O27">
+        <v>0.46</v>
+      </c>
+      <c r="P27">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>42948.553784722222</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>10000</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>11.121917885806059</v>
+      </c>
+      <c r="G28">
+        <v>1.2820512820512822</v>
+      </c>
+      <c r="H28">
+        <v>0.3</v>
+      </c>
+      <c r="I28">
+        <v>0.1</v>
+      </c>
+      <c r="J28">
+        <v>4</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <v>2</v>
+      </c>
+      <c r="M28">
+        <v>0.36</v>
+      </c>
+      <c r="N28">
+        <v>1.5</v>
+      </c>
+      <c r="O28">
+        <v>0.46</v>
+      </c>
+      <c r="P28">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>42948.578252314815</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>10000</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>5.731394357981074</v>
+      </c>
+      <c r="G29">
+        <v>1.2820512820512822</v>
+      </c>
+      <c r="H29">
+        <v>0.3</v>
+      </c>
+      <c r="I29">
+        <v>0.1</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+      <c r="K29">
+        <v>4</v>
+      </c>
+      <c r="L29">
+        <v>2</v>
+      </c>
+      <c r="M29">
+        <v>0.36</v>
+      </c>
+      <c r="N29">
+        <v>1.5</v>
+      </c>
+      <c r="O29">
+        <v>0.46</v>
+      </c>
+      <c r="P29">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>42948.579594907409</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>10000</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>5.8572270147999079</v>
+      </c>
+      <c r="G30">
+        <v>1.2820512820512822</v>
+      </c>
+      <c r="H30">
+        <v>0.3</v>
+      </c>
+      <c r="I30">
+        <v>0.1</v>
+      </c>
+      <c r="J30">
+        <v>4</v>
+      </c>
+      <c r="K30">
+        <v>4</v>
+      </c>
+      <c r="L30">
+        <v>2</v>
+      </c>
+      <c r="M30">
+        <v>0.36</v>
+      </c>
+      <c r="N30">
+        <v>1.5</v>
+      </c>
+      <c r="O30">
+        <v>0.46</v>
+      </c>
+      <c r="P30">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>42948.580474537041</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>10000</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>5.6712568322097914</v>
+      </c>
+      <c r="G31">
+        <v>1.2820512820512822</v>
+      </c>
+      <c r="H31">
+        <v>0.3</v>
+      </c>
+      <c r="I31">
+        <v>0.1</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
+      </c>
+      <c r="K31">
+        <v>4</v>
+      </c>
+      <c r="L31">
+        <v>2</v>
+      </c>
+      <c r="M31">
+        <v>0.36</v>
+      </c>
+      <c r="N31">
+        <v>1.5</v>
+      </c>
+      <c r="O31">
+        <v>0.46</v>
+      </c>
+      <c r="P31">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>42948.581018518518</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>10000</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>5.8272342497984857</v>
+      </c>
+      <c r="G32">
+        <v>1.2820512820512822</v>
+      </c>
+      <c r="H32">
+        <v>0.3</v>
+      </c>
+      <c r="I32">
+        <v>0.1</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>2</v>
+      </c>
+      <c r="M32">
+        <v>0.36</v>
+      </c>
+      <c r="N32">
+        <v>1.5</v>
+      </c>
+      <c r="O32">
+        <v>0.46</v>
+      </c>
+      <c r="P32">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>42948.587685185186</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>10000</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>15.350285288057581</v>
+      </c>
+      <c r="G33">
+        <v>1.2820512820512822</v>
+      </c>
+      <c r="H33">
+        <v>0.3</v>
+      </c>
+      <c r="I33">
+        <v>0.1</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+      <c r="K33">
+        <v>4</v>
+      </c>
+      <c r="L33">
+        <v>2</v>
+      </c>
+      <c r="M33">
+        <v>0.36</v>
+      </c>
+      <c r="N33">
+        <v>1.5</v>
+      </c>
+      <c r="O33">
+        <v>0.46</v>
+      </c>
+      <c r="P33">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>42948.591168981482</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>10000</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>5.8492595566139443</v>
+      </c>
+      <c r="G34">
+        <v>1.2820512820512822</v>
+      </c>
+      <c r="H34">
+        <v>0.3</v>
+      </c>
+      <c r="I34">
+        <v>0.1</v>
+      </c>
+      <c r="J34">
+        <v>4</v>
+      </c>
+      <c r="K34">
+        <v>4</v>
+      </c>
+      <c r="L34">
+        <v>2</v>
+      </c>
+      <c r="M34">
+        <v>0.36</v>
+      </c>
+      <c r="N34">
+        <v>1.5</v>
+      </c>
+      <c r="O34">
+        <v>0.46</v>
+      </c>
+      <c r="P34">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>42948.593113425923</v>
+      </c>
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>10000</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>5.6098444619301802</v>
+      </c>
+      <c r="G35">
+        <v>1.2820512820512822</v>
+      </c>
+      <c r="H35">
+        <v>0.3</v>
+      </c>
+      <c r="I35">
+        <v>0.1</v>
+      </c>
+      <c r="J35">
+        <v>4</v>
+      </c>
+      <c r="K35">
+        <v>4</v>
+      </c>
+      <c r="L35">
+        <v>2</v>
+      </c>
+      <c r="M35">
+        <v>0.36</v>
+      </c>
+      <c r="N35">
+        <v>1.5</v>
+      </c>
+      <c r="O35">
+        <v>0.46</v>
+      </c>
+      <c r="P35">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>42948.764282407406</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>10000</v>
+      </c>
+      <c r="E36">
+        <v>8</v>
+      </c>
+      <c r="F36">
+        <v>32.657379138564785</v>
+      </c>
+      <c r="G36">
+        <v>4.9145299145299139</v>
+      </c>
+      <c r="H36">
+        <v>0.3</v>
+      </c>
+      <c r="I36">
+        <v>0.1</v>
+      </c>
+      <c r="J36">
+        <v>4</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <v>2</v>
+      </c>
+      <c r="M36">
+        <v>0.36</v>
+      </c>
+      <c r="N36">
+        <v>1.5</v>
+      </c>
+      <c r="O36">
+        <v>0.46</v>
+      </c>
+      <c r="P36">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>42948.900358796294</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>10000</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>19.955785870921353</v>
+      </c>
+      <c r="G37">
+        <v>11.538461538461538</v>
+      </c>
+      <c r="H37">
+        <v>0.3</v>
+      </c>
+      <c r="I37">
+        <v>0.1</v>
+      </c>
+      <c r="J37">
+        <v>4</v>
+      </c>
+      <c r="K37">
+        <v>4</v>
+      </c>
+      <c r="L37">
+        <v>2</v>
+      </c>
+      <c r="M37">
+        <v>0.36</v>
+      </c>
+      <c r="N37">
+        <v>1.5</v>
+      </c>
+      <c r="O37">
+        <v>0.46</v>
+      </c>
+      <c r="P37">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>42950.620891203704</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>20</v>
+      </c>
+      <c r="E38">
+        <v>8</v>
+      </c>
+      <c r="F38">
+        <v>42.516463701650544</v>
+      </c>
+      <c r="G38">
+        <v>5.575158786167961</v>
+      </c>
+      <c r="H38">
+        <v>0.3</v>
+      </c>
+      <c r="I38">
+        <v>0.1</v>
+      </c>
+      <c r="J38">
+        <v>4</v>
+      </c>
+      <c r="K38">
+        <v>4</v>
+      </c>
+      <c r="L38">
+        <v>2</v>
+      </c>
+      <c r="M38">
+        <v>0.36</v>
+      </c>
+      <c r="N38">
+        <v>1.5</v>
+      </c>
+      <c r="O38">
+        <v>0.46</v>
+      </c>
+      <c r="P38">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>42950.623182870368</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>20</v>
+      </c>
+      <c r="E39">
+        <v>8</v>
+      </c>
+      <c r="F39">
+        <v>20.428312235787356</v>
+      </c>
+      <c r="G39">
+        <v>5.575158786167961</v>
+      </c>
+      <c r="H39">
+        <v>0.3</v>
+      </c>
+      <c r="I39">
+        <v>0.1</v>
+      </c>
+      <c r="J39">
+        <v>4</v>
+      </c>
+      <c r="K39">
+        <v>4</v>
+      </c>
+      <c r="L39">
+        <v>2</v>
+      </c>
+      <c r="M39">
+        <v>0.36</v>
+      </c>
+      <c r="N39">
+        <v>1.5</v>
+      </c>
+      <c r="O39">
+        <v>0.46</v>
+      </c>
+      <c r="P39">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>42950.623900462961</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>20</v>
+      </c>
+      <c r="E40">
+        <v>8</v>
+      </c>
+      <c r="F40">
+        <v>19.434780535709887</v>
+      </c>
+      <c r="G40">
+        <v>5.575158786167961</v>
+      </c>
+      <c r="H40">
+        <v>0.3</v>
+      </c>
+      <c r="I40">
+        <v>0.1</v>
+      </c>
+      <c r="J40">
+        <v>4</v>
+      </c>
+      <c r="K40">
+        <v>4</v>
+      </c>
+      <c r="L40">
+        <v>2</v>
+      </c>
+      <c r="M40">
+        <v>0.36</v>
+      </c>
+      <c r="N40">
+        <v>1.5</v>
+      </c>
+      <c r="O40">
+        <v>0.46</v>
+      </c>
+      <c r="P40">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>42950.628275462965</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>20</v>
+      </c>
+      <c r="E41">
+        <v>8</v>
+      </c>
+      <c r="F41">
+        <v>21.089719422211285</v>
+      </c>
+      <c r="G41">
+        <v>5.575158786167961</v>
+      </c>
+      <c r="H41">
+        <v>0.3</v>
+      </c>
+      <c r="I41">
+        <v>0.1</v>
+      </c>
+      <c r="J41">
+        <v>4</v>
+      </c>
+      <c r="K41">
+        <v>4</v>
+      </c>
+      <c r="L41">
+        <v>2</v>
+      </c>
+      <c r="M41">
+        <v>0.36</v>
+      </c>
+      <c r="N41">
+        <v>1.5</v>
+      </c>
+      <c r="O41">
+        <v>0.46</v>
+      </c>
+      <c r="P41">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>42950.646331018521</v>
+      </c>
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>20</v>
+      </c>
+      <c r="E42">
+        <v>8</v>
+      </c>
+      <c r="F42">
+        <v>28.311024301083457</v>
+      </c>
+      <c r="G42">
+        <v>5.457875457875458</v>
+      </c>
+      <c r="H42">
+        <v>0.3</v>
+      </c>
+      <c r="I42">
+        <v>0.1</v>
+      </c>
+      <c r="J42">
+        <v>4</v>
+      </c>
+      <c r="K42">
+        <v>4</v>
+      </c>
+      <c r="L42">
+        <v>2</v>
+      </c>
+      <c r="M42">
+        <v>0.36</v>
+      </c>
+      <c r="N42">
+        <v>1.5</v>
+      </c>
+      <c r="O42">
+        <v>0.46</v>
+      </c>
+      <c r="P42">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42950.647256944445</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>20</v>
+      </c>
+      <c r="E43">
+        <v>8</v>
+      </c>
+      <c r="F43">
+        <v>22.765830839269434</v>
+      </c>
+      <c r="G43">
+        <v>5.457875457875458</v>
+      </c>
+      <c r="H43">
+        <v>0.3</v>
+      </c>
+      <c r="I43">
+        <v>0.1</v>
+      </c>
+      <c r="J43">
+        <v>4</v>
+      </c>
+      <c r="K43">
+        <v>4</v>
+      </c>
+      <c r="L43">
+        <v>2</v>
+      </c>
+      <c r="M43">
+        <v>0.36</v>
+      </c>
+      <c r="N43">
+        <v>1.5</v>
+      </c>
+      <c r="O43">
+        <v>0.46</v>
+      </c>
+      <c r="P43">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>42950.651423611111</v>
+      </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>20</v>
+      </c>
+      <c r="E44">
+        <v>8</v>
+      </c>
+      <c r="F44">
+        <v>22.221955100769996</v>
+      </c>
+      <c r="G44">
+        <v>5.457875457875458</v>
+      </c>
+      <c r="H44">
+        <v>0.3</v>
+      </c>
+      <c r="I44">
+        <v>0.1</v>
+      </c>
+      <c r="J44">
+        <v>4</v>
+      </c>
+      <c r="K44">
+        <v>4</v>
+      </c>
+      <c r="L44">
+        <v>2</v>
+      </c>
+      <c r="M44">
+        <v>0.36</v>
+      </c>
+      <c r="N44">
+        <v>1.5</v>
+      </c>
+      <c r="O44">
+        <v>0.46</v>
+      </c>
+      <c r="P44">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>42950.65388888889</v>
+      </c>
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>20</v>
+      </c>
+      <c r="E45">
+        <v>8</v>
+      </c>
+      <c r="F45">
+        <v>22.490358508419124</v>
+      </c>
+      <c r="G45">
+        <v>5.457875457875458</v>
+      </c>
+      <c r="H45">
+        <v>0.3</v>
+      </c>
+      <c r="I45">
+        <v>0.1</v>
+      </c>
+      <c r="J45">
+        <v>4</v>
+      </c>
+      <c r="K45">
+        <v>4</v>
+      </c>
+      <c r="L45">
+        <v>2</v>
+      </c>
+      <c r="M45">
+        <v>0.36</v>
+      </c>
+      <c r="N45">
+        <v>1.5</v>
+      </c>
+      <c r="O45">
+        <v>0.46</v>
+      </c>
+      <c r="P45">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>42950.655497685184</v>
+      </c>
+      <c r="B46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>20</v>
+      </c>
+      <c r="E46">
+        <v>8</v>
+      </c>
+      <c r="F46">
+        <v>23.075022871363263</v>
+      </c>
+      <c r="G46">
+        <v>5.457875457875458</v>
+      </c>
+      <c r="H46">
+        <v>0.3</v>
+      </c>
+      <c r="I46">
+        <v>0.1</v>
+      </c>
+      <c r="J46">
+        <v>4</v>
+      </c>
+      <c r="K46">
+        <v>4</v>
+      </c>
+      <c r="L46">
+        <v>2</v>
+      </c>
+      <c r="M46">
+        <v>0.36</v>
+      </c>
+      <c r="N46">
+        <v>1.5</v>
+      </c>
+      <c r="O46">
+        <v>0.46</v>
+      </c>
+      <c r="P46">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>42950.656944444447</v>
+      </c>
+      <c r="B47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>8</v>
+      </c>
+      <c r="F47">
+        <v>33.542326021643561</v>
+      </c>
+      <c r="G47">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H47">
+        <v>0.3</v>
+      </c>
+      <c r="I47">
+        <v>0.1</v>
+      </c>
+      <c r="J47">
+        <v>4</v>
+      </c>
+      <c r="K47">
+        <v>4</v>
+      </c>
+      <c r="L47">
+        <v>2</v>
+      </c>
+      <c r="M47">
+        <v>0.36</v>
+      </c>
+      <c r="N47">
+        <v>1.5</v>
+      </c>
+      <c r="O47">
+        <v>0.46</v>
+      </c>
+      <c r="P47">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>42950.665219907409</v>
+      </c>
+      <c r="B48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>8</v>
+      </c>
+      <c r="F48">
+        <v>309.79539385623502</v>
+      </c>
+      <c r="G48">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H48">
+        <v>0.3</v>
+      </c>
+      <c r="I48">
+        <v>0.1</v>
+      </c>
+      <c r="J48">
+        <v>4</v>
+      </c>
+      <c r="K48">
+        <v>4</v>
+      </c>
+      <c r="L48">
+        <v>2</v>
+      </c>
+      <c r="M48">
+        <v>0.36</v>
+      </c>
+      <c r="N48">
+        <v>1.5</v>
+      </c>
+      <c r="O48">
+        <v>0.46</v>
+      </c>
+      <c r="P48">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>42950.674722222226</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>8</v>
+      </c>
+      <c r="F49">
+        <v>23.531067135090961</v>
+      </c>
+      <c r="G49">
+        <v>4.9930069930069925</v>
+      </c>
+      <c r="H49">
+        <v>0.3</v>
+      </c>
+      <c r="I49">
+        <v>0.1</v>
+      </c>
+      <c r="J49">
+        <v>4</v>
+      </c>
+      <c r="K49">
+        <v>4</v>
+      </c>
+      <c r="L49">
+        <v>2</v>
+      </c>
+      <c r="M49">
+        <v>0.36</v>
+      </c>
+      <c r="N49">
+        <v>1.5</v>
+      </c>
+      <c r="O49">
+        <v>0.46</v>
+      </c>
+      <c r="P49">
+        <v>4.1849999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>42950.67496527778</v>
+      </c>
+      <c r="B50" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>8</v>
+      </c>
+      <c r="F50">
+        <v>19.611533694901933</v>
+      </c>
+      <c r="G50">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H50">
+        <v>0.3</v>
+      </c>
+      <c r="I50">
+        <v>0.1</v>
+      </c>
+      <c r="J50">
+        <v>4</v>
+      </c>
+      <c r="K50">
+        <v>4</v>
+      </c>
+      <c r="L50">
+        <v>2</v>
+      </c>
+      <c r="M50">
+        <v>0.36</v>
+      </c>
+      <c r="N50">
+        <v>1.5</v>
+      </c>
+      <c r="O50">
+        <v>0.46</v>
+      </c>
+      <c r="P50">
+        <v>4.3616999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>42950.675196759257</v>
+      </c>
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>8</v>
+      </c>
+      <c r="F51">
+        <v>18.241380159976345</v>
+      </c>
+      <c r="G51">
+        <v>5.0009990009990011</v>
+      </c>
+      <c r="H51">
+        <v>0.3</v>
+      </c>
+      <c r="I51">
+        <v>0.1</v>
+      </c>
+      <c r="J51">
+        <v>4</v>
+      </c>
+      <c r="K51">
+        <v>4</v>
+      </c>
+      <c r="L51">
+        <v>2</v>
+      </c>
+      <c r="M51">
+        <v>0.36</v>
+      </c>
+      <c r="N51">
+        <v>1.5</v>
+      </c>
+      <c r="O51">
+        <v>0.46</v>
+      </c>
+      <c r="P51">
+        <v>4.2077</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>42950.675428240742</v>
+      </c>
+      <c r="B52" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>8</v>
+      </c>
+      <c r="F52">
+        <v>18.208555473815608</v>
+      </c>
+      <c r="G52">
+        <v>4.9870129870129869</v>
+      </c>
+      <c r="H52">
+        <v>0.3</v>
+      </c>
+      <c r="I52">
+        <v>0.1</v>
+      </c>
+      <c r="J52">
+        <v>4</v>
+      </c>
+      <c r="K52">
+        <v>4</v>
+      </c>
+      <c r="L52">
+        <v>2</v>
+      </c>
+      <c r="M52">
+        <v>0.36</v>
+      </c>
+      <c r="N52">
+        <v>1.5</v>
+      </c>
+      <c r="O52">
+        <v>0.46</v>
+      </c>
+      <c r="P52">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>42950.67564814815</v>
+      </c>
+      <c r="B53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>8</v>
+      </c>
+      <c r="F53">
+        <v>18.049780374114384</v>
+      </c>
+      <c r="G53">
+        <v>4.9870129870129869</v>
+      </c>
+      <c r="H53">
+        <v>0.3</v>
+      </c>
+      <c r="I53">
+        <v>0.1</v>
+      </c>
+      <c r="J53">
+        <v>4</v>
+      </c>
+      <c r="K53">
+        <v>4</v>
+      </c>
+      <c r="L53">
+        <v>2</v>
+      </c>
+      <c r="M53">
+        <v>0.36</v>
+      </c>
+      <c r="N53">
+        <v>1.5</v>
+      </c>
+      <c r="O53">
+        <v>0.46</v>
+      </c>
+      <c r="P53">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>42950.675879629627</v>
+      </c>
+      <c r="B54" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>8</v>
+      </c>
+      <c r="F54">
+        <v>18.293084320532515</v>
+      </c>
+      <c r="G54">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H54">
+        <v>0.3</v>
+      </c>
+      <c r="I54">
+        <v>0.1</v>
+      </c>
+      <c r="J54">
+        <v>4</v>
+      </c>
+      <c r="K54">
+        <v>4</v>
+      </c>
+      <c r="L54">
+        <v>2</v>
+      </c>
+      <c r="M54">
+        <v>0.36</v>
+      </c>
+      <c r="N54">
+        <v>1.5</v>
+      </c>
+      <c r="O54">
+        <v>0.46</v>
+      </c>
+      <c r="P54">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>42950.676111111112</v>
+      </c>
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>8</v>
+      </c>
+      <c r="F55">
+        <v>18.041409407162103</v>
+      </c>
+      <c r="G55">
+        <v>4.9950049950049946</v>
+      </c>
+      <c r="H55">
+        <v>0.3</v>
+      </c>
+      <c r="I55">
+        <v>0.1</v>
+      </c>
+      <c r="J55">
+        <v>4</v>
+      </c>
+      <c r="K55">
+        <v>4</v>
+      </c>
+      <c r="L55">
+        <v>2</v>
+      </c>
+      <c r="M55">
+        <v>0.36</v>
+      </c>
+      <c r="N55">
+        <v>1.5</v>
+      </c>
+      <c r="O55">
+        <v>0.46</v>
+      </c>
+      <c r="P55">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>42950.67633101852</v>
+      </c>
+      <c r="B56" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>8</v>
+      </c>
+      <c r="F56">
+        <v>17.956479611607612</v>
+      </c>
+      <c r="G56">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H56">
+        <v>0.3</v>
+      </c>
+      <c r="I56">
+        <v>0.1</v>
+      </c>
+      <c r="J56">
+        <v>4</v>
+      </c>
+      <c r="K56">
+        <v>4</v>
+      </c>
+      <c r="L56">
+        <v>2</v>
+      </c>
+      <c r="M56">
+        <v>0.36</v>
+      </c>
+      <c r="N56">
+        <v>1.5</v>
+      </c>
+      <c r="O56">
+        <v>0.46</v>
+      </c>
+      <c r="P56">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>42950.676562499997</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>8</v>
+      </c>
+      <c r="F57">
+        <v>18.044715875110036</v>
+      </c>
+      <c r="G57">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H57">
+        <v>0.3</v>
+      </c>
+      <c r="I57">
+        <v>0.1</v>
+      </c>
+      <c r="J57">
+        <v>4</v>
+      </c>
+      <c r="K57">
+        <v>4</v>
+      </c>
+      <c r="L57">
+        <v>2</v>
+      </c>
+      <c r="M57">
+        <v>0.36</v>
+      </c>
+      <c r="N57">
+        <v>1.5</v>
+      </c>
+      <c r="O57">
+        <v>0.46</v>
+      </c>
+      <c r="P57">
+        <v>4.1849999999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>42950.676782407405</v>
+      </c>
+      <c r="B58" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>8</v>
+      </c>
+      <c r="F58">
+        <v>18.023171514905027</v>
+      </c>
+      <c r="G58">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H58">
+        <v>0.3</v>
+      </c>
+      <c r="I58">
+        <v>0.1</v>
+      </c>
+      <c r="J58">
+        <v>4</v>
+      </c>
+      <c r="K58">
+        <v>4</v>
+      </c>
+      <c r="L58">
+        <v>2</v>
+      </c>
+      <c r="M58">
+        <v>0.36</v>
+      </c>
+      <c r="N58">
+        <v>1.5</v>
+      </c>
+      <c r="O58">
+        <v>0.46</v>
+      </c>
+      <c r="P58">
+        <v>4.3616999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>42950.67701388889</v>
+      </c>
+      <c r="B59" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>8</v>
+      </c>
+      <c r="F59">
+        <v>18.040013606021208</v>
+      </c>
+      <c r="G59">
+        <v>5.0009990009990011</v>
+      </c>
+      <c r="H59">
+        <v>0.3</v>
+      </c>
+      <c r="I59">
+        <v>0.1</v>
+      </c>
+      <c r="J59">
+        <v>4</v>
+      </c>
+      <c r="K59">
+        <v>4</v>
+      </c>
+      <c r="L59">
+        <v>2</v>
+      </c>
+      <c r="M59">
+        <v>0.36</v>
+      </c>
+      <c r="N59">
+        <v>1.5</v>
+      </c>
+      <c r="O59">
+        <v>0.46</v>
+      </c>
+      <c r="P59">
+        <v>4.2077</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>42950.677245370367</v>
+      </c>
+      <c r="B60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>8</v>
+      </c>
+      <c r="F60">
+        <v>18.100111452897153</v>
+      </c>
+      <c r="G60">
+        <v>4.9850149850149847</v>
+      </c>
+      <c r="H60">
+        <v>0.3</v>
+      </c>
+      <c r="I60">
+        <v>0.1</v>
+      </c>
+      <c r="J60">
+        <v>4</v>
+      </c>
+      <c r="K60">
+        <v>4</v>
+      </c>
+      <c r="L60">
+        <v>2</v>
+      </c>
+      <c r="M60">
+        <v>0.36</v>
+      </c>
+      <c r="N60">
+        <v>1.5</v>
+      </c>
+      <c r="O60">
+        <v>0.46</v>
+      </c>
+      <c r="P60">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>42950.677465277775</v>
+      </c>
+      <c r="B61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>8</v>
+      </c>
+      <c r="F61">
+        <v>17.996418339713422</v>
+      </c>
+      <c r="G61">
+        <v>5.0109890109890109</v>
+      </c>
+      <c r="H61">
+        <v>0.3</v>
+      </c>
+      <c r="I61">
+        <v>0.1</v>
+      </c>
+      <c r="J61">
+        <v>4</v>
+      </c>
+      <c r="K61">
+        <v>4</v>
+      </c>
+      <c r="L61">
+        <v>2</v>
+      </c>
+      <c r="M61">
+        <v>0.36</v>
+      </c>
+      <c r="N61">
+        <v>1.5</v>
+      </c>
+      <c r="O61">
+        <v>0.46</v>
+      </c>
+      <c r="P61">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>42950.67769675926</v>
+      </c>
+      <c r="B62" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>8</v>
+      </c>
+      <c r="F62">
+        <v>18.05337675399117</v>
+      </c>
+      <c r="G62">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H62">
+        <v>0.3</v>
+      </c>
+      <c r="I62">
+        <v>0.1</v>
+      </c>
+      <c r="J62">
+        <v>4</v>
+      </c>
+      <c r="K62">
+        <v>4</v>
+      </c>
+      <c r="L62">
+        <v>2</v>
+      </c>
+      <c r="M62">
+        <v>0.36</v>
+      </c>
+      <c r="N62">
+        <v>1.5</v>
+      </c>
+      <c r="O62">
+        <v>0.46</v>
+      </c>
+      <c r="P62">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>42950.677916666667</v>
+      </c>
+      <c r="B63" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>8</v>
+      </c>
+      <c r="F63">
+        <v>18.03355650578688</v>
+      </c>
+      <c r="G63">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H63">
+        <v>0.3</v>
+      </c>
+      <c r="I63">
+        <v>0.1</v>
+      </c>
+      <c r="J63">
+        <v>4</v>
+      </c>
+      <c r="K63">
+        <v>4</v>
+      </c>
+      <c r="L63">
+        <v>2</v>
+      </c>
+      <c r="M63">
+        <v>0.36</v>
+      </c>
+      <c r="N63">
+        <v>1.5</v>
+      </c>
+      <c r="O63">
+        <v>0.46</v>
+      </c>
+      <c r="P63">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>42950.678148148145</v>
+      </c>
+      <c r="B64" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>8</v>
+      </c>
+      <c r="F64">
+        <v>17.936061620044498</v>
+      </c>
+      <c r="G64">
+        <v>5.0009990009990011</v>
+      </c>
+      <c r="H64">
+        <v>0.3</v>
+      </c>
+      <c r="I64">
+        <v>0.1</v>
+      </c>
+      <c r="J64">
+        <v>4</v>
+      </c>
+      <c r="K64">
+        <v>4</v>
+      </c>
+      <c r="L64">
+        <v>2</v>
+      </c>
+      <c r="M64">
+        <v>0.36</v>
+      </c>
+      <c r="N64">
+        <v>1.5</v>
+      </c>
+      <c r="O64">
+        <v>0.46</v>
+      </c>
+      <c r="P64">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>42950.683749999997</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>8</v>
+      </c>
+      <c r="F65">
+        <v>19.028563044804834</v>
+      </c>
+      <c r="G65">
+        <v>4.9930069930069925</v>
+      </c>
+      <c r="H65">
+        <v>0.3</v>
+      </c>
+      <c r="I65">
+        <v>0.1</v>
+      </c>
+      <c r="J65">
+        <v>4</v>
+      </c>
+      <c r="K65">
+        <v>4</v>
+      </c>
+      <c r="L65">
+        <v>2</v>
+      </c>
+      <c r="M65">
+        <v>0.36</v>
+      </c>
+      <c r="N65">
+        <v>1.5</v>
+      </c>
+      <c r="O65">
+        <v>0.46</v>
+      </c>
+      <c r="P65">
+        <v>4.1849999999999996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>42950.683993055558</v>
+      </c>
+      <c r="B66" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>8</v>
+      </c>
+      <c r="F66">
+        <v>18.776473102988813</v>
+      </c>
+      <c r="G66">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H66">
+        <v>0.3</v>
+      </c>
+      <c r="I66">
+        <v>0.1</v>
+      </c>
+      <c r="J66">
+        <v>4</v>
+      </c>
+      <c r="K66">
+        <v>4</v>
+      </c>
+      <c r="L66">
+        <v>2</v>
+      </c>
+      <c r="M66">
+        <v>0.36</v>
+      </c>
+      <c r="N66">
+        <v>1.5</v>
+      </c>
+      <c r="O66">
+        <v>0.46</v>
+      </c>
+      <c r="P66">
+        <v>4.3616999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>42950.684212962966</v>
+      </c>
+      <c r="B67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>8</v>
+      </c>
+      <c r="F67">
+        <v>18.263416986471096</v>
+      </c>
+      <c r="G67">
+        <v>5.0009990009990011</v>
+      </c>
+      <c r="H67">
+        <v>0.3</v>
+      </c>
+      <c r="I67">
+        <v>0.1</v>
+      </c>
+      <c r="J67">
+        <v>4</v>
+      </c>
+      <c r="K67">
+        <v>4</v>
+      </c>
+      <c r="L67">
+        <v>2</v>
+      </c>
+      <c r="M67">
+        <v>0.36</v>
+      </c>
+      <c r="N67">
+        <v>1.5</v>
+      </c>
+      <c r="O67">
+        <v>0.46</v>
+      </c>
+      <c r="P67">
+        <v>4.2077</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>42950.684444444443</v>
+      </c>
+      <c r="B68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>8</v>
+      </c>
+      <c r="F68">
+        <v>18.493792972803636</v>
+      </c>
+      <c r="G68">
+        <v>4.9870129870129869</v>
+      </c>
+      <c r="H68">
+        <v>0.3</v>
+      </c>
+      <c r="I68">
+        <v>0.1</v>
+      </c>
+      <c r="J68">
+        <v>4</v>
+      </c>
+      <c r="K68">
+        <v>4</v>
+      </c>
+      <c r="L68">
+        <v>2</v>
+      </c>
+      <c r="M68">
+        <v>0.36</v>
+      </c>
+      <c r="N68">
+        <v>1.5</v>
+      </c>
+      <c r="O68">
+        <v>0.46</v>
+      </c>
+      <c r="P68">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>42950.684687499997</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>8</v>
+      </c>
+      <c r="F69">
+        <v>18.50474754782827</v>
+      </c>
+      <c r="G69">
+        <v>4.9870129870129869</v>
+      </c>
+      <c r="H69">
+        <v>0.3</v>
+      </c>
+      <c r="I69">
+        <v>0.1</v>
+      </c>
+      <c r="J69">
+        <v>4</v>
+      </c>
+      <c r="K69">
+        <v>4</v>
+      </c>
+      <c r="L69">
+        <v>2</v>
+      </c>
+      <c r="M69">
+        <v>0.36</v>
+      </c>
+      <c r="N69">
+        <v>1.5</v>
+      </c>
+      <c r="O69">
+        <v>0.46</v>
+      </c>
+      <c r="P69">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>42950.684976851851</v>
+      </c>
+      <c r="B70" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>8</v>
+      </c>
+      <c r="F70">
+        <v>24.064077256089192</v>
+      </c>
+      <c r="G70">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H70">
+        <v>0.3</v>
+      </c>
+      <c r="I70">
+        <v>0.1</v>
+      </c>
+      <c r="J70">
+        <v>4</v>
+      </c>
+      <c r="K70">
+        <v>4</v>
+      </c>
+      <c r="L70">
+        <v>2</v>
+      </c>
+      <c r="M70">
+        <v>0.36</v>
+      </c>
+      <c r="N70">
+        <v>1.5</v>
+      </c>
+      <c r="O70">
+        <v>0.46</v>
+      </c>
+      <c r="P70">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>42950.685208333336</v>
+      </c>
+      <c r="B71" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>8</v>
+      </c>
+      <c r="F71">
+        <v>18.430263861454097</v>
+      </c>
+      <c r="G71">
+        <v>4.9950049950049946</v>
+      </c>
+      <c r="H71">
+        <v>0.3</v>
+      </c>
+      <c r="I71">
+        <v>0.1</v>
+      </c>
+      <c r="J71">
+        <v>4</v>
+      </c>
+      <c r="K71">
+        <v>4</v>
+      </c>
+      <c r="L71">
+        <v>2</v>
+      </c>
+      <c r="M71">
+        <v>0.36</v>
+      </c>
+      <c r="N71">
+        <v>1.5</v>
+      </c>
+      <c r="O71">
+        <v>0.46</v>
+      </c>
+      <c r="P71">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>42950.685439814813</v>
+      </c>
+      <c r="B72" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>8</v>
+      </c>
+      <c r="F72">
+        <v>18.363254846985061</v>
+      </c>
+      <c r="G72">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H72">
+        <v>0.3</v>
+      </c>
+      <c r="I72">
+        <v>0.1</v>
+      </c>
+      <c r="J72">
+        <v>4</v>
+      </c>
+      <c r="K72">
+        <v>4</v>
+      </c>
+      <c r="L72">
+        <v>2</v>
+      </c>
+      <c r="M72">
+        <v>0.36</v>
+      </c>
+      <c r="N72">
+        <v>1.5</v>
+      </c>
+      <c r="O72">
+        <v>0.46</v>
+      </c>
+      <c r="P72">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>42950.685960648145</v>
+      </c>
+      <c r="B73" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>8</v>
+      </c>
+      <c r="F73">
+        <v>18.844260655783344</v>
+      </c>
+      <c r="G73">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H73">
+        <v>0.3</v>
+      </c>
+      <c r="I73">
+        <v>0.1</v>
+      </c>
+      <c r="J73">
+        <v>4</v>
+      </c>
+      <c r="K73">
+        <v>4</v>
+      </c>
+      <c r="L73">
+        <v>2</v>
+      </c>
+      <c r="M73">
+        <v>0.36</v>
+      </c>
+      <c r="N73">
+        <v>1.5</v>
+      </c>
+      <c r="O73">
+        <v>0.46</v>
+      </c>
+      <c r="P73">
+        <v>4.1849999999999996</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>42950.686192129629</v>
+      </c>
+      <c r="B74" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>8</v>
+      </c>
+      <c r="F74">
+        <v>18.13469769001631</v>
+      </c>
+      <c r="G74">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H74">
+        <v>0.3</v>
+      </c>
+      <c r="I74">
+        <v>0.1</v>
+      </c>
+      <c r="J74">
+        <v>4</v>
+      </c>
+      <c r="K74">
+        <v>4</v>
+      </c>
+      <c r="L74">
+        <v>2</v>
+      </c>
+      <c r="M74">
+        <v>0.36</v>
+      </c>
+      <c r="N74">
+        <v>1.5</v>
+      </c>
+      <c r="O74">
+        <v>0.46</v>
+      </c>
+      <c r="P74">
+        <v>4.3616999999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>42950.686412037037</v>
+      </c>
+      <c r="B75" t="s">
+        <v>16</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>8</v>
+      </c>
+      <c r="F75">
+        <v>18.329689701438713</v>
+      </c>
+      <c r="G75">
+        <v>5.0009990009990011</v>
+      </c>
+      <c r="H75">
+        <v>0.3</v>
+      </c>
+      <c r="I75">
+        <v>0.1</v>
+      </c>
+      <c r="J75">
+        <v>4</v>
+      </c>
+      <c r="K75">
+        <v>4</v>
+      </c>
+      <c r="L75">
+        <v>2</v>
+      </c>
+      <c r="M75">
+        <v>0.36</v>
+      </c>
+      <c r="N75">
+        <v>1.5</v>
+      </c>
+      <c r="O75">
+        <v>0.46</v>
+      </c>
+      <c r="P75">
+        <v>4.2077</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>42950.686643518522</v>
+      </c>
+      <c r="B76" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>8</v>
+      </c>
+      <c r="F76">
+        <v>18.198526633018538</v>
+      </c>
+      <c r="G76">
+        <v>4.9850149850149847</v>
+      </c>
+      <c r="H76">
+        <v>0.3</v>
+      </c>
+      <c r="I76">
+        <v>0.1</v>
+      </c>
+      <c r="J76">
+        <v>4</v>
+      </c>
+      <c r="K76">
+        <v>4</v>
+      </c>
+      <c r="L76">
+        <v>2</v>
+      </c>
+      <c r="M76">
+        <v>0.36</v>
+      </c>
+      <c r="N76">
+        <v>1.5</v>
+      </c>
+      <c r="O76">
+        <v>0.46</v>
+      </c>
+      <c r="P76">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>42950.686874999999</v>
+      </c>
+      <c r="B77" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>8</v>
+      </c>
+      <c r="F77">
+        <v>18.187266786492664</v>
+      </c>
+      <c r="G77">
+        <v>5.0109890109890109</v>
+      </c>
+      <c r="H77">
+        <v>0.3</v>
+      </c>
+      <c r="I77">
+        <v>0.1</v>
+      </c>
+      <c r="J77">
+        <v>4</v>
+      </c>
+      <c r="K77">
+        <v>4</v>
+      </c>
+      <c r="L77">
+        <v>2</v>
+      </c>
+      <c r="M77">
+        <v>0.36</v>
+      </c>
+      <c r="N77">
+        <v>1.5</v>
+      </c>
+      <c r="O77">
+        <v>0.46</v>
+      </c>
+      <c r="P77">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>42950.687106481484</v>
+      </c>
+      <c r="B78" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>8</v>
+      </c>
+      <c r="F78">
+        <v>19.114680007308596</v>
+      </c>
+      <c r="G78">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H78">
+        <v>0.3</v>
+      </c>
+      <c r="I78">
+        <v>0.1</v>
+      </c>
+      <c r="J78">
+        <v>4</v>
+      </c>
+      <c r="K78">
+        <v>4</v>
+      </c>
+      <c r="L78">
+        <v>2</v>
+      </c>
+      <c r="M78">
+        <v>0.36</v>
+      </c>
+      <c r="N78">
+        <v>1.5</v>
+      </c>
+      <c r="O78">
+        <v>0.46</v>
+      </c>
+      <c r="P78">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>42950.687349537038</v>
+      </c>
+      <c r="B79" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>8</v>
+      </c>
+      <c r="F79">
+        <v>18.703314499724328</v>
+      </c>
+      <c r="G79">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H79">
+        <v>0.3</v>
+      </c>
+      <c r="I79">
+        <v>0.1</v>
+      </c>
+      <c r="J79">
+        <v>4</v>
+      </c>
+      <c r="K79">
+        <v>4</v>
+      </c>
+      <c r="L79">
+        <v>2</v>
+      </c>
+      <c r="M79">
+        <v>0.36</v>
+      </c>
+      <c r="N79">
+        <v>1.5</v>
+      </c>
+      <c r="O79">
+        <v>0.46</v>
+      </c>
+      <c r="P79">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>42950.687569444446</v>
+      </c>
+      <c r="B80" t="s">
+        <v>17</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>8</v>
+      </c>
+      <c r="F80">
+        <v>18.040489432774191</v>
+      </c>
+      <c r="G80">
+        <v>5.0009990009990011</v>
+      </c>
+      <c r="H80">
+        <v>0.3</v>
+      </c>
+      <c r="I80">
+        <v>0.1</v>
+      </c>
+      <c r="J80">
+        <v>4</v>
+      </c>
+      <c r="K80">
+        <v>4</v>
+      </c>
+      <c r="L80">
+        <v>2</v>
+      </c>
+      <c r="M80">
+        <v>0.36</v>
+      </c>
+      <c r="N80">
+        <v>1.5</v>
+      </c>
+      <c r="O80">
+        <v>0.46</v>
+      </c>
+      <c r="P80">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>42950.696111111109</v>
+      </c>
+      <c r="B81" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>8</v>
+      </c>
+      <c r="F81">
+        <v>18.216251259564935</v>
+      </c>
+      <c r="G81">
+        <v>4.9930069930069925</v>
+      </c>
+      <c r="H81">
+        <v>0.3</v>
+      </c>
+      <c r="I81">
+        <v>0.1</v>
+      </c>
+      <c r="J81">
+        <v>4</v>
+      </c>
+      <c r="K81">
+        <v>4</v>
+      </c>
+      <c r="L81">
+        <v>2</v>
+      </c>
+      <c r="M81">
+        <v>0.36</v>
+      </c>
+      <c r="N81">
+        <v>1.5</v>
+      </c>
+      <c r="O81">
+        <v>0.46</v>
+      </c>
+      <c r="P81">
+        <v>4.1849999999999996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>42950.696331018517</v>
+      </c>
+      <c r="B82" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>8</v>
+      </c>
+      <c r="F82">
+        <v>17.995057417601494</v>
+      </c>
+      <c r="G82">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H82">
+        <v>0.3</v>
+      </c>
+      <c r="I82">
+        <v>0.1</v>
+      </c>
+      <c r="J82">
+        <v>4</v>
+      </c>
+      <c r="K82">
+        <v>4</v>
+      </c>
+      <c r="L82">
+        <v>2</v>
+      </c>
+      <c r="M82">
+        <v>0.36</v>
+      </c>
+      <c r="N82">
+        <v>1.5</v>
+      </c>
+      <c r="O82">
+        <v>0.46</v>
+      </c>
+      <c r="P82">
+        <v>4.3616999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>42950.696562500001</v>
+      </c>
+      <c r="B83" t="s">
+        <v>16</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>8</v>
+      </c>
+      <c r="F83">
+        <v>18.177899047290524</v>
+      </c>
+      <c r="G83">
+        <v>5.0009990009990011</v>
+      </c>
+      <c r="H83">
+        <v>0.3</v>
+      </c>
+      <c r="I83">
+        <v>0.1</v>
+      </c>
+      <c r="J83">
+        <v>4</v>
+      </c>
+      <c r="K83">
+        <v>4</v>
+      </c>
+      <c r="L83">
+        <v>2</v>
+      </c>
+      <c r="M83">
+        <v>0.36</v>
+      </c>
+      <c r="N83">
+        <v>1.5</v>
+      </c>
+      <c r="O83">
+        <v>0.46</v>
+      </c>
+      <c r="P83">
+        <v>4.2077</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>42950.696805555555</v>
+      </c>
+      <c r="B84" t="s">
+        <v>17</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>8</v>
+      </c>
+      <c r="F84">
+        <v>19.108041472125414</v>
+      </c>
+      <c r="G84">
+        <v>4.9870129870129869</v>
+      </c>
+      <c r="H84">
+        <v>0.3</v>
+      </c>
+      <c r="I84">
+        <v>0.1</v>
+      </c>
+      <c r="J84">
+        <v>4</v>
+      </c>
+      <c r="K84">
+        <v>4</v>
+      </c>
+      <c r="L84">
+        <v>2</v>
+      </c>
+      <c r="M84">
+        <v>0.36</v>
+      </c>
+      <c r="N84">
+        <v>1.5</v>
+      </c>
+      <c r="O84">
+        <v>0.46</v>
+      </c>
+      <c r="P84">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>42950.697025462963</v>
+      </c>
+      <c r="B85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>8</v>
+      </c>
+      <c r="F85">
+        <v>18.074015219416292</v>
+      </c>
+      <c r="G85">
+        <v>4.9870129870129869</v>
+      </c>
+      <c r="H85">
+        <v>0.3</v>
+      </c>
+      <c r="I85">
+        <v>0.1</v>
+      </c>
+      <c r="J85">
+        <v>4</v>
+      </c>
+      <c r="K85">
+        <v>4</v>
+      </c>
+      <c r="L85">
+        <v>2</v>
+      </c>
+      <c r="M85">
+        <v>0.36</v>
+      </c>
+      <c r="N85">
+        <v>1.5</v>
+      </c>
+      <c r="O85">
+        <v>0.46</v>
+      </c>
+      <c r="P85">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>42950.697256944448</v>
+      </c>
+      <c r="B86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>8</v>
+      </c>
+      <c r="F86">
+        <v>18.074863835790811</v>
+      </c>
+      <c r="G86">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H86">
+        <v>0.3</v>
+      </c>
+      <c r="I86">
+        <v>0.1</v>
+      </c>
+      <c r="J86">
+        <v>4</v>
+      </c>
+      <c r="K86">
+        <v>4</v>
+      </c>
+      <c r="L86">
+        <v>2</v>
+      </c>
+      <c r="M86">
+        <v>0.36</v>
+      </c>
+      <c r="N86">
+        <v>1.5</v>
+      </c>
+      <c r="O86">
+        <v>0.46</v>
+      </c>
+      <c r="P86">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>42950.697488425925</v>
+      </c>
+      <c r="B87" t="s">
+        <v>16</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>8</v>
+      </c>
+      <c r="F87">
+        <v>18.184543662304442</v>
+      </c>
+      <c r="G87">
+        <v>4.9950049950049946</v>
+      </c>
+      <c r="H87">
+        <v>0.3</v>
+      </c>
+      <c r="I87">
+        <v>0.1</v>
+      </c>
+      <c r="J87">
+        <v>4</v>
+      </c>
+      <c r="K87">
+        <v>4</v>
+      </c>
+      <c r="L87">
+        <v>2</v>
+      </c>
+      <c r="M87">
+        <v>0.36</v>
+      </c>
+      <c r="N87">
+        <v>1.5</v>
+      </c>
+      <c r="O87">
+        <v>0.46</v>
+      </c>
+      <c r="P87">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>42950.697708333333</v>
+      </c>
+      <c r="B88" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>8</v>
+      </c>
+      <c r="F88">
+        <v>17.856046887654649</v>
+      </c>
+      <c r="G88">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H88">
+        <v>0.3</v>
+      </c>
+      <c r="I88">
+        <v>0.1</v>
+      </c>
+      <c r="J88">
+        <v>4</v>
+      </c>
+      <c r="K88">
+        <v>4</v>
+      </c>
+      <c r="L88">
+        <v>2</v>
+      </c>
+      <c r="M88">
+        <v>0.36</v>
+      </c>
+      <c r="N88">
+        <v>1.5</v>
+      </c>
+      <c r="O88">
+        <v>0.46</v>
+      </c>
+      <c r="P88">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>42950.697928240741</v>
+      </c>
+      <c r="B89" t="s">
+        <v>18</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>8</v>
+      </c>
+      <c r="F89">
+        <v>17.78955049891411</v>
+      </c>
+      <c r="G89">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H89">
+        <v>0.3</v>
+      </c>
+      <c r="I89">
+        <v>0.1</v>
+      </c>
+      <c r="J89">
+        <v>4</v>
+      </c>
+      <c r="K89">
+        <v>4</v>
+      </c>
+      <c r="L89">
+        <v>2</v>
+      </c>
+      <c r="M89">
+        <v>0.36</v>
+      </c>
+      <c r="N89">
+        <v>1.5</v>
+      </c>
+      <c r="O89">
+        <v>0.46</v>
+      </c>
+      <c r="P89">
+        <v>4.1849999999999996</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>42950.698159722226</v>
+      </c>
+      <c r="B90" t="s">
+        <v>19</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>8</v>
+      </c>
+      <c r="F90">
+        <v>17.987847378328986</v>
+      </c>
+      <c r="G90">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H90">
+        <v>0.3</v>
+      </c>
+      <c r="I90">
+        <v>0.1</v>
+      </c>
+      <c r="J90">
+        <v>4</v>
+      </c>
+      <c r="K90">
+        <v>4</v>
+      </c>
+      <c r="L90">
+        <v>2</v>
+      </c>
+      <c r="M90">
+        <v>0.36</v>
+      </c>
+      <c r="N90">
+        <v>1.5</v>
+      </c>
+      <c r="O90">
+        <v>0.46</v>
+      </c>
+      <c r="P90">
+        <v>4.3616999999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>42950.698391203703</v>
+      </c>
+      <c r="B91" t="s">
+        <v>16</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>8</v>
+      </c>
+      <c r="F91">
+        <v>18.545626089769662</v>
+      </c>
+      <c r="G91">
+        <v>5.0009990009990011</v>
+      </c>
+      <c r="H91">
+        <v>0.3</v>
+      </c>
+      <c r="I91">
+        <v>0.1</v>
+      </c>
+      <c r="J91">
+        <v>4</v>
+      </c>
+      <c r="K91">
+        <v>4</v>
+      </c>
+      <c r="L91">
+        <v>2</v>
+      </c>
+      <c r="M91">
+        <v>0.36</v>
+      </c>
+      <c r="N91">
+        <v>1.5</v>
+      </c>
+      <c r="O91">
+        <v>0.46</v>
+      </c>
+      <c r="P91">
+        <v>4.2077</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>42950.698622685188</v>
+      </c>
+      <c r="B92" t="s">
+        <v>17</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>8</v>
+      </c>
+      <c r="F92">
+        <v>18.439260410990158</v>
+      </c>
+      <c r="G92">
+        <v>4.9850149850149847</v>
+      </c>
+      <c r="H92">
+        <v>0.3</v>
+      </c>
+      <c r="I92">
+        <v>0.1</v>
+      </c>
+      <c r="J92">
+        <v>4</v>
+      </c>
+      <c r="K92">
+        <v>4</v>
+      </c>
+      <c r="L92">
+        <v>2</v>
+      </c>
+      <c r="M92">
+        <v>0.36</v>
+      </c>
+      <c r="N92">
+        <v>1.5</v>
+      </c>
+      <c r="O92">
+        <v>0.46</v>
+      </c>
+      <c r="P92">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>42950.698854166665</v>
+      </c>
+      <c r="B93" t="s">
+        <v>18</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>8</v>
+      </c>
+      <c r="F93">
+        <v>18.649250084877636</v>
+      </c>
+      <c r="G93">
+        <v>5.0109890109890109</v>
+      </c>
+      <c r="H93">
+        <v>0.3</v>
+      </c>
+      <c r="I93">
+        <v>0.1</v>
+      </c>
+      <c r="J93">
+        <v>4</v>
+      </c>
+      <c r="K93">
+        <v>4</v>
+      </c>
+      <c r="L93">
+        <v>2</v>
+      </c>
+      <c r="M93">
+        <v>0.36</v>
+      </c>
+      <c r="N93">
+        <v>1.5</v>
+      </c>
+      <c r="O93">
+        <v>0.46</v>
+      </c>
+      <c r="P93">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>42950.69908564815</v>
+      </c>
+      <c r="B94" t="s">
+        <v>19</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <v>8</v>
+      </c>
+      <c r="F94">
+        <v>18.47814572842292</v>
+      </c>
+      <c r="G94">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H94">
+        <v>0.3</v>
+      </c>
+      <c r="I94">
+        <v>0.1</v>
+      </c>
+      <c r="J94">
+        <v>4</v>
+      </c>
+      <c r="K94">
+        <v>4</v>
+      </c>
+      <c r="L94">
+        <v>2</v>
+      </c>
+      <c r="M94">
+        <v>0.36</v>
+      </c>
+      <c r="N94">
+        <v>1.5</v>
+      </c>
+      <c r="O94">
+        <v>0.46</v>
+      </c>
+      <c r="P94">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>42950.699317129627</v>
+      </c>
+      <c r="B95" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95">
+        <v>8</v>
+      </c>
+      <c r="F95">
+        <v>18.521495561563565</v>
+      </c>
+      <c r="G95">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H95">
+        <v>0.3</v>
+      </c>
+      <c r="I95">
+        <v>0.1</v>
+      </c>
+      <c r="J95">
+        <v>4</v>
+      </c>
+      <c r="K95">
+        <v>4</v>
+      </c>
+      <c r="L95">
+        <v>2</v>
+      </c>
+      <c r="M95">
+        <v>0.36</v>
+      </c>
+      <c r="N95">
+        <v>1.5</v>
+      </c>
+      <c r="O95">
+        <v>0.46</v>
+      </c>
+      <c r="P95">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>42950.699548611112</v>
+      </c>
+      <c r="B96" t="s">
+        <v>17</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>8</v>
+      </c>
+      <c r="F96">
+        <v>18.498346126043852</v>
+      </c>
+      <c r="G96">
+        <v>5.0009990009990011</v>
+      </c>
+      <c r="H96">
+        <v>0.3</v>
+      </c>
+      <c r="I96">
+        <v>0.1</v>
+      </c>
+      <c r="J96">
+        <v>4</v>
+      </c>
+      <c r="K96">
+        <v>4</v>
+      </c>
+      <c r="L96">
+        <v>2</v>
+      </c>
+      <c r="M96">
+        <v>0.36</v>
+      </c>
+      <c r="N96">
+        <v>1.5</v>
+      </c>
+      <c r="O96">
+        <v>0.46</v>
+      </c>
+      <c r="P96">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>42951.748981481483</v>
+      </c>
+      <c r="B97" t="s">
+        <v>17</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>100</v>
+      </c>
+      <c r="E97">
+        <v>8</v>
+      </c>
+      <c r="F97">
+        <v>15.868170390136338</v>
+      </c>
+      <c r="G97">
+        <v>7.3076923076923075</v>
+      </c>
+      <c r="H97">
+        <v>0.3</v>
+      </c>
+      <c r="I97">
+        <v>0.1</v>
+      </c>
+      <c r="J97">
+        <v>4</v>
+      </c>
+      <c r="K97">
+        <v>4</v>
+      </c>
+      <c r="L97">
+        <v>2</v>
+      </c>
+      <c r="M97">
+        <v>0.36</v>
+      </c>
+      <c r="N97">
+        <v>1.5</v>
+      </c>
+      <c r="O97">
+        <v>0.46</v>
+      </c>
+      <c r="P97">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>42951.872708333336</v>
+      </c>
+      <c r="B98" t="s">
+        <v>17</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>8</v>
+      </c>
+      <c r="F98">
+        <v>24.973420579971055</v>
+      </c>
+      <c r="G98">
+        <v>3.6163836163836161</v>
+      </c>
+      <c r="H98">
+        <v>0.3</v>
+      </c>
+      <c r="I98">
+        <v>0.1</v>
+      </c>
+      <c r="J98">
+        <v>4</v>
+      </c>
+      <c r="K98">
+        <v>4</v>
+      </c>
+      <c r="L98">
+        <v>2</v>
+      </c>
+      <c r="M98">
+        <v>0.36</v>
+      </c>
+      <c r="N98">
+        <v>1.5</v>
+      </c>
+      <c r="O98">
+        <v>0.46</v>
+      </c>
+      <c r="P98">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Get codegen out of the repository
Plus some minor change elsewhere.
</commit_message>
<xml_diff>
--- a/RunSummaries.xlsx
+++ b/RunSummaries.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -452,10 +452,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P98"/>
+  <dimension ref="A1:P124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:P98"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124:P124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5360,6 +5360,1306 @@
         <v>4.7156000000000002</v>
       </c>
     </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>42956.645231481481</v>
+      </c>
+      <c r="B99" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>8</v>
+      </c>
+      <c r="F99">
+        <v>47.62330968705831</v>
+      </c>
+      <c r="G99">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H99">
+        <v>0.3</v>
+      </c>
+      <c r="I99">
+        <v>0.1</v>
+      </c>
+      <c r="J99">
+        <v>4</v>
+      </c>
+      <c r="K99">
+        <v>4</v>
+      </c>
+      <c r="L99">
+        <v>2</v>
+      </c>
+      <c r="M99">
+        <v>0.36</v>
+      </c>
+      <c r="N99">
+        <v>1.5</v>
+      </c>
+      <c r="O99">
+        <v>0.46</v>
+      </c>
+      <c r="P99">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>42956.652326388888</v>
+      </c>
+      <c r="B100" t="s">
+        <v>17</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100">
+        <v>8</v>
+      </c>
+      <c r="F100">
+        <v>301.17806192275606</v>
+      </c>
+      <c r="G100">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H100">
+        <v>0.3</v>
+      </c>
+      <c r="I100">
+        <v>0.1</v>
+      </c>
+      <c r="J100">
+        <v>4</v>
+      </c>
+      <c r="K100">
+        <v>4</v>
+      </c>
+      <c r="L100">
+        <v>2</v>
+      </c>
+      <c r="M100">
+        <v>0.36</v>
+      </c>
+      <c r="N100">
+        <v>1.5</v>
+      </c>
+      <c r="O100">
+        <v>0.46</v>
+      </c>
+      <c r="P100">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>42956.682754629626</v>
+      </c>
+      <c r="B101" t="s">
+        <v>17</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>1000</v>
+      </c>
+      <c r="E101">
+        <v>6</v>
+      </c>
+      <c r="F101">
+        <v>19.633311968594793</v>
+      </c>
+      <c r="G101">
+        <v>9.615384615384615</v>
+      </c>
+      <c r="H101">
+        <v>0.3</v>
+      </c>
+      <c r="I101">
+        <v>0.1</v>
+      </c>
+      <c r="J101">
+        <v>4</v>
+      </c>
+      <c r="K101">
+        <v>4</v>
+      </c>
+      <c r="L101">
+        <v>2</v>
+      </c>
+      <c r="M101">
+        <v>0.36</v>
+      </c>
+      <c r="N101">
+        <v>1.5</v>
+      </c>
+      <c r="O101">
+        <v>0.46</v>
+      </c>
+      <c r="P101">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>42956.850173611114</v>
+      </c>
+      <c r="B102" t="s">
+        <v>17</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>10</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102">
+        <v>28.813696706683686</v>
+      </c>
+      <c r="G102">
+        <v>4.6661460367044123</v>
+      </c>
+      <c r="H102">
+        <v>0.3</v>
+      </c>
+      <c r="I102">
+        <v>0.1</v>
+      </c>
+      <c r="J102">
+        <v>4</v>
+      </c>
+      <c r="K102">
+        <v>4</v>
+      </c>
+      <c r="L102">
+        <v>2</v>
+      </c>
+      <c r="M102">
+        <v>0.36</v>
+      </c>
+      <c r="N102">
+        <v>1.5</v>
+      </c>
+      <c r="O102">
+        <v>0.46</v>
+      </c>
+      <c r="P102">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>42956.850439814814</v>
+      </c>
+      <c r="B103" t="s">
+        <v>17</v>
+      </c>
+      <c r="C103">
+        <v>1</v>
+      </c>
+      <c r="D103">
+        <v>10</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+      <c r="F103">
+        <v>16.1089326473151</v>
+      </c>
+      <c r="G103">
+        <v>4.6661460367044123</v>
+      </c>
+      <c r="H103">
+        <v>0.3</v>
+      </c>
+      <c r="I103">
+        <v>0.1</v>
+      </c>
+      <c r="J103">
+        <v>4</v>
+      </c>
+      <c r="K103">
+        <v>4</v>
+      </c>
+      <c r="L103">
+        <v>2</v>
+      </c>
+      <c r="M103">
+        <v>0.36</v>
+      </c>
+      <c r="N103">
+        <v>1.5</v>
+      </c>
+      <c r="O103">
+        <v>0.46</v>
+      </c>
+      <c r="P103">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>42956.85119212963</v>
+      </c>
+      <c r="B104" t="s">
+        <v>17</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>10</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="F104">
+        <v>14.267030005884637</v>
+      </c>
+      <c r="G104">
+        <v>4.6661460367044123</v>
+      </c>
+      <c r="H104">
+        <v>0.3</v>
+      </c>
+      <c r="I104">
+        <v>0.1</v>
+      </c>
+      <c r="J104">
+        <v>4</v>
+      </c>
+      <c r="K104">
+        <v>4</v>
+      </c>
+      <c r="L104">
+        <v>2</v>
+      </c>
+      <c r="M104">
+        <v>0.36</v>
+      </c>
+      <c r="N104">
+        <v>1.5</v>
+      </c>
+      <c r="O104">
+        <v>0.46</v>
+      </c>
+      <c r="P104">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>42956.851574074077</v>
+      </c>
+      <c r="B105" t="s">
+        <v>17</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105">
+        <v>10</v>
+      </c>
+      <c r="E105">
+        <v>1</v>
+      </c>
+      <c r="F105">
+        <v>11.997601346778506</v>
+      </c>
+      <c r="G105">
+        <v>4.6661460367044123</v>
+      </c>
+      <c r="H105">
+        <v>0.3</v>
+      </c>
+      <c r="I105">
+        <v>0.1</v>
+      </c>
+      <c r="J105">
+        <v>4</v>
+      </c>
+      <c r="K105">
+        <v>4</v>
+      </c>
+      <c r="L105">
+        <v>2</v>
+      </c>
+      <c r="M105">
+        <v>0.36</v>
+      </c>
+      <c r="N105">
+        <v>1.5</v>
+      </c>
+      <c r="O105">
+        <v>0.46</v>
+      </c>
+      <c r="P105">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>42956.852013888885</v>
+      </c>
+      <c r="B106" t="s">
+        <v>17</v>
+      </c>
+      <c r="C106">
+        <v>1</v>
+      </c>
+      <c r="D106">
+        <v>10</v>
+      </c>
+      <c r="E106">
+        <v>1</v>
+      </c>
+      <c r="F106">
+        <v>20.510265474209199</v>
+      </c>
+      <c r="G106">
+        <v>4.6661460367044123</v>
+      </c>
+      <c r="H106">
+        <v>0.3</v>
+      </c>
+      <c r="I106">
+        <v>0.1</v>
+      </c>
+      <c r="J106">
+        <v>4</v>
+      </c>
+      <c r="K106">
+        <v>4</v>
+      </c>
+      <c r="L106">
+        <v>2</v>
+      </c>
+      <c r="M106">
+        <v>0.36</v>
+      </c>
+      <c r="N106">
+        <v>1.5</v>
+      </c>
+      <c r="O106">
+        <v>0.46</v>
+      </c>
+      <c r="P106">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>42956.855196759258</v>
+      </c>
+      <c r="B107" t="s">
+        <v>17</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>10</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+      <c r="F107">
+        <v>11.85646735594881</v>
+      </c>
+      <c r="G107">
+        <v>4.6661460367044123</v>
+      </c>
+      <c r="H107">
+        <v>0.3</v>
+      </c>
+      <c r="I107">
+        <v>0.1</v>
+      </c>
+      <c r="J107">
+        <v>4</v>
+      </c>
+      <c r="K107">
+        <v>4</v>
+      </c>
+      <c r="L107">
+        <v>2</v>
+      </c>
+      <c r="M107">
+        <v>0.36</v>
+      </c>
+      <c r="N107">
+        <v>1.5</v>
+      </c>
+      <c r="O107">
+        <v>0.46</v>
+      </c>
+      <c r="P107">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>42956.855474537035</v>
+      </c>
+      <c r="B108" t="s">
+        <v>17</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="D108">
+        <v>10</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+      <c r="F108">
+        <v>11.591607209655283</v>
+      </c>
+      <c r="G108">
+        <v>4.6661460367044123</v>
+      </c>
+      <c r="H108">
+        <v>0.3</v>
+      </c>
+      <c r="I108">
+        <v>0.1</v>
+      </c>
+      <c r="J108">
+        <v>4</v>
+      </c>
+      <c r="K108">
+        <v>4</v>
+      </c>
+      <c r="L108">
+        <v>2</v>
+      </c>
+      <c r="M108">
+        <v>0.36</v>
+      </c>
+      <c r="N108">
+        <v>1.5</v>
+      </c>
+      <c r="O108">
+        <v>0.46</v>
+      </c>
+      <c r="P108">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>42956.856041666666</v>
+      </c>
+      <c r="B109" t="s">
+        <v>17</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="D109">
+        <v>5</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="F109">
+        <v>17.15924036674819</v>
+      </c>
+      <c r="G109">
+        <v>4.7557840616966578</v>
+      </c>
+      <c r="H109">
+        <v>0.3</v>
+      </c>
+      <c r="I109">
+        <v>0.1</v>
+      </c>
+      <c r="J109">
+        <v>4</v>
+      </c>
+      <c r="K109">
+        <v>4</v>
+      </c>
+      <c r="L109">
+        <v>2</v>
+      </c>
+      <c r="M109">
+        <v>0.36</v>
+      </c>
+      <c r="N109">
+        <v>1.5</v>
+      </c>
+      <c r="O109">
+        <v>0.46</v>
+      </c>
+      <c r="P109">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>42956.85633101852</v>
+      </c>
+      <c r="B110" t="s">
+        <v>17</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110">
+        <v>5</v>
+      </c>
+      <c r="E110">
+        <v>1</v>
+      </c>
+      <c r="F110">
+        <v>17.206368014714471</v>
+      </c>
+      <c r="G110">
+        <v>4.7557840616966578</v>
+      </c>
+      <c r="H110">
+        <v>0.3</v>
+      </c>
+      <c r="I110">
+        <v>0.1</v>
+      </c>
+      <c r="J110">
+        <v>4</v>
+      </c>
+      <c r="K110">
+        <v>4</v>
+      </c>
+      <c r="L110">
+        <v>2</v>
+      </c>
+      <c r="M110">
+        <v>0.36</v>
+      </c>
+      <c r="N110">
+        <v>1.5</v>
+      </c>
+      <c r="O110">
+        <v>0.46</v>
+      </c>
+      <c r="P110">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>42956.85665509259</v>
+      </c>
+      <c r="B111" t="s">
+        <v>17</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111">
+        <v>5</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="F111">
+        <v>18.301213054228569</v>
+      </c>
+      <c r="G111">
+        <v>4.7557840616966578</v>
+      </c>
+      <c r="H111">
+        <v>0.3</v>
+      </c>
+      <c r="I111">
+        <v>0.1</v>
+      </c>
+      <c r="J111">
+        <v>4</v>
+      </c>
+      <c r="K111">
+        <v>4</v>
+      </c>
+      <c r="L111">
+        <v>2</v>
+      </c>
+      <c r="M111">
+        <v>0.36</v>
+      </c>
+      <c r="N111">
+        <v>1.5</v>
+      </c>
+      <c r="O111">
+        <v>0.46</v>
+      </c>
+      <c r="P111">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>42956.857569444444</v>
+      </c>
+      <c r="B112" t="s">
+        <v>17</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112">
+        <v>5</v>
+      </c>
+      <c r="E112">
+        <v>1</v>
+      </c>
+      <c r="F112">
+        <v>34.42381156108614</v>
+      </c>
+      <c r="G112">
+        <v>4.7557840616966578</v>
+      </c>
+      <c r="H112">
+        <v>0.3</v>
+      </c>
+      <c r="I112">
+        <v>0.1</v>
+      </c>
+      <c r="J112">
+        <v>4</v>
+      </c>
+      <c r="K112">
+        <v>4</v>
+      </c>
+      <c r="L112">
+        <v>2</v>
+      </c>
+      <c r="M112">
+        <v>0.36</v>
+      </c>
+      <c r="N112">
+        <v>1.5</v>
+      </c>
+      <c r="O112">
+        <v>0.46</v>
+      </c>
+      <c r="P112">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>42956.857939814814</v>
+      </c>
+      <c r="B113" t="s">
+        <v>17</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113">
+        <v>5</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="F113">
+        <v>22.853282484615629</v>
+      </c>
+      <c r="G113">
+        <v>4.7557840616966578</v>
+      </c>
+      <c r="H113">
+        <v>0.3</v>
+      </c>
+      <c r="I113">
+        <v>0.1</v>
+      </c>
+      <c r="J113">
+        <v>4</v>
+      </c>
+      <c r="K113">
+        <v>4</v>
+      </c>
+      <c r="L113">
+        <v>2</v>
+      </c>
+      <c r="M113">
+        <v>0.36</v>
+      </c>
+      <c r="N113">
+        <v>1.5</v>
+      </c>
+      <c r="O113">
+        <v>0.46</v>
+      </c>
+      <c r="P113">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>42956.858344907407</v>
+      </c>
+      <c r="B114" t="s">
+        <v>17</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114">
+        <v>5</v>
+      </c>
+      <c r="E114">
+        <v>1</v>
+      </c>
+      <c r="F114">
+        <v>22.492494448954542</v>
+      </c>
+      <c r="G114">
+        <v>4.7557840616966578</v>
+      </c>
+      <c r="H114">
+        <v>0.3</v>
+      </c>
+      <c r="I114">
+        <v>0.1</v>
+      </c>
+      <c r="J114">
+        <v>4</v>
+      </c>
+      <c r="K114">
+        <v>4</v>
+      </c>
+      <c r="L114">
+        <v>2</v>
+      </c>
+      <c r="M114">
+        <v>0.36</v>
+      </c>
+      <c r="N114">
+        <v>1.5</v>
+      </c>
+      <c r="O114">
+        <v>0.46</v>
+      </c>
+      <c r="P114">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>42956.858935185184</v>
+      </c>
+      <c r="B115" t="s">
+        <v>17</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115">
+        <v>5</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="F115">
+        <v>34.52645382352555</v>
+      </c>
+      <c r="G115">
+        <v>4.7557840616966578</v>
+      </c>
+      <c r="H115">
+        <v>0.3</v>
+      </c>
+      <c r="I115">
+        <v>0.1</v>
+      </c>
+      <c r="J115">
+        <v>4</v>
+      </c>
+      <c r="K115">
+        <v>4</v>
+      </c>
+      <c r="L115">
+        <v>2</v>
+      </c>
+      <c r="M115">
+        <v>0.36</v>
+      </c>
+      <c r="N115">
+        <v>1.5</v>
+      </c>
+      <c r="O115">
+        <v>0.46</v>
+      </c>
+      <c r="P115">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>42956.860717592594</v>
+      </c>
+      <c r="B116" t="s">
+        <v>17</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116">
+        <v>5</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+      <c r="F116">
+        <v>18.546751818429374</v>
+      </c>
+      <c r="G116">
+        <v>4.7557840616966578</v>
+      </c>
+      <c r="H116">
+        <v>0.3</v>
+      </c>
+      <c r="I116">
+        <v>0.1</v>
+      </c>
+      <c r="J116">
+        <v>4</v>
+      </c>
+      <c r="K116">
+        <v>4</v>
+      </c>
+      <c r="L116">
+        <v>2</v>
+      </c>
+      <c r="M116">
+        <v>0.36</v>
+      </c>
+      <c r="N116">
+        <v>1.5</v>
+      </c>
+      <c r="O116">
+        <v>0.46</v>
+      </c>
+      <c r="P116">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>42956.861284722225</v>
+      </c>
+      <c r="B117" t="s">
+        <v>17</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="D117">
+        <v>5</v>
+      </c>
+      <c r="E117">
+        <v>1</v>
+      </c>
+      <c r="F117">
+        <v>18.184056315872166</v>
+      </c>
+      <c r="G117">
+        <v>4.7557840616966578</v>
+      </c>
+      <c r="H117">
+        <v>0.3</v>
+      </c>
+      <c r="I117">
+        <v>0.1</v>
+      </c>
+      <c r="J117">
+        <v>4</v>
+      </c>
+      <c r="K117">
+        <v>4</v>
+      </c>
+      <c r="L117">
+        <v>2</v>
+      </c>
+      <c r="M117">
+        <v>0.36</v>
+      </c>
+      <c r="N117">
+        <v>1.5</v>
+      </c>
+      <c r="O117">
+        <v>0.46</v>
+      </c>
+      <c r="P117">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>42956.974212962959</v>
+      </c>
+      <c r="B118" t="s">
+        <v>17</v>
+      </c>
+      <c r="C118">
+        <v>1</v>
+      </c>
+      <c r="D118">
+        <v>10000</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <v>21.975067894109827</v>
+      </c>
+      <c r="G118">
+        <v>5.384615384615385</v>
+      </c>
+      <c r="H118">
+        <v>0.3</v>
+      </c>
+      <c r="I118">
+        <v>0.1</v>
+      </c>
+      <c r="J118">
+        <v>4</v>
+      </c>
+      <c r="K118">
+        <v>4</v>
+      </c>
+      <c r="L118">
+        <v>2</v>
+      </c>
+      <c r="M118">
+        <v>0.36</v>
+      </c>
+      <c r="N118">
+        <v>1.5</v>
+      </c>
+      <c r="O118">
+        <v>0.46</v>
+      </c>
+      <c r="P118">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>42956.975682870368</v>
+      </c>
+      <c r="B119" t="s">
+        <v>17</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+      <c r="D119">
+        <v>10000</v>
+      </c>
+      <c r="E119">
+        <v>1</v>
+      </c>
+      <c r="F119">
+        <v>3.4992485009217345</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+      <c r="H119">
+        <v>0.3</v>
+      </c>
+      <c r="I119">
+        <v>0.1</v>
+      </c>
+      <c r="J119">
+        <v>4</v>
+      </c>
+      <c r="K119">
+        <v>4</v>
+      </c>
+      <c r="L119">
+        <v>2</v>
+      </c>
+      <c r="M119">
+        <v>0.36</v>
+      </c>
+      <c r="N119">
+        <v>1.5</v>
+      </c>
+      <c r="O119">
+        <v>0.46</v>
+      </c>
+      <c r="P119">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>42956.975949074076</v>
+      </c>
+      <c r="B120" t="s">
+        <v>17</v>
+      </c>
+      <c r="C120">
+        <v>1</v>
+      </c>
+      <c r="D120">
+        <v>10000</v>
+      </c>
+      <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="F120">
+        <v>3.2868390544007253</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>0.3</v>
+      </c>
+      <c r="I120">
+        <v>0.1</v>
+      </c>
+      <c r="J120">
+        <v>4</v>
+      </c>
+      <c r="K120">
+        <v>4</v>
+      </c>
+      <c r="L120">
+        <v>2</v>
+      </c>
+      <c r="M120">
+        <v>0.36</v>
+      </c>
+      <c r="N120">
+        <v>1.5</v>
+      </c>
+      <c r="O120">
+        <v>0.46</v>
+      </c>
+      <c r="P120">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>42956.97797453704</v>
+      </c>
+      <c r="B121" t="s">
+        <v>17</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
+      <c r="D121">
+        <v>10000</v>
+      </c>
+      <c r="E121">
+        <v>1</v>
+      </c>
+      <c r="F121">
+        <v>5.1121139987462749</v>
+      </c>
+      <c r="G121">
+        <v>0</v>
+      </c>
+      <c r="H121">
+        <v>0.3</v>
+      </c>
+      <c r="I121">
+        <v>0.1</v>
+      </c>
+      <c r="J121">
+        <v>4</v>
+      </c>
+      <c r="K121">
+        <v>4</v>
+      </c>
+      <c r="L121">
+        <v>2</v>
+      </c>
+      <c r="M121">
+        <v>0.36</v>
+      </c>
+      <c r="N121">
+        <v>1.5</v>
+      </c>
+      <c r="O121">
+        <v>0.46</v>
+      </c>
+      <c r="P121">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>42956.979097222225</v>
+      </c>
+      <c r="B122" t="s">
+        <v>17</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122">
+        <v>6</v>
+      </c>
+      <c r="F122">
+        <v>71.727423908518389</v>
+      </c>
+      <c r="G122">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H122">
+        <v>0.3</v>
+      </c>
+      <c r="I122">
+        <v>0.1</v>
+      </c>
+      <c r="J122">
+        <v>4</v>
+      </c>
+      <c r="K122">
+        <v>4</v>
+      </c>
+      <c r="L122">
+        <v>2</v>
+      </c>
+      <c r="M122">
+        <v>0.36</v>
+      </c>
+      <c r="N122">
+        <v>1.5</v>
+      </c>
+      <c r="O122">
+        <v>0.46</v>
+      </c>
+      <c r="P122">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>42956.980752314812</v>
+      </c>
+      <c r="B123" t="s">
+        <v>17</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123">
+        <v>6</v>
+      </c>
+      <c r="F123">
+        <v>57.564139494356475</v>
+      </c>
+      <c r="G123">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H123">
+        <v>0.3</v>
+      </c>
+      <c r="I123">
+        <v>0.1</v>
+      </c>
+      <c r="J123">
+        <v>4</v>
+      </c>
+      <c r="K123">
+        <v>4</v>
+      </c>
+      <c r="L123">
+        <v>2</v>
+      </c>
+      <c r="M123">
+        <v>0.36</v>
+      </c>
+      <c r="N123">
+        <v>1.5</v>
+      </c>
+      <c r="O123">
+        <v>0.46</v>
+      </c>
+      <c r="P123">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>42956.984583333331</v>
+      </c>
+      <c r="B124" t="s">
+        <v>17</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124">
+        <v>6</v>
+      </c>
+      <c r="F124">
+        <v>19.456468251923866</v>
+      </c>
+      <c r="G124">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H124">
+        <v>0.3</v>
+      </c>
+      <c r="I124">
+        <v>0.1</v>
+      </c>
+      <c r="J124">
+        <v>4</v>
+      </c>
+      <c r="K124">
+        <v>4</v>
+      </c>
+      <c r="L124">
+        <v>2</v>
+      </c>
+      <c r="M124">
+        <v>0.36</v>
+      </c>
+      <c r="N124">
+        <v>1.5</v>
+      </c>
+      <c r="O124">
+        <v>0.46</v>
+      </c>
+      <c r="P124">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Properly ignore codegen directory
The contents of codegen is a side effect of compiling mex files, and not something we ever use directly.  By editing .gitignore it doesn't go to the repository or get updated there.
</commit_message>
<xml_diff>
--- a/RunSummaries.xlsx
+++ b/RunSummaries.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -452,10 +452,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P124"/>
+  <dimension ref="A1:P131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124:P124"/>
+      <selection activeCell="A131" sqref="A131:P131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6660,6 +6660,356 @@
         <v>4.7156000000000002</v>
       </c>
     </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>42956.989444444444</v>
+      </c>
+      <c r="B125" t="s">
+        <v>17</v>
+      </c>
+      <c r="C125">
+        <v>1</v>
+      </c>
+      <c r="D125">
+        <v>10000</v>
+      </c>
+      <c r="E125">
+        <v>1</v>
+      </c>
+      <c r="F125">
+        <v>2.5123978948426076</v>
+      </c>
+      <c r="G125">
+        <v>0</v>
+      </c>
+      <c r="H125">
+        <v>0.3</v>
+      </c>
+      <c r="I125">
+        <v>0.1</v>
+      </c>
+      <c r="J125">
+        <v>4</v>
+      </c>
+      <c r="K125">
+        <v>4</v>
+      </c>
+      <c r="L125">
+        <v>2</v>
+      </c>
+      <c r="M125">
+        <v>0.36</v>
+      </c>
+      <c r="N125">
+        <v>1.5</v>
+      </c>
+      <c r="O125">
+        <v>0.46</v>
+      </c>
+      <c r="P125">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>42956.989837962959</v>
+      </c>
+      <c r="B126" t="s">
+        <v>17</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
+      <c r="D126">
+        <v>10000</v>
+      </c>
+      <c r="E126">
+        <v>1</v>
+      </c>
+      <c r="F126">
+        <v>2.4294366844827042</v>
+      </c>
+      <c r="G126">
+        <v>0</v>
+      </c>
+      <c r="H126">
+        <v>0.3</v>
+      </c>
+      <c r="I126">
+        <v>0.1</v>
+      </c>
+      <c r="J126">
+        <v>4</v>
+      </c>
+      <c r="K126">
+        <v>4</v>
+      </c>
+      <c r="L126">
+        <v>2</v>
+      </c>
+      <c r="M126">
+        <v>0.36</v>
+      </c>
+      <c r="N126">
+        <v>1.5</v>
+      </c>
+      <c r="O126">
+        <v>0.46</v>
+      </c>
+      <c r="P126">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>42956.990289351852</v>
+      </c>
+      <c r="B127" t="s">
+        <v>17</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
+      </c>
+      <c r="D127">
+        <v>1000</v>
+      </c>
+      <c r="E127">
+        <v>2</v>
+      </c>
+      <c r="F127">
+        <v>2.4243488261286807</v>
+      </c>
+      <c r="G127">
+        <v>15.384615384615385</v>
+      </c>
+      <c r="H127">
+        <v>0.3</v>
+      </c>
+      <c r="I127">
+        <v>0.1</v>
+      </c>
+      <c r="J127">
+        <v>4</v>
+      </c>
+      <c r="K127">
+        <v>4</v>
+      </c>
+      <c r="L127">
+        <v>2</v>
+      </c>
+      <c r="M127">
+        <v>0.36</v>
+      </c>
+      <c r="N127">
+        <v>1.5</v>
+      </c>
+      <c r="O127">
+        <v>0.46</v>
+      </c>
+      <c r="P127">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>42956.990694444445</v>
+      </c>
+      <c r="B128" t="s">
+        <v>17</v>
+      </c>
+      <c r="C128">
+        <v>1</v>
+      </c>
+      <c r="D128">
+        <v>1000</v>
+      </c>
+      <c r="E128">
+        <v>1</v>
+      </c>
+      <c r="F128">
+        <v>2.318066985015137</v>
+      </c>
+      <c r="G128">
+        <v>15.384615384615385</v>
+      </c>
+      <c r="H128">
+        <v>0.3</v>
+      </c>
+      <c r="I128">
+        <v>0.1</v>
+      </c>
+      <c r="J128">
+        <v>4</v>
+      </c>
+      <c r="K128">
+        <v>4</v>
+      </c>
+      <c r="L128">
+        <v>2</v>
+      </c>
+      <c r="M128">
+        <v>0.36</v>
+      </c>
+      <c r="N128">
+        <v>1.5</v>
+      </c>
+      <c r="O128">
+        <v>0.46</v>
+      </c>
+      <c r="P128">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>42956.99113425926</v>
+      </c>
+      <c r="B129" t="s">
+        <v>17</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+      <c r="D129">
+        <v>1000</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+      <c r="F129">
+        <v>3.6538281974229836</v>
+      </c>
+      <c r="G129">
+        <v>15.384615384615385</v>
+      </c>
+      <c r="H129">
+        <v>0.3</v>
+      </c>
+      <c r="I129">
+        <v>0.1</v>
+      </c>
+      <c r="J129">
+        <v>4</v>
+      </c>
+      <c r="K129">
+        <v>4</v>
+      </c>
+      <c r="L129">
+        <v>2</v>
+      </c>
+      <c r="M129">
+        <v>0.36</v>
+      </c>
+      <c r="N129">
+        <v>1.5</v>
+      </c>
+      <c r="O129">
+        <v>0.46</v>
+      </c>
+      <c r="P129">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>42956.991215277776</v>
+      </c>
+      <c r="B130" t="s">
+        <v>17</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="D130">
+        <v>1000</v>
+      </c>
+      <c r="E130">
+        <v>1</v>
+      </c>
+      <c r="F130">
+        <v>3.5865519903925875</v>
+      </c>
+      <c r="G130">
+        <v>15.384615384615385</v>
+      </c>
+      <c r="H130">
+        <v>0.3</v>
+      </c>
+      <c r="I130">
+        <v>0.1</v>
+      </c>
+      <c r="J130">
+        <v>4</v>
+      </c>
+      <c r="K130">
+        <v>4</v>
+      </c>
+      <c r="L130">
+        <v>2</v>
+      </c>
+      <c r="M130">
+        <v>0.36</v>
+      </c>
+      <c r="N130">
+        <v>1.5</v>
+      </c>
+      <c r="O130">
+        <v>0.46</v>
+      </c>
+      <c r="P130">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>42956.991481481484</v>
+      </c>
+      <c r="B131" t="s">
+        <v>17</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
+      </c>
+      <c r="D131">
+        <v>1000</v>
+      </c>
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <v>2.5608333463996362</v>
+      </c>
+      <c r="G131">
+        <v>15.384615384615385</v>
+      </c>
+      <c r="H131">
+        <v>0.3</v>
+      </c>
+      <c r="I131">
+        <v>0.1</v>
+      </c>
+      <c r="J131">
+        <v>4</v>
+      </c>
+      <c r="K131">
+        <v>4</v>
+      </c>
+      <c r="L131">
+        <v>2</v>
+      </c>
+      <c r="M131">
+        <v>0.36</v>
+      </c>
+      <c r="N131">
+        <v>1.5</v>
+      </c>
+      <c r="O131">
+        <v>0.46</v>
+      </c>
+      <c r="P131">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added plotting functions and optional Omega curves
This includes some new plotting scripts as well as the ability  to manually choose from several Omega-factor curves.
</commit_message>
<xml_diff>
--- a/RunSummaries.xlsx
+++ b/RunSummaries.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>rcp45</t>
+  </si>
+  <si>
+    <t>control400</t>
   </si>
 </sst>
 </file>
@@ -452,10 +455,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P131"/>
+  <dimension ref="A1:P202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131:P131"/>
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="A202" sqref="A202:P202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7010,6 +7013,3556 @@
         <v>4.7156000000000002</v>
       </c>
     </row>
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>42957.002951388888</v>
+      </c>
+      <c r="B132" t="s">
+        <v>17</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="F132">
+        <v>62.902967821375853</v>
+      </c>
+      <c r="G132">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H132">
+        <v>0.3</v>
+      </c>
+      <c r="I132">
+        <v>0.1</v>
+      </c>
+      <c r="J132">
+        <v>4</v>
+      </c>
+      <c r="K132">
+        <v>4</v>
+      </c>
+      <c r="L132">
+        <v>2</v>
+      </c>
+      <c r="M132">
+        <v>0.36</v>
+      </c>
+      <c r="N132">
+        <v>1.5</v>
+      </c>
+      <c r="O132">
+        <v>0.46</v>
+      </c>
+      <c r="P132">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>42957.4996875</v>
+      </c>
+      <c r="B133" t="s">
+        <v>17</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
+      <c r="D133">
+        <v>1000</v>
+      </c>
+      <c r="E133">
+        <v>1</v>
+      </c>
+      <c r="F133">
+        <v>11.888252711044524</v>
+      </c>
+      <c r="G133">
+        <v>15.384615384615385</v>
+      </c>
+      <c r="H133">
+        <v>0.3</v>
+      </c>
+      <c r="I133">
+        <v>0.1</v>
+      </c>
+      <c r="J133">
+        <v>4</v>
+      </c>
+      <c r="K133">
+        <v>4</v>
+      </c>
+      <c r="L133">
+        <v>2</v>
+      </c>
+      <c r="M133">
+        <v>0.36</v>
+      </c>
+      <c r="N133">
+        <v>1.5</v>
+      </c>
+      <c r="O133">
+        <v>0.46</v>
+      </c>
+      <c r="P133">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>42957.508032407408</v>
+      </c>
+      <c r="B134" t="s">
+        <v>16</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134">
+        <v>1000</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="F134">
+        <v>13.603447840012134</v>
+      </c>
+      <c r="G134">
+        <v>15.384615384615385</v>
+      </c>
+      <c r="H134">
+        <v>0.3</v>
+      </c>
+      <c r="I134">
+        <v>0.1</v>
+      </c>
+      <c r="J134">
+        <v>4</v>
+      </c>
+      <c r="K134">
+        <v>4</v>
+      </c>
+      <c r="L134">
+        <v>2</v>
+      </c>
+      <c r="M134">
+        <v>0.36</v>
+      </c>
+      <c r="N134">
+        <v>1.5</v>
+      </c>
+      <c r="O134">
+        <v>0.46</v>
+      </c>
+      <c r="P134">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>42957.513055555559</v>
+      </c>
+      <c r="B135" t="s">
+        <v>16</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
+      </c>
+      <c r="D135">
+        <v>100</v>
+      </c>
+      <c r="E135">
+        <v>6</v>
+      </c>
+      <c r="F135">
+        <v>13.298190738369843</v>
+      </c>
+      <c r="G135">
+        <v>6.1538461538461542</v>
+      </c>
+      <c r="H135">
+        <v>0.3</v>
+      </c>
+      <c r="I135">
+        <v>0.1</v>
+      </c>
+      <c r="J135">
+        <v>4</v>
+      </c>
+      <c r="K135">
+        <v>4</v>
+      </c>
+      <c r="L135">
+        <v>2</v>
+      </c>
+      <c r="M135">
+        <v>0.36</v>
+      </c>
+      <c r="N135">
+        <v>1.5</v>
+      </c>
+      <c r="O135">
+        <v>0.46</v>
+      </c>
+      <c r="P135">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>42957.571574074071</v>
+      </c>
+      <c r="B136" t="s">
+        <v>16</v>
+      </c>
+      <c r="C136">
+        <v>1</v>
+      </c>
+      <c r="D136">
+        <v>100</v>
+      </c>
+      <c r="E136">
+        <v>6</v>
+      </c>
+      <c r="F136">
+        <v>17.038819079276834</v>
+      </c>
+      <c r="G136">
+        <v>6.1538461538461542</v>
+      </c>
+      <c r="H136">
+        <v>0.3</v>
+      </c>
+      <c r="I136">
+        <v>0.1</v>
+      </c>
+      <c r="J136">
+        <v>4</v>
+      </c>
+      <c r="K136">
+        <v>4</v>
+      </c>
+      <c r="L136">
+        <v>2</v>
+      </c>
+      <c r="M136">
+        <v>0.36</v>
+      </c>
+      <c r="N136">
+        <v>1.5</v>
+      </c>
+      <c r="O136">
+        <v>0.46</v>
+      </c>
+      <c r="P136">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>42957.574444444443</v>
+      </c>
+      <c r="B137" t="s">
+        <v>16</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <v>100</v>
+      </c>
+      <c r="E137">
+        <v>6</v>
+      </c>
+      <c r="F137">
+        <v>18.642487713142067</v>
+      </c>
+      <c r="G137">
+        <v>6.1538461538461542</v>
+      </c>
+      <c r="H137">
+        <v>0.3</v>
+      </c>
+      <c r="I137">
+        <v>0.1</v>
+      </c>
+      <c r="J137">
+        <v>4</v>
+      </c>
+      <c r="K137">
+        <v>4</v>
+      </c>
+      <c r="L137">
+        <v>2</v>
+      </c>
+      <c r="M137">
+        <v>0.36</v>
+      </c>
+      <c r="N137">
+        <v>1.5</v>
+      </c>
+      <c r="O137">
+        <v>0.46</v>
+      </c>
+      <c r="P137">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>42957.581134259257</v>
+      </c>
+      <c r="B138" t="s">
+        <v>16</v>
+      </c>
+      <c r="C138">
+        <v>1</v>
+      </c>
+      <c r="D138">
+        <v>100</v>
+      </c>
+      <c r="E138">
+        <v>6</v>
+      </c>
+      <c r="F138">
+        <v>3.3770819820376201</v>
+      </c>
+      <c r="G138">
+        <v>6.1538461538461542</v>
+      </c>
+      <c r="H138">
+        <v>0.3</v>
+      </c>
+      <c r="I138">
+        <v>0.1</v>
+      </c>
+      <c r="J138">
+        <v>4</v>
+      </c>
+      <c r="K138">
+        <v>4</v>
+      </c>
+      <c r="L138">
+        <v>2</v>
+      </c>
+      <c r="M138">
+        <v>0.36</v>
+      </c>
+      <c r="N138">
+        <v>1.5</v>
+      </c>
+      <c r="O138">
+        <v>0.46</v>
+      </c>
+      <c r="P138">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>42957.583773148152</v>
+      </c>
+      <c r="B139" t="s">
+        <v>16</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <v>100</v>
+      </c>
+      <c r="E139">
+        <v>6</v>
+      </c>
+      <c r="F139">
+        <v>3.2931131197307466</v>
+      </c>
+      <c r="G139">
+        <v>6.5384615384615383</v>
+      </c>
+      <c r="H139">
+        <v>0.3</v>
+      </c>
+      <c r="I139">
+        <v>0.1</v>
+      </c>
+      <c r="J139">
+        <v>4</v>
+      </c>
+      <c r="K139">
+        <v>4</v>
+      </c>
+      <c r="L139">
+        <v>2</v>
+      </c>
+      <c r="M139">
+        <v>0.36</v>
+      </c>
+      <c r="N139">
+        <v>1.5</v>
+      </c>
+      <c r="O139">
+        <v>0.46</v>
+      </c>
+      <c r="P139">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>42957.594050925924</v>
+      </c>
+      <c r="B140" t="s">
+        <v>16</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140">
+        <v>6</v>
+      </c>
+      <c r="F140">
+        <v>59.541133734836819</v>
+      </c>
+      <c r="G140">
+        <v>5.0189810189810187</v>
+      </c>
+      <c r="H140">
+        <v>0.3</v>
+      </c>
+      <c r="I140">
+        <v>0.1</v>
+      </c>
+      <c r="J140">
+        <v>4</v>
+      </c>
+      <c r="K140">
+        <v>4</v>
+      </c>
+      <c r="L140">
+        <v>2</v>
+      </c>
+      <c r="M140">
+        <v>0.36</v>
+      </c>
+      <c r="N140">
+        <v>1.5</v>
+      </c>
+      <c r="O140">
+        <v>0.46</v>
+      </c>
+      <c r="P140">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>42957.59716435185</v>
+      </c>
+      <c r="B141" t="s">
+        <v>16</v>
+      </c>
+      <c r="C141">
+        <v>1</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="E141">
+        <v>6</v>
+      </c>
+      <c r="F141">
+        <v>59.195022090584999</v>
+      </c>
+      <c r="G141">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H141">
+        <v>0.3</v>
+      </c>
+      <c r="I141">
+        <v>0.1</v>
+      </c>
+      <c r="J141">
+        <v>4</v>
+      </c>
+      <c r="K141">
+        <v>4</v>
+      </c>
+      <c r="L141">
+        <v>2</v>
+      </c>
+      <c r="M141">
+        <v>0.36</v>
+      </c>
+      <c r="N141">
+        <v>1.5</v>
+      </c>
+      <c r="O141">
+        <v>0.46</v>
+      </c>
+      <c r="P141">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>42957.598391203705</v>
+      </c>
+      <c r="B142" t="s">
+        <v>16</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>6</v>
+      </c>
+      <c r="F142">
+        <v>59.018364288738205</v>
+      </c>
+      <c r="G142">
+        <v>4.9950049950049946</v>
+      </c>
+      <c r="H142">
+        <v>0.3</v>
+      </c>
+      <c r="I142">
+        <v>0.1</v>
+      </c>
+      <c r="J142">
+        <v>4</v>
+      </c>
+      <c r="K142">
+        <v>4</v>
+      </c>
+      <c r="L142">
+        <v>2</v>
+      </c>
+      <c r="M142">
+        <v>0.36</v>
+      </c>
+      <c r="N142">
+        <v>1.5</v>
+      </c>
+      <c r="O142">
+        <v>0.46</v>
+      </c>
+      <c r="P142">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>42957.600902777776</v>
+      </c>
+      <c r="B143" t="s">
+        <v>16</v>
+      </c>
+      <c r="C143">
+        <v>1</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143">
+        <v>6</v>
+      </c>
+      <c r="F143">
+        <v>59.375413548486812</v>
+      </c>
+      <c r="G143">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H143">
+        <v>0.3</v>
+      </c>
+      <c r="I143">
+        <v>0.1</v>
+      </c>
+      <c r="J143">
+        <v>4</v>
+      </c>
+      <c r="K143">
+        <v>4</v>
+      </c>
+      <c r="L143">
+        <v>2</v>
+      </c>
+      <c r="M143">
+        <v>0.36</v>
+      </c>
+      <c r="N143">
+        <v>1.5</v>
+      </c>
+      <c r="O143">
+        <v>0.46</v>
+      </c>
+      <c r="P143">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>42957.602118055554</v>
+      </c>
+      <c r="B144" t="s">
+        <v>16</v>
+      </c>
+      <c r="C144">
+        <v>1</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144">
+        <v>6</v>
+      </c>
+      <c r="F144">
+        <v>59.025479610647636</v>
+      </c>
+      <c r="G144">
+        <v>5.022977022977023</v>
+      </c>
+      <c r="H144">
+        <v>0.3</v>
+      </c>
+      <c r="I144">
+        <v>0.1</v>
+      </c>
+      <c r="J144">
+        <v>4</v>
+      </c>
+      <c r="K144">
+        <v>4</v>
+      </c>
+      <c r="L144">
+        <v>2</v>
+      </c>
+      <c r="M144">
+        <v>0.36</v>
+      </c>
+      <c r="N144">
+        <v>1.5</v>
+      </c>
+      <c r="O144">
+        <v>0.46</v>
+      </c>
+      <c r="P144">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>42957.603483796294</v>
+      </c>
+      <c r="B145" t="s">
+        <v>16</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+      <c r="E145">
+        <v>6</v>
+      </c>
+      <c r="F145">
+        <v>21.082561861477778</v>
+      </c>
+      <c r="G145">
+        <v>5.0189810189810187</v>
+      </c>
+      <c r="H145">
+        <v>0.3</v>
+      </c>
+      <c r="I145">
+        <v>0.1</v>
+      </c>
+      <c r="J145">
+        <v>4</v>
+      </c>
+      <c r="K145">
+        <v>4</v>
+      </c>
+      <c r="L145">
+        <v>2</v>
+      </c>
+      <c r="M145">
+        <v>0.36</v>
+      </c>
+      <c r="N145">
+        <v>1.5</v>
+      </c>
+      <c r="O145">
+        <v>0.46</v>
+      </c>
+      <c r="P145">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>42957.626006944447</v>
+      </c>
+      <c r="B146" t="s">
+        <v>16</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146">
+        <v>6</v>
+      </c>
+      <c r="F146">
+        <v>19.258903832117316</v>
+      </c>
+      <c r="G146">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H146">
+        <v>0.3</v>
+      </c>
+      <c r="I146">
+        <v>0.1</v>
+      </c>
+      <c r="J146">
+        <v>4</v>
+      </c>
+      <c r="K146">
+        <v>4</v>
+      </c>
+      <c r="L146">
+        <v>2</v>
+      </c>
+      <c r="M146">
+        <v>0.36</v>
+      </c>
+      <c r="N146">
+        <v>1.5</v>
+      </c>
+      <c r="O146">
+        <v>0.46</v>
+      </c>
+      <c r="P146">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>42957.627187500002</v>
+      </c>
+      <c r="B147" t="s">
+        <v>16</v>
+      </c>
+      <c r="C147">
+        <v>1</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+      <c r="E147">
+        <v>6</v>
+      </c>
+      <c r="F147">
+        <v>19.06129045367377</v>
+      </c>
+      <c r="G147">
+        <v>5.0189810189810187</v>
+      </c>
+      <c r="H147">
+        <v>0.3</v>
+      </c>
+      <c r="I147">
+        <v>0.1</v>
+      </c>
+      <c r="J147">
+        <v>4</v>
+      </c>
+      <c r="K147">
+        <v>4</v>
+      </c>
+      <c r="L147">
+        <v>2</v>
+      </c>
+      <c r="M147">
+        <v>0.36</v>
+      </c>
+      <c r="N147">
+        <v>1.5</v>
+      </c>
+      <c r="O147">
+        <v>0.46</v>
+      </c>
+      <c r="P147">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>42957.641458333332</v>
+      </c>
+      <c r="B148" t="s">
+        <v>20</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
+      </c>
+      <c r="D148">
+        <v>1000</v>
+      </c>
+      <c r="E148">
+        <v>2</v>
+      </c>
+      <c r="F148">
+        <v>76.406863232927591</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+      <c r="H148">
+        <v>0.3</v>
+      </c>
+      <c r="I148">
+        <v>0.1</v>
+      </c>
+      <c r="J148">
+        <v>4</v>
+      </c>
+      <c r="K148">
+        <v>4</v>
+      </c>
+      <c r="L148">
+        <v>2</v>
+      </c>
+      <c r="M148">
+        <v>0.36</v>
+      </c>
+      <c r="N148">
+        <v>1.5</v>
+      </c>
+      <c r="O148">
+        <v>0.46</v>
+      </c>
+      <c r="P148">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>42957.642060185186</v>
+      </c>
+      <c r="B149" t="s">
+        <v>20</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
+      </c>
+      <c r="D149">
+        <v>1000</v>
+      </c>
+      <c r="E149">
+        <v>2</v>
+      </c>
+      <c r="F149">
+        <v>24.58546722059258</v>
+      </c>
+      <c r="G149">
+        <v>0</v>
+      </c>
+      <c r="H149">
+        <v>0.3</v>
+      </c>
+      <c r="I149">
+        <v>0.1</v>
+      </c>
+      <c r="J149">
+        <v>4</v>
+      </c>
+      <c r="K149">
+        <v>4</v>
+      </c>
+      <c r="L149">
+        <v>2</v>
+      </c>
+      <c r="M149">
+        <v>0.36</v>
+      </c>
+      <c r="N149">
+        <v>1.5</v>
+      </c>
+      <c r="O149">
+        <v>0.46</v>
+      </c>
+      <c r="P149">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>42957.642256944448</v>
+      </c>
+      <c r="B150" t="s">
+        <v>20</v>
+      </c>
+      <c r="C150">
+        <v>1</v>
+      </c>
+      <c r="D150">
+        <v>1000</v>
+      </c>
+      <c r="E150">
+        <v>2</v>
+      </c>
+      <c r="F150">
+        <v>4.4351075666053461</v>
+      </c>
+      <c r="G150">
+        <v>0</v>
+      </c>
+      <c r="H150">
+        <v>0.3</v>
+      </c>
+      <c r="I150">
+        <v>0.1</v>
+      </c>
+      <c r="J150">
+        <v>4</v>
+      </c>
+      <c r="K150">
+        <v>4</v>
+      </c>
+      <c r="L150">
+        <v>2</v>
+      </c>
+      <c r="M150">
+        <v>0.36</v>
+      </c>
+      <c r="N150">
+        <v>1.5</v>
+      </c>
+      <c r="O150">
+        <v>0.46</v>
+      </c>
+      <c r="P150">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>42957.646898148145</v>
+      </c>
+      <c r="B151" t="s">
+        <v>20</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+      <c r="E151">
+        <v>6</v>
+      </c>
+      <c r="F151">
+        <v>29.867333613432201</v>
+      </c>
+      <c r="G151">
+        <v>0.62937062937062938</v>
+      </c>
+      <c r="H151">
+        <v>0.3</v>
+      </c>
+      <c r="I151">
+        <v>0.1</v>
+      </c>
+      <c r="J151">
+        <v>4</v>
+      </c>
+      <c r="K151">
+        <v>4</v>
+      </c>
+      <c r="L151">
+        <v>2</v>
+      </c>
+      <c r="M151">
+        <v>0.36</v>
+      </c>
+      <c r="N151">
+        <v>1.5</v>
+      </c>
+      <c r="O151">
+        <v>0.46</v>
+      </c>
+      <c r="P151">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>42957.648715277777</v>
+      </c>
+      <c r="B152" t="s">
+        <v>20</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+      <c r="E152">
+        <v>6</v>
+      </c>
+      <c r="F152">
+        <v>29.688067884190104</v>
+      </c>
+      <c r="G152">
+        <v>0.62537462537462529</v>
+      </c>
+      <c r="H152">
+        <v>0.3</v>
+      </c>
+      <c r="I152">
+        <v>0.1</v>
+      </c>
+      <c r="J152">
+        <v>4</v>
+      </c>
+      <c r="K152">
+        <v>4</v>
+      </c>
+      <c r="L152">
+        <v>2</v>
+      </c>
+      <c r="M152">
+        <v>0.36</v>
+      </c>
+      <c r="N152">
+        <v>1.5</v>
+      </c>
+      <c r="O152">
+        <v>0.46</v>
+      </c>
+      <c r="P152">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>42957.65184027778</v>
+      </c>
+      <c r="B153" t="s">
+        <v>20</v>
+      </c>
+      <c r="C153">
+        <v>1</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+      <c r="E153">
+        <v>6</v>
+      </c>
+      <c r="F153">
+        <v>34.676261812871132</v>
+      </c>
+      <c r="G153">
+        <v>0.62537462537462529</v>
+      </c>
+      <c r="H153">
+        <v>0.3</v>
+      </c>
+      <c r="I153">
+        <v>0.1</v>
+      </c>
+      <c r="J153">
+        <v>4</v>
+      </c>
+      <c r="K153">
+        <v>4</v>
+      </c>
+      <c r="L153">
+        <v>2</v>
+      </c>
+      <c r="M153">
+        <v>0.36</v>
+      </c>
+      <c r="N153">
+        <v>1.5</v>
+      </c>
+      <c r="O153">
+        <v>0.46</v>
+      </c>
+      <c r="P153">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>42957.652002314811</v>
+      </c>
+      <c r="B154" t="s">
+        <v>20</v>
+      </c>
+      <c r="C154">
+        <v>1</v>
+      </c>
+      <c r="D154">
+        <v>100</v>
+      </c>
+      <c r="E154">
+        <v>6</v>
+      </c>
+      <c r="F154">
+        <v>8.6008296729019058</v>
+      </c>
+      <c r="G154">
+        <v>0.73260073260073255</v>
+      </c>
+      <c r="H154">
+        <v>0.3</v>
+      </c>
+      <c r="I154">
+        <v>0.1</v>
+      </c>
+      <c r="J154">
+        <v>4</v>
+      </c>
+      <c r="K154">
+        <v>4</v>
+      </c>
+      <c r="L154">
+        <v>2</v>
+      </c>
+      <c r="M154">
+        <v>0.36</v>
+      </c>
+      <c r="N154">
+        <v>1.5</v>
+      </c>
+      <c r="O154">
+        <v>0.46</v>
+      </c>
+      <c r="P154">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>42957.656504629631</v>
+      </c>
+      <c r="B155" t="s">
+        <v>20</v>
+      </c>
+      <c r="C155">
+        <v>1</v>
+      </c>
+      <c r="D155">
+        <v>100</v>
+      </c>
+      <c r="E155">
+        <v>6</v>
+      </c>
+      <c r="F155">
+        <v>8.4300353878148027</v>
+      </c>
+      <c r="G155">
+        <v>0.73260073260073255</v>
+      </c>
+      <c r="H155">
+        <v>0.3</v>
+      </c>
+      <c r="I155">
+        <v>0.1</v>
+      </c>
+      <c r="J155">
+        <v>4</v>
+      </c>
+      <c r="K155">
+        <v>4</v>
+      </c>
+      <c r="L155">
+        <v>2</v>
+      </c>
+      <c r="M155">
+        <v>0.36</v>
+      </c>
+      <c r="N155">
+        <v>1.5</v>
+      </c>
+      <c r="O155">
+        <v>0.46</v>
+      </c>
+      <c r="P155">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>42957.657164351855</v>
+      </c>
+      <c r="B156" t="s">
+        <v>20</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+      <c r="D156">
+        <v>100</v>
+      </c>
+      <c r="E156">
+        <v>6</v>
+      </c>
+      <c r="F156">
+        <v>8.278543925337118</v>
+      </c>
+      <c r="G156">
+        <v>0.73260073260073255</v>
+      </c>
+      <c r="H156">
+        <v>0.3</v>
+      </c>
+      <c r="I156">
+        <v>0.1</v>
+      </c>
+      <c r="J156">
+        <v>4</v>
+      </c>
+      <c r="K156">
+        <v>4</v>
+      </c>
+      <c r="L156">
+        <v>2</v>
+      </c>
+      <c r="M156">
+        <v>0.36</v>
+      </c>
+      <c r="N156">
+        <v>1.5</v>
+      </c>
+      <c r="O156">
+        <v>0.46</v>
+      </c>
+      <c r="P156">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>42957.660578703704</v>
+      </c>
+      <c r="B157" t="s">
+        <v>20</v>
+      </c>
+      <c r="C157">
+        <v>1</v>
+      </c>
+      <c r="D157">
+        <v>100</v>
+      </c>
+      <c r="E157">
+        <v>6</v>
+      </c>
+      <c r="F157">
+        <v>8.5740464185477077</v>
+      </c>
+      <c r="G157">
+        <v>0.73260073260073255</v>
+      </c>
+      <c r="H157">
+        <v>0.3</v>
+      </c>
+      <c r="I157">
+        <v>0.1</v>
+      </c>
+      <c r="J157">
+        <v>4</v>
+      </c>
+      <c r="K157">
+        <v>4</v>
+      </c>
+      <c r="L157">
+        <v>2</v>
+      </c>
+      <c r="M157">
+        <v>0.36</v>
+      </c>
+      <c r="N157">
+        <v>1.5</v>
+      </c>
+      <c r="O157">
+        <v>0.46</v>
+      </c>
+      <c r="P157">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>42957.663194444445</v>
+      </c>
+      <c r="B158" t="s">
+        <v>20</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+      <c r="D158">
+        <v>100</v>
+      </c>
+      <c r="E158">
+        <v>6</v>
+      </c>
+      <c r="F158">
+        <v>14.7483695653913</v>
+      </c>
+      <c r="G158">
+        <v>0.73260073260073255</v>
+      </c>
+      <c r="H158">
+        <v>0.3</v>
+      </c>
+      <c r="I158">
+        <v>0.1</v>
+      </c>
+      <c r="J158">
+        <v>4</v>
+      </c>
+      <c r="K158">
+        <v>4</v>
+      </c>
+      <c r="L158">
+        <v>2</v>
+      </c>
+      <c r="M158">
+        <v>0.36</v>
+      </c>
+      <c r="N158">
+        <v>1.5</v>
+      </c>
+      <c r="O158">
+        <v>0.46</v>
+      </c>
+      <c r="P158">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>42960.496620370373</v>
+      </c>
+      <c r="B159" t="s">
+        <v>17</v>
+      </c>
+      <c r="C159">
+        <v>1</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+      <c r="E159">
+        <v>6</v>
+      </c>
+      <c r="F159">
+        <v>78.309013477064795</v>
+      </c>
+      <c r="G159">
+        <v>4.9990009990009989</v>
+      </c>
+      <c r="H159">
+        <v>0.3</v>
+      </c>
+      <c r="I159">
+        <v>0.1</v>
+      </c>
+      <c r="J159">
+        <v>4</v>
+      </c>
+      <c r="K159">
+        <v>4</v>
+      </c>
+      <c r="L159">
+        <v>2</v>
+      </c>
+      <c r="M159">
+        <v>0.36</v>
+      </c>
+      <c r="N159">
+        <v>1.5</v>
+      </c>
+      <c r="O159">
+        <v>0.46</v>
+      </c>
+      <c r="P159">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>42960.497673611113</v>
+      </c>
+      <c r="B160" t="s">
+        <v>18</v>
+      </c>
+      <c r="C160">
+        <v>1</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+      <c r="E160">
+        <v>6</v>
+      </c>
+      <c r="F160">
+        <v>22.906805154544497</v>
+      </c>
+      <c r="G160">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H160">
+        <v>0.3</v>
+      </c>
+      <c r="I160">
+        <v>0.1</v>
+      </c>
+      <c r="J160">
+        <v>4</v>
+      </c>
+      <c r="K160">
+        <v>4</v>
+      </c>
+      <c r="L160">
+        <v>2</v>
+      </c>
+      <c r="M160">
+        <v>0.36</v>
+      </c>
+      <c r="N160">
+        <v>1.5</v>
+      </c>
+      <c r="O160">
+        <v>0.46</v>
+      </c>
+      <c r="P160">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>42960.497997685183</v>
+      </c>
+      <c r="B161" t="s">
+        <v>19</v>
+      </c>
+      <c r="C161">
+        <v>1</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+      <c r="E161">
+        <v>6</v>
+      </c>
+      <c r="F161">
+        <v>20.166203052907008</v>
+      </c>
+      <c r="G161">
+        <v>5.0029970029970023</v>
+      </c>
+      <c r="H161">
+        <v>0.3</v>
+      </c>
+      <c r="I161">
+        <v>0.1</v>
+      </c>
+      <c r="J161">
+        <v>4</v>
+      </c>
+      <c r="K161">
+        <v>4</v>
+      </c>
+      <c r="L161">
+        <v>2</v>
+      </c>
+      <c r="M161">
+        <v>0.36</v>
+      </c>
+      <c r="N161">
+        <v>1.5</v>
+      </c>
+      <c r="O161">
+        <v>0.46</v>
+      </c>
+      <c r="P161">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>42960.499236111114</v>
+      </c>
+      <c r="B162" t="s">
+        <v>18</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+      <c r="E162">
+        <v>6</v>
+      </c>
+      <c r="F162">
+        <v>19.463902604951478</v>
+      </c>
+      <c r="G162">
+        <v>4.9930069930069925</v>
+      </c>
+      <c r="H162">
+        <v>0.3</v>
+      </c>
+      <c r="I162">
+        <v>0.1</v>
+      </c>
+      <c r="J162">
+        <v>4</v>
+      </c>
+      <c r="K162">
+        <v>4</v>
+      </c>
+      <c r="L162">
+        <v>2</v>
+      </c>
+      <c r="M162">
+        <v>0.36</v>
+      </c>
+      <c r="N162">
+        <v>1.5</v>
+      </c>
+      <c r="O162">
+        <v>0.46</v>
+      </c>
+      <c r="P162">
+        <v>4.1849999999999996</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>42960.499490740738</v>
+      </c>
+      <c r="B163" t="s">
+        <v>19</v>
+      </c>
+      <c r="C163">
+        <v>0</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+      <c r="E163">
+        <v>6</v>
+      </c>
+      <c r="F163">
+        <v>20.195672632473912</v>
+      </c>
+      <c r="G163">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H163">
+        <v>0.3</v>
+      </c>
+      <c r="I163">
+        <v>0.1</v>
+      </c>
+      <c r="J163">
+        <v>4</v>
+      </c>
+      <c r="K163">
+        <v>4</v>
+      </c>
+      <c r="L163">
+        <v>2</v>
+      </c>
+      <c r="M163">
+        <v>0.36</v>
+      </c>
+      <c r="N163">
+        <v>1.5</v>
+      </c>
+      <c r="O163">
+        <v>0.46</v>
+      </c>
+      <c r="P163">
+        <v>4.3616999999999999</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>42960.4997337963</v>
+      </c>
+      <c r="B164" t="s">
+        <v>17</v>
+      </c>
+      <c r="C164">
+        <v>0</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+      <c r="E164">
+        <v>6</v>
+      </c>
+      <c r="F164">
+        <v>18.925173923157978</v>
+      </c>
+      <c r="G164">
+        <v>4.9870129870129869</v>
+      </c>
+      <c r="H164">
+        <v>0.3</v>
+      </c>
+      <c r="I164">
+        <v>0.1</v>
+      </c>
+      <c r="J164">
+        <v>4</v>
+      </c>
+      <c r="K164">
+        <v>4</v>
+      </c>
+      <c r="L164">
+        <v>2</v>
+      </c>
+      <c r="M164">
+        <v>0.36</v>
+      </c>
+      <c r="N164">
+        <v>1.5</v>
+      </c>
+      <c r="O164">
+        <v>0.46</v>
+      </c>
+      <c r="P164">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>42960.499976851854</v>
+      </c>
+      <c r="B165" t="s">
+        <v>18</v>
+      </c>
+      <c r="C165">
+        <v>1</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+      <c r="E165">
+        <v>6</v>
+      </c>
+      <c r="F165">
+        <v>19.263766096751866</v>
+      </c>
+      <c r="G165">
+        <v>4.9870129870129869</v>
+      </c>
+      <c r="H165">
+        <v>0.3</v>
+      </c>
+      <c r="I165">
+        <v>0.1</v>
+      </c>
+      <c r="J165">
+        <v>4</v>
+      </c>
+      <c r="K165">
+        <v>4</v>
+      </c>
+      <c r="L165">
+        <v>2</v>
+      </c>
+      <c r="M165">
+        <v>0.36</v>
+      </c>
+      <c r="N165">
+        <v>1.5</v>
+      </c>
+      <c r="O165">
+        <v>0.46</v>
+      </c>
+      <c r="P165">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>42960.500219907408</v>
+      </c>
+      <c r="B166" t="s">
+        <v>19</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+      <c r="D166">
+        <v>1</v>
+      </c>
+      <c r="E166">
+        <v>6</v>
+      </c>
+      <c r="F166">
+        <v>19.483969566287275</v>
+      </c>
+      <c r="G166">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H166">
+        <v>0.3</v>
+      </c>
+      <c r="I166">
+        <v>0.1</v>
+      </c>
+      <c r="J166">
+        <v>4</v>
+      </c>
+      <c r="K166">
+        <v>4</v>
+      </c>
+      <c r="L166">
+        <v>2</v>
+      </c>
+      <c r="M166">
+        <v>0.36</v>
+      </c>
+      <c r="N166">
+        <v>1.5</v>
+      </c>
+      <c r="O166">
+        <v>0.46</v>
+      </c>
+      <c r="P166">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>42960.500451388885</v>
+      </c>
+      <c r="B167" t="s">
+        <v>17</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+      <c r="E167">
+        <v>6</v>
+      </c>
+      <c r="F167">
+        <v>18.600395764981904</v>
+      </c>
+      <c r="G167">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H167">
+        <v>0.3</v>
+      </c>
+      <c r="I167">
+        <v>0.1</v>
+      </c>
+      <c r="J167">
+        <v>4</v>
+      </c>
+      <c r="K167">
+        <v>4</v>
+      </c>
+      <c r="L167">
+        <v>2</v>
+      </c>
+      <c r="M167">
+        <v>0.36</v>
+      </c>
+      <c r="N167">
+        <v>1.5</v>
+      </c>
+      <c r="O167">
+        <v>0.46</v>
+      </c>
+      <c r="P167">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>42960.500671296293</v>
+      </c>
+      <c r="B168" t="s">
+        <v>18</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+      <c r="E168">
+        <v>6</v>
+      </c>
+      <c r="F168">
+        <v>18.203098025750965</v>
+      </c>
+      <c r="G168">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H168">
+        <v>0.3</v>
+      </c>
+      <c r="I168">
+        <v>0.1</v>
+      </c>
+      <c r="J168">
+        <v>4</v>
+      </c>
+      <c r="K168">
+        <v>4</v>
+      </c>
+      <c r="L168">
+        <v>2</v>
+      </c>
+      <c r="M168">
+        <v>0.36</v>
+      </c>
+      <c r="N168">
+        <v>1.5</v>
+      </c>
+      <c r="O168">
+        <v>0.46</v>
+      </c>
+      <c r="P168">
+        <v>4.1849999999999996</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>42960.500902777778</v>
+      </c>
+      <c r="B169" t="s">
+        <v>19</v>
+      </c>
+      <c r="C169">
+        <v>0</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+      <c r="E169">
+        <v>6</v>
+      </c>
+      <c r="F169">
+        <v>17.754741228004214</v>
+      </c>
+      <c r="G169">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H169">
+        <v>0.3</v>
+      </c>
+      <c r="I169">
+        <v>0.1</v>
+      </c>
+      <c r="J169">
+        <v>4</v>
+      </c>
+      <c r="K169">
+        <v>4</v>
+      </c>
+      <c r="L169">
+        <v>2</v>
+      </c>
+      <c r="M169">
+        <v>0.36</v>
+      </c>
+      <c r="N169">
+        <v>1.5</v>
+      </c>
+      <c r="O169">
+        <v>0.46</v>
+      </c>
+      <c r="P169">
+        <v>4.3616999999999999</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <v>42960.501122685186</v>
+      </c>
+      <c r="B170" t="s">
+        <v>17</v>
+      </c>
+      <c r="C170">
+        <v>0</v>
+      </c>
+      <c r="D170">
+        <v>1</v>
+      </c>
+      <c r="E170">
+        <v>6</v>
+      </c>
+      <c r="F170">
+        <v>17.820155406873472</v>
+      </c>
+      <c r="G170">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H170">
+        <v>0.3</v>
+      </c>
+      <c r="I170">
+        <v>0.1</v>
+      </c>
+      <c r="J170">
+        <v>4</v>
+      </c>
+      <c r="K170">
+        <v>4</v>
+      </c>
+      <c r="L170">
+        <v>2</v>
+      </c>
+      <c r="M170">
+        <v>0.36</v>
+      </c>
+      <c r="N170">
+        <v>1.5</v>
+      </c>
+      <c r="O170">
+        <v>0.46</v>
+      </c>
+      <c r="P170">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <v>42960.501354166663</v>
+      </c>
+      <c r="B171" t="s">
+        <v>18</v>
+      </c>
+      <c r="C171">
+        <v>1</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+      <c r="E171">
+        <v>6</v>
+      </c>
+      <c r="F171">
+        <v>18.453888483744613</v>
+      </c>
+      <c r="G171">
+        <v>5.0089910089910088</v>
+      </c>
+      <c r="H171">
+        <v>0.3</v>
+      </c>
+      <c r="I171">
+        <v>0.1</v>
+      </c>
+      <c r="J171">
+        <v>4</v>
+      </c>
+      <c r="K171">
+        <v>4</v>
+      </c>
+      <c r="L171">
+        <v>2</v>
+      </c>
+      <c r="M171">
+        <v>0.36</v>
+      </c>
+      <c r="N171">
+        <v>1.5</v>
+      </c>
+      <c r="O171">
+        <v>0.46</v>
+      </c>
+      <c r="P171">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>42960.501585648148</v>
+      </c>
+      <c r="B172" t="s">
+        <v>19</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+      <c r="E172">
+        <v>6</v>
+      </c>
+      <c r="F172">
+        <v>18.173215017693906</v>
+      </c>
+      <c r="G172">
+        <v>5.0029970029970023</v>
+      </c>
+      <c r="H172">
+        <v>0.3</v>
+      </c>
+      <c r="I172">
+        <v>0.1</v>
+      </c>
+      <c r="J172">
+        <v>4</v>
+      </c>
+      <c r="K172">
+        <v>4</v>
+      </c>
+      <c r="L172">
+        <v>2</v>
+      </c>
+      <c r="M172">
+        <v>0.36</v>
+      </c>
+      <c r="N172">
+        <v>1.5</v>
+      </c>
+      <c r="O172">
+        <v>0.46</v>
+      </c>
+      <c r="P172">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>42960.501805555556</v>
+      </c>
+      <c r="B173" t="s">
+        <v>17</v>
+      </c>
+      <c r="C173">
+        <v>1</v>
+      </c>
+      <c r="D173">
+        <v>1</v>
+      </c>
+      <c r="E173">
+        <v>6</v>
+      </c>
+      <c r="F173">
+        <v>18.025063942219848</v>
+      </c>
+      <c r="G173">
+        <v>4.9990009990009989</v>
+      </c>
+      <c r="H173">
+        <v>0.3</v>
+      </c>
+      <c r="I173">
+        <v>0.1</v>
+      </c>
+      <c r="J173">
+        <v>4</v>
+      </c>
+      <c r="K173">
+        <v>4</v>
+      </c>
+      <c r="L173">
+        <v>2</v>
+      </c>
+      <c r="M173">
+        <v>0.36</v>
+      </c>
+      <c r="N173">
+        <v>1.5</v>
+      </c>
+      <c r="O173">
+        <v>0.46</v>
+      </c>
+      <c r="P173">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <v>42960.504965277774</v>
+      </c>
+      <c r="B174" t="s">
+        <v>18</v>
+      </c>
+      <c r="C174">
+        <v>0</v>
+      </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
+      <c r="E174">
+        <v>6</v>
+      </c>
+      <c r="F174">
+        <v>18.561240375067957</v>
+      </c>
+      <c r="G174">
+        <v>4.9930069930069925</v>
+      </c>
+      <c r="H174">
+        <v>0.3</v>
+      </c>
+      <c r="I174">
+        <v>0.1</v>
+      </c>
+      <c r="J174">
+        <v>4</v>
+      </c>
+      <c r="K174">
+        <v>4</v>
+      </c>
+      <c r="L174">
+        <v>2</v>
+      </c>
+      <c r="M174">
+        <v>0.36</v>
+      </c>
+      <c r="N174">
+        <v>1.5</v>
+      </c>
+      <c r="O174">
+        <v>0.46</v>
+      </c>
+      <c r="P174">
+        <v>4.1849999999999996</v>
+      </c>
+    </row>
+    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>42960.505208333336</v>
+      </c>
+      <c r="B175" t="s">
+        <v>19</v>
+      </c>
+      <c r="C175">
+        <v>0</v>
+      </c>
+      <c r="D175">
+        <v>1</v>
+      </c>
+      <c r="E175">
+        <v>6</v>
+      </c>
+      <c r="F175">
+        <v>18.455886188128524</v>
+      </c>
+      <c r="G175">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H175">
+        <v>0.3</v>
+      </c>
+      <c r="I175">
+        <v>0.1</v>
+      </c>
+      <c r="J175">
+        <v>4</v>
+      </c>
+      <c r="K175">
+        <v>4</v>
+      </c>
+      <c r="L175">
+        <v>2</v>
+      </c>
+      <c r="M175">
+        <v>0.36</v>
+      </c>
+      <c r="N175">
+        <v>1.5</v>
+      </c>
+      <c r="O175">
+        <v>0.46</v>
+      </c>
+      <c r="P175">
+        <v>4.3616999999999999</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>42960.505439814813</v>
+      </c>
+      <c r="B176" t="s">
+        <v>17</v>
+      </c>
+      <c r="C176">
+        <v>0</v>
+      </c>
+      <c r="D176">
+        <v>1</v>
+      </c>
+      <c r="E176">
+        <v>6</v>
+      </c>
+      <c r="F176">
+        <v>18.296431107357972</v>
+      </c>
+      <c r="G176">
+        <v>4.9870129870129869</v>
+      </c>
+      <c r="H176">
+        <v>0.3</v>
+      </c>
+      <c r="I176">
+        <v>0.1</v>
+      </c>
+      <c r="J176">
+        <v>4</v>
+      </c>
+      <c r="K176">
+        <v>4</v>
+      </c>
+      <c r="L176">
+        <v>2</v>
+      </c>
+      <c r="M176">
+        <v>0.36</v>
+      </c>
+      <c r="N176">
+        <v>1.5</v>
+      </c>
+      <c r="O176">
+        <v>0.46</v>
+      </c>
+      <c r="P176">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>42960.505671296298</v>
+      </c>
+      <c r="B177" t="s">
+        <v>18</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="E177">
+        <v>6</v>
+      </c>
+      <c r="F177">
+        <v>18.534198247920777</v>
+      </c>
+      <c r="G177">
+        <v>4.9870129870129869</v>
+      </c>
+      <c r="H177">
+        <v>0.3</v>
+      </c>
+      <c r="I177">
+        <v>0.1</v>
+      </c>
+      <c r="J177">
+        <v>4</v>
+      </c>
+      <c r="K177">
+        <v>4</v>
+      </c>
+      <c r="L177">
+        <v>2</v>
+      </c>
+      <c r="M177">
+        <v>0.36</v>
+      </c>
+      <c r="N177">
+        <v>1.5</v>
+      </c>
+      <c r="O177">
+        <v>0.46</v>
+      </c>
+      <c r="P177">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>42960.505902777775</v>
+      </c>
+      <c r="B178" t="s">
+        <v>19</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
+      <c r="D178">
+        <v>1</v>
+      </c>
+      <c r="E178">
+        <v>6</v>
+      </c>
+      <c r="F178">
+        <v>18.509483415981698</v>
+      </c>
+      <c r="G178">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H178">
+        <v>0.3</v>
+      </c>
+      <c r="I178">
+        <v>0.1</v>
+      </c>
+      <c r="J178">
+        <v>4</v>
+      </c>
+      <c r="K178">
+        <v>4</v>
+      </c>
+      <c r="L178">
+        <v>2</v>
+      </c>
+      <c r="M178">
+        <v>0.36</v>
+      </c>
+      <c r="N178">
+        <v>1.5</v>
+      </c>
+      <c r="O178">
+        <v>0.46</v>
+      </c>
+      <c r="P178">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
+        <v>42960.50613425926</v>
+      </c>
+      <c r="B179" t="s">
+        <v>17</v>
+      </c>
+      <c r="C179">
+        <v>1</v>
+      </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
+      <c r="E179">
+        <v>6</v>
+      </c>
+      <c r="F179">
+        <v>18.531687277826187</v>
+      </c>
+      <c r="G179">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H179">
+        <v>0.3</v>
+      </c>
+      <c r="I179">
+        <v>0.1</v>
+      </c>
+      <c r="J179">
+        <v>4</v>
+      </c>
+      <c r="K179">
+        <v>4</v>
+      </c>
+      <c r="L179">
+        <v>2</v>
+      </c>
+      <c r="M179">
+        <v>0.36</v>
+      </c>
+      <c r="N179">
+        <v>1.5</v>
+      </c>
+      <c r="O179">
+        <v>0.46</v>
+      </c>
+      <c r="P179">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>42960.506377314814</v>
+      </c>
+      <c r="B180" t="s">
+        <v>18</v>
+      </c>
+      <c r="C180">
+        <v>0</v>
+      </c>
+      <c r="D180">
+        <v>1</v>
+      </c>
+      <c r="E180">
+        <v>6</v>
+      </c>
+      <c r="F180">
+        <v>19.212594401371867</v>
+      </c>
+      <c r="G180">
+        <v>4.9930069930069925</v>
+      </c>
+      <c r="H180">
+        <v>0.3</v>
+      </c>
+      <c r="I180">
+        <v>0.1</v>
+      </c>
+      <c r="J180">
+        <v>4</v>
+      </c>
+      <c r="K180">
+        <v>4</v>
+      </c>
+      <c r="L180">
+        <v>2</v>
+      </c>
+      <c r="M180">
+        <v>0.36</v>
+      </c>
+      <c r="N180">
+        <v>1.5</v>
+      </c>
+      <c r="O180">
+        <v>0.46</v>
+      </c>
+      <c r="P180">
+        <v>4.1849999999999996</v>
+      </c>
+    </row>
+    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <v>42960.506620370368</v>
+      </c>
+      <c r="B181" t="s">
+        <v>19</v>
+      </c>
+      <c r="C181">
+        <v>0</v>
+      </c>
+      <c r="D181">
+        <v>1</v>
+      </c>
+      <c r="E181">
+        <v>6</v>
+      </c>
+      <c r="F181">
+        <v>19.817954508146492</v>
+      </c>
+      <c r="G181">
+        <v>4.9930069930069925</v>
+      </c>
+      <c r="H181">
+        <v>0.3</v>
+      </c>
+      <c r="I181">
+        <v>0.1</v>
+      </c>
+      <c r="J181">
+        <v>4</v>
+      </c>
+      <c r="K181">
+        <v>4</v>
+      </c>
+      <c r="L181">
+        <v>2</v>
+      </c>
+      <c r="M181">
+        <v>0.36</v>
+      </c>
+      <c r="N181">
+        <v>1.5</v>
+      </c>
+      <c r="O181">
+        <v>0.46</v>
+      </c>
+      <c r="P181">
+        <v>4.3616999999999999</v>
+      </c>
+    </row>
+    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>42960.506863425922</v>
+      </c>
+      <c r="B182" t="s">
+        <v>17</v>
+      </c>
+      <c r="C182">
+        <v>0</v>
+      </c>
+      <c r="D182">
+        <v>1</v>
+      </c>
+      <c r="E182">
+        <v>6</v>
+      </c>
+      <c r="F182">
+        <v>19.572197510021322</v>
+      </c>
+      <c r="G182">
+        <v>4.9730269730269736</v>
+      </c>
+      <c r="H182">
+        <v>0.3</v>
+      </c>
+      <c r="I182">
+        <v>0.1</v>
+      </c>
+      <c r="J182">
+        <v>4</v>
+      </c>
+      <c r="K182">
+        <v>4</v>
+      </c>
+      <c r="L182">
+        <v>2</v>
+      </c>
+      <c r="M182">
+        <v>0.36</v>
+      </c>
+      <c r="N182">
+        <v>1.5</v>
+      </c>
+      <c r="O182">
+        <v>0.46</v>
+      </c>
+      <c r="P182">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>42960.507118055553</v>
+      </c>
+      <c r="B183" t="s">
+        <v>18</v>
+      </c>
+      <c r="C183">
+        <v>1</v>
+      </c>
+      <c r="D183">
+        <v>1</v>
+      </c>
+      <c r="E183">
+        <v>6</v>
+      </c>
+      <c r="F183">
+        <v>20.479820881786651</v>
+      </c>
+      <c r="G183">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H183">
+        <v>0.3</v>
+      </c>
+      <c r="I183">
+        <v>0.1</v>
+      </c>
+      <c r="J183">
+        <v>4</v>
+      </c>
+      <c r="K183">
+        <v>4</v>
+      </c>
+      <c r="L183">
+        <v>2</v>
+      </c>
+      <c r="M183">
+        <v>0.36</v>
+      </c>
+      <c r="N183">
+        <v>1.5</v>
+      </c>
+      <c r="O183">
+        <v>0.46</v>
+      </c>
+      <c r="P183">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>42960.507372685184</v>
+      </c>
+      <c r="B184" t="s">
+        <v>19</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+      <c r="D184">
+        <v>1</v>
+      </c>
+      <c r="E184">
+        <v>6</v>
+      </c>
+      <c r="F184">
+        <v>19.62903528765759</v>
+      </c>
+      <c r="G184">
+        <v>4.9990009990009989</v>
+      </c>
+      <c r="H184">
+        <v>0.3</v>
+      </c>
+      <c r="I184">
+        <v>0.1</v>
+      </c>
+      <c r="J184">
+        <v>4</v>
+      </c>
+      <c r="K184">
+        <v>4</v>
+      </c>
+      <c r="L184">
+        <v>2</v>
+      </c>
+      <c r="M184">
+        <v>0.36</v>
+      </c>
+      <c r="N184">
+        <v>1.5</v>
+      </c>
+      <c r="O184">
+        <v>0.46</v>
+      </c>
+      <c r="P184">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>42960.507615740738</v>
+      </c>
+      <c r="B185" t="s">
+        <v>17</v>
+      </c>
+      <c r="C185">
+        <v>1</v>
+      </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
+      <c r="E185">
+        <v>6</v>
+      </c>
+      <c r="F185">
+        <v>19.489024785549969</v>
+      </c>
+      <c r="G185">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H185">
+        <v>0.3</v>
+      </c>
+      <c r="I185">
+        <v>0.1</v>
+      </c>
+      <c r="J185">
+        <v>4</v>
+      </c>
+      <c r="K185">
+        <v>4</v>
+      </c>
+      <c r="L185">
+        <v>2</v>
+      </c>
+      <c r="M185">
+        <v>0.36</v>
+      </c>
+      <c r="N185">
+        <v>1.5</v>
+      </c>
+      <c r="O185">
+        <v>0.46</v>
+      </c>
+      <c r="P185">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>42960.510324074072</v>
+      </c>
+      <c r="B186" t="s">
+        <v>18</v>
+      </c>
+      <c r="C186">
+        <v>0</v>
+      </c>
+      <c r="D186">
+        <v>1</v>
+      </c>
+      <c r="E186">
+        <v>6</v>
+      </c>
+      <c r="F186">
+        <v>19.687673335174349</v>
+      </c>
+      <c r="G186">
+        <v>4.9930069930069925</v>
+      </c>
+      <c r="H186">
+        <v>0.3</v>
+      </c>
+      <c r="I186">
+        <v>0.1</v>
+      </c>
+      <c r="J186">
+        <v>4</v>
+      </c>
+      <c r="K186">
+        <v>4</v>
+      </c>
+      <c r="L186">
+        <v>2</v>
+      </c>
+      <c r="M186">
+        <v>0.36</v>
+      </c>
+      <c r="N186">
+        <v>1.5</v>
+      </c>
+      <c r="O186">
+        <v>0.46</v>
+      </c>
+      <c r="P186">
+        <v>4.1849999999999996</v>
+      </c>
+    </row>
+    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>42960.510578703703</v>
+      </c>
+      <c r="B187" t="s">
+        <v>19</v>
+      </c>
+      <c r="C187">
+        <v>0</v>
+      </c>
+      <c r="D187">
+        <v>1</v>
+      </c>
+      <c r="E187">
+        <v>6</v>
+      </c>
+      <c r="F187">
+        <v>19.742720442662876</v>
+      </c>
+      <c r="G187">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H187">
+        <v>0.3</v>
+      </c>
+      <c r="I187">
+        <v>0.1</v>
+      </c>
+      <c r="J187">
+        <v>4</v>
+      </c>
+      <c r="K187">
+        <v>4</v>
+      </c>
+      <c r="L187">
+        <v>2</v>
+      </c>
+      <c r="M187">
+        <v>0.36</v>
+      </c>
+      <c r="N187">
+        <v>1.5</v>
+      </c>
+      <c r="O187">
+        <v>0.46</v>
+      </c>
+      <c r="P187">
+        <v>4.3616999999999999</v>
+      </c>
+    </row>
+    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>42960.510821759257</v>
+      </c>
+      <c r="B188" t="s">
+        <v>17</v>
+      </c>
+      <c r="C188">
+        <v>0</v>
+      </c>
+      <c r="D188">
+        <v>1</v>
+      </c>
+      <c r="E188">
+        <v>6</v>
+      </c>
+      <c r="F188">
+        <v>19.413367051861275</v>
+      </c>
+      <c r="G188">
+        <v>4.9870129870129869</v>
+      </c>
+      <c r="H188">
+        <v>0.3</v>
+      </c>
+      <c r="I188">
+        <v>0.1</v>
+      </c>
+      <c r="J188">
+        <v>4</v>
+      </c>
+      <c r="K188">
+        <v>4</v>
+      </c>
+      <c r="L188">
+        <v>2</v>
+      </c>
+      <c r="M188">
+        <v>0.36</v>
+      </c>
+      <c r="N188">
+        <v>1.5</v>
+      </c>
+      <c r="O188">
+        <v>0.46</v>
+      </c>
+      <c r="P188">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>42960.511064814818</v>
+      </c>
+      <c r="B189" t="s">
+        <v>18</v>
+      </c>
+      <c r="C189">
+        <v>1</v>
+      </c>
+      <c r="D189">
+        <v>1</v>
+      </c>
+      <c r="E189">
+        <v>6</v>
+      </c>
+      <c r="F189">
+        <v>19.872586587189414</v>
+      </c>
+      <c r="G189">
+        <v>4.9870129870129869</v>
+      </c>
+      <c r="H189">
+        <v>0.3</v>
+      </c>
+      <c r="I189">
+        <v>0.1</v>
+      </c>
+      <c r="J189">
+        <v>4</v>
+      </c>
+      <c r="K189">
+        <v>4</v>
+      </c>
+      <c r="L189">
+        <v>2</v>
+      </c>
+      <c r="M189">
+        <v>0.36</v>
+      </c>
+      <c r="N189">
+        <v>1.5</v>
+      </c>
+      <c r="O189">
+        <v>0.46</v>
+      </c>
+      <c r="P189">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>42960.511307870373</v>
+      </c>
+      <c r="B190" t="s">
+        <v>19</v>
+      </c>
+      <c r="C190">
+        <v>1</v>
+      </c>
+      <c r="D190">
+        <v>1</v>
+      </c>
+      <c r="E190">
+        <v>6</v>
+      </c>
+      <c r="F190">
+        <v>19.739045344977598</v>
+      </c>
+      <c r="G190">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H190">
+        <v>0.3</v>
+      </c>
+      <c r="I190">
+        <v>0.1</v>
+      </c>
+      <c r="J190">
+        <v>4</v>
+      </c>
+      <c r="K190">
+        <v>4</v>
+      </c>
+      <c r="L190">
+        <v>2</v>
+      </c>
+      <c r="M190">
+        <v>0.36</v>
+      </c>
+      <c r="N190">
+        <v>1.5</v>
+      </c>
+      <c r="O190">
+        <v>0.46</v>
+      </c>
+      <c r="P190">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>42960.511562500003</v>
+      </c>
+      <c r="B191" t="s">
+        <v>17</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+      <c r="D191">
+        <v>1</v>
+      </c>
+      <c r="E191">
+        <v>6</v>
+      </c>
+      <c r="F191">
+        <v>19.716772365057356</v>
+      </c>
+      <c r="G191">
+        <v>4.9810189810189813</v>
+      </c>
+      <c r="H191">
+        <v>0.3</v>
+      </c>
+      <c r="I191">
+        <v>0.1</v>
+      </c>
+      <c r="J191">
+        <v>4</v>
+      </c>
+      <c r="K191">
+        <v>4</v>
+      </c>
+      <c r="L191">
+        <v>2</v>
+      </c>
+      <c r="M191">
+        <v>0.36</v>
+      </c>
+      <c r="N191">
+        <v>1.5</v>
+      </c>
+      <c r="O191">
+        <v>0.46</v>
+      </c>
+      <c r="P191">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>42960.511805555558</v>
+      </c>
+      <c r="B192" t="s">
+        <v>18</v>
+      </c>
+      <c r="C192">
+        <v>0</v>
+      </c>
+      <c r="D192">
+        <v>1</v>
+      </c>
+      <c r="E192">
+        <v>6</v>
+      </c>
+      <c r="F192">
+        <v>19.765673403652443</v>
+      </c>
+      <c r="G192">
+        <v>4.9930069930069925</v>
+      </c>
+      <c r="H192">
+        <v>0.3</v>
+      </c>
+      <c r="I192">
+        <v>0.1</v>
+      </c>
+      <c r="J192">
+        <v>4</v>
+      </c>
+      <c r="K192">
+        <v>4</v>
+      </c>
+      <c r="L192">
+        <v>2</v>
+      </c>
+      <c r="M192">
+        <v>0.36</v>
+      </c>
+      <c r="N192">
+        <v>1.5</v>
+      </c>
+      <c r="O192">
+        <v>0.46</v>
+      </c>
+      <c r="P192">
+        <v>4.1849999999999996</v>
+      </c>
+    </row>
+    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>42960.512048611112</v>
+      </c>
+      <c r="B193" t="s">
+        <v>19</v>
+      </c>
+      <c r="C193">
+        <v>0</v>
+      </c>
+      <c r="D193">
+        <v>1</v>
+      </c>
+      <c r="E193">
+        <v>6</v>
+      </c>
+      <c r="F193">
+        <v>19.512423814121014</v>
+      </c>
+      <c r="G193">
+        <v>4.9930069930069925</v>
+      </c>
+      <c r="H193">
+        <v>0.3</v>
+      </c>
+      <c r="I193">
+        <v>0.1</v>
+      </c>
+      <c r="J193">
+        <v>4</v>
+      </c>
+      <c r="K193">
+        <v>4</v>
+      </c>
+      <c r="L193">
+        <v>2</v>
+      </c>
+      <c r="M193">
+        <v>0.36</v>
+      </c>
+      <c r="N193">
+        <v>1.5</v>
+      </c>
+      <c r="O193">
+        <v>0.46</v>
+      </c>
+      <c r="P193">
+        <v>4.3616999999999999</v>
+      </c>
+    </row>
+    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>42960.512303240743</v>
+      </c>
+      <c r="B194" t="s">
+        <v>17</v>
+      </c>
+      <c r="C194">
+        <v>0</v>
+      </c>
+      <c r="D194">
+        <v>1</v>
+      </c>
+      <c r="E194">
+        <v>6</v>
+      </c>
+      <c r="F194">
+        <v>19.537917504376679</v>
+      </c>
+      <c r="G194">
+        <v>4.9730269730269736</v>
+      </c>
+      <c r="H194">
+        <v>0.3</v>
+      </c>
+      <c r="I194">
+        <v>0.1</v>
+      </c>
+      <c r="J194">
+        <v>4</v>
+      </c>
+      <c r="K194">
+        <v>4</v>
+      </c>
+      <c r="L194">
+        <v>2</v>
+      </c>
+      <c r="M194">
+        <v>0.36</v>
+      </c>
+      <c r="N194">
+        <v>1.5</v>
+      </c>
+      <c r="O194">
+        <v>0.46</v>
+      </c>
+      <c r="P194">
+        <v>4.2549999999999999</v>
+      </c>
+    </row>
+    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>42960.512546296297</v>
+      </c>
+      <c r="B195" t="s">
+        <v>18</v>
+      </c>
+      <c r="C195">
+        <v>1</v>
+      </c>
+      <c r="D195">
+        <v>1</v>
+      </c>
+      <c r="E195">
+        <v>6</v>
+      </c>
+      <c r="F195">
+        <v>19.894502457051594</v>
+      </c>
+      <c r="G195">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H195">
+        <v>0.3</v>
+      </c>
+      <c r="I195">
+        <v>0.1</v>
+      </c>
+      <c r="J195">
+        <v>4</v>
+      </c>
+      <c r="K195">
+        <v>4</v>
+      </c>
+      <c r="L195">
+        <v>2</v>
+      </c>
+      <c r="M195">
+        <v>0.36</v>
+      </c>
+      <c r="N195">
+        <v>1.5</v>
+      </c>
+      <c r="O195">
+        <v>0.46</v>
+      </c>
+      <c r="P195">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>42960.512789351851</v>
+      </c>
+      <c r="B196" t="s">
+        <v>19</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+      <c r="D196">
+        <v>1</v>
+      </c>
+      <c r="E196">
+        <v>6</v>
+      </c>
+      <c r="F196">
+        <v>19.703744887742324</v>
+      </c>
+      <c r="G196">
+        <v>4.9990009990009989</v>
+      </c>
+      <c r="H196">
+        <v>0.3</v>
+      </c>
+      <c r="I196">
+        <v>0.1</v>
+      </c>
+      <c r="J196">
+        <v>4</v>
+      </c>
+      <c r="K196">
+        <v>4</v>
+      </c>
+      <c r="L196">
+        <v>2</v>
+      </c>
+      <c r="M196">
+        <v>0.36</v>
+      </c>
+      <c r="N196">
+        <v>1.5</v>
+      </c>
+      <c r="O196">
+        <v>0.46</v>
+      </c>
+      <c r="P196">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>42960.513043981482</v>
+      </c>
+      <c r="B197" t="s">
+        <v>17</v>
+      </c>
+      <c r="C197">
+        <v>1</v>
+      </c>
+      <c r="D197">
+        <v>1</v>
+      </c>
+      <c r="E197">
+        <v>6</v>
+      </c>
+      <c r="F197">
+        <v>19.745414127670685</v>
+      </c>
+      <c r="G197">
+        <v>4.9910089910089912</v>
+      </c>
+      <c r="H197">
+        <v>0.3</v>
+      </c>
+      <c r="I197">
+        <v>0.1</v>
+      </c>
+      <c r="J197">
+        <v>4</v>
+      </c>
+      <c r="K197">
+        <v>4</v>
+      </c>
+      <c r="L197">
+        <v>2</v>
+      </c>
+      <c r="M197">
+        <v>0.36</v>
+      </c>
+      <c r="N197">
+        <v>1.5</v>
+      </c>
+      <c r="O197">
+        <v>0.46</v>
+      </c>
+      <c r="P197">
+        <v>4.7156000000000002</v>
+      </c>
+    </row>
+    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>42960.692754629628</v>
+      </c>
+      <c r="B198" t="s">
+        <v>20</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+      <c r="D198">
+        <v>1</v>
+      </c>
+      <c r="E198">
+        <v>6</v>
+      </c>
+      <c r="F198">
+        <v>47.198455914987328</v>
+      </c>
+      <c r="G198">
+        <v>0.62737262737262733</v>
+      </c>
+      <c r="H198">
+        <v>0.3</v>
+      </c>
+      <c r="I198">
+        <v>0.1</v>
+      </c>
+      <c r="J198">
+        <v>4</v>
+      </c>
+      <c r="K198">
+        <v>4</v>
+      </c>
+      <c r="L198">
+        <v>2</v>
+      </c>
+      <c r="M198">
+        <v>0.36</v>
+      </c>
+      <c r="N198">
+        <v>1.5</v>
+      </c>
+      <c r="O198">
+        <v>0.46</v>
+      </c>
+      <c r="P198">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>42960.693668981483</v>
+      </c>
+      <c r="B199" t="s">
+        <v>20</v>
+      </c>
+      <c r="C199">
+        <v>1</v>
+      </c>
+      <c r="D199">
+        <v>1</v>
+      </c>
+      <c r="E199">
+        <v>6</v>
+      </c>
+      <c r="F199">
+        <v>35.539485460724777</v>
+      </c>
+      <c r="G199">
+        <v>0.62537462537462529</v>
+      </c>
+      <c r="H199">
+        <v>0.3</v>
+      </c>
+      <c r="I199">
+        <v>0.1</v>
+      </c>
+      <c r="J199">
+        <v>4</v>
+      </c>
+      <c r="K199">
+        <v>4</v>
+      </c>
+      <c r="L199">
+        <v>2</v>
+      </c>
+      <c r="M199">
+        <v>0.36</v>
+      </c>
+      <c r="N199">
+        <v>1.5</v>
+      </c>
+      <c r="O199">
+        <v>0.46</v>
+      </c>
+      <c r="P199">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>42960.694895833331</v>
+      </c>
+      <c r="B200" t="s">
+        <v>20</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+      <c r="D200">
+        <v>1</v>
+      </c>
+      <c r="E200">
+        <v>6</v>
+      </c>
+      <c r="F200">
+        <v>31.824127776282708</v>
+      </c>
+      <c r="G200">
+        <v>0.62937062937062938</v>
+      </c>
+      <c r="H200">
+        <v>0.3</v>
+      </c>
+      <c r="I200">
+        <v>0.1</v>
+      </c>
+      <c r="J200">
+        <v>4</v>
+      </c>
+      <c r="K200">
+        <v>4</v>
+      </c>
+      <c r="L200">
+        <v>2</v>
+      </c>
+      <c r="M200">
+        <v>0.36</v>
+      </c>
+      <c r="N200">
+        <v>1.5</v>
+      </c>
+      <c r="O200">
+        <v>0.46</v>
+      </c>
+      <c r="P200">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>42961.610706018517</v>
+      </c>
+      <c r="B201" t="s">
+        <v>19</v>
+      </c>
+      <c r="C201">
+        <v>1</v>
+      </c>
+      <c r="D201">
+        <v>10000</v>
+      </c>
+      <c r="E201">
+        <v>1</v>
+      </c>
+      <c r="F201">
+        <v>24.679417245023899</v>
+      </c>
+      <c r="G201">
+        <v>0</v>
+      </c>
+      <c r="H201">
+        <v>0.3</v>
+      </c>
+      <c r="I201">
+        <v>0.1</v>
+      </c>
+      <c r="J201">
+        <v>4</v>
+      </c>
+      <c r="K201">
+        <v>4</v>
+      </c>
+      <c r="L201">
+        <v>2</v>
+      </c>
+      <c r="M201">
+        <v>0.36</v>
+      </c>
+      <c r="N201">
+        <v>1.5</v>
+      </c>
+      <c r="O201">
+        <v>0.46</v>
+      </c>
+      <c r="P201">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>42961.794999999998</v>
+      </c>
+      <c r="B202" t="s">
+        <v>19</v>
+      </c>
+      <c r="C202">
+        <v>1</v>
+      </c>
+      <c r="D202">
+        <v>10000</v>
+      </c>
+      <c r="E202">
+        <v>1</v>
+      </c>
+      <c r="F202">
+        <v>26.562735291943603</v>
+      </c>
+      <c r="G202">
+        <v>0</v>
+      </c>
+      <c r="H202">
+        <v>0.3</v>
+      </c>
+      <c r="I202">
+        <v>0.1</v>
+      </c>
+      <c r="J202">
+        <v>4</v>
+      </c>
+      <c r="K202">
+        <v>4</v>
+      </c>
+      <c r="L202">
+        <v>2</v>
+      </c>
+      <c r="M202">
+        <v>0.36</v>
+      </c>
+      <c r="N202">
+        <v>1.5</v>
+      </c>
+      <c r="O202">
+        <v>0.46</v>
+      </c>
+      <c r="P202">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Clean up turning the various plots and maps on and off
The accumulated figure types often required commenting blocks of code in or out between runs.  Now all of the major figures can be controlled with flags (names starting with "do') at the top of the file.  This should be less time consuming and error prone.
The main file is almost 80 lines shorter now thanks to moving code out to functions.  It's still too long!
</commit_message>
<xml_diff>
--- a/RunSummaries.xlsx
+++ b/RunSummaries.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -455,10 +455,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P202"/>
+  <dimension ref="A1:P205"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="A202" sqref="A202:P202"/>
+      <selection activeCell="A205" sqref="A205:P205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10563,6 +10563,156 @@
         <v>4.8444000000000003</v>
       </c>
     </row>
+    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>42962.441550925927</v>
+      </c>
+      <c r="B203" t="s">
+        <v>19</v>
+      </c>
+      <c r="C203">
+        <v>1</v>
+      </c>
+      <c r="D203">
+        <v>10000</v>
+      </c>
+      <c r="E203">
+        <v>1</v>
+      </c>
+      <c r="F203">
+        <v>8.8682453696637253</v>
+      </c>
+      <c r="G203">
+        <v>0</v>
+      </c>
+      <c r="H203">
+        <v>0.3</v>
+      </c>
+      <c r="I203">
+        <v>0.1</v>
+      </c>
+      <c r="J203">
+        <v>4</v>
+      </c>
+      <c r="K203">
+        <v>4</v>
+      </c>
+      <c r="L203">
+        <v>2</v>
+      </c>
+      <c r="M203">
+        <v>0.36</v>
+      </c>
+      <c r="N203">
+        <v>1.5</v>
+      </c>
+      <c r="O203">
+        <v>0.46</v>
+      </c>
+      <c r="P203">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>42962.480162037034</v>
+      </c>
+      <c r="B204" t="s">
+        <v>19</v>
+      </c>
+      <c r="C204">
+        <v>1</v>
+      </c>
+      <c r="D204">
+        <v>10000</v>
+      </c>
+      <c r="E204">
+        <v>2</v>
+      </c>
+      <c r="F204">
+        <v>4.2437469940933035</v>
+      </c>
+      <c r="G204">
+        <v>0</v>
+      </c>
+      <c r="H204">
+        <v>0.3</v>
+      </c>
+      <c r="I204">
+        <v>0.1</v>
+      </c>
+      <c r="J204">
+        <v>4</v>
+      </c>
+      <c r="K204">
+        <v>4</v>
+      </c>
+      <c r="L204">
+        <v>2</v>
+      </c>
+      <c r="M204">
+        <v>0.36</v>
+      </c>
+      <c r="N204">
+        <v>1.5</v>
+      </c>
+      <c r="O204">
+        <v>0.46</v>
+      </c>
+      <c r="P204">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>42962.489386574074</v>
+      </c>
+      <c r="B205" t="s">
+        <v>19</v>
+      </c>
+      <c r="C205">
+        <v>1</v>
+      </c>
+      <c r="D205">
+        <v>1</v>
+      </c>
+      <c r="E205">
+        <v>6</v>
+      </c>
+      <c r="F205">
+        <v>39.402462387567489</v>
+      </c>
+      <c r="G205">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H205">
+        <v>0.3</v>
+      </c>
+      <c r="I205">
+        <v>0.1</v>
+      </c>
+      <c r="J205">
+        <v>4</v>
+      </c>
+      <c r="K205">
+        <v>4</v>
+      </c>
+      <c r="L205">
+        <v>2</v>
+      </c>
+      <c r="M205">
+        <v>0.36</v>
+      </c>
+      <c r="N205">
+        <v>1.5</v>
+      </c>
+      <c r="O205">
+        <v>0.46</v>
+      </c>
+      <c r="P205">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Move saving of long mortality and bleaching out of the main program.
Another move the shrink the main program file.
</commit_message>
<xml_diff>
--- a/RunSummaries.xlsx
+++ b/RunSummaries.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -455,10 +455,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P205"/>
+  <dimension ref="A1:P209"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="A205" sqref="A205:P205"/>
+      <selection activeCell="A209" sqref="A209:P209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10713,6 +10713,206 @@
         <v>4.8444000000000003</v>
       </c>
     </row>
+    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>42962.527442129627</v>
+      </c>
+      <c r="B206" t="s">
+        <v>19</v>
+      </c>
+      <c r="C206">
+        <v>1</v>
+      </c>
+      <c r="D206">
+        <v>1</v>
+      </c>
+      <c r="E206">
+        <v>6</v>
+      </c>
+      <c r="F206">
+        <v>19.147612058121716</v>
+      </c>
+      <c r="G206">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H206">
+        <v>0.3</v>
+      </c>
+      <c r="I206">
+        <v>0.1</v>
+      </c>
+      <c r="J206">
+        <v>4</v>
+      </c>
+      <c r="K206">
+        <v>4</v>
+      </c>
+      <c r="L206">
+        <v>2</v>
+      </c>
+      <c r="M206">
+        <v>0.36</v>
+      </c>
+      <c r="N206">
+        <v>1.5</v>
+      </c>
+      <c r="O206">
+        <v>0.46</v>
+      </c>
+      <c r="P206">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>42962.527881944443</v>
+      </c>
+      <c r="B207" t="s">
+        <v>19</v>
+      </c>
+      <c r="C207">
+        <v>1</v>
+      </c>
+      <c r="D207">
+        <v>1</v>
+      </c>
+      <c r="E207">
+        <v>6</v>
+      </c>
+      <c r="F207">
+        <v>21.710316191785406</v>
+      </c>
+      <c r="G207">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H207">
+        <v>0.3</v>
+      </c>
+      <c r="I207">
+        <v>0.1</v>
+      </c>
+      <c r="J207">
+        <v>4</v>
+      </c>
+      <c r="K207">
+        <v>4</v>
+      </c>
+      <c r="L207">
+        <v>2</v>
+      </c>
+      <c r="M207">
+        <v>0.36</v>
+      </c>
+      <c r="N207">
+        <v>1.5</v>
+      </c>
+      <c r="O207">
+        <v>0.46</v>
+      </c>
+      <c r="P207">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>42962.530034722222</v>
+      </c>
+      <c r="B208" t="s">
+        <v>19</v>
+      </c>
+      <c r="C208">
+        <v>1</v>
+      </c>
+      <c r="D208">
+        <v>100</v>
+      </c>
+      <c r="E208">
+        <v>6</v>
+      </c>
+      <c r="F208">
+        <v>7.8395451405188386</v>
+      </c>
+      <c r="G208">
+        <v>6.4685314685314683</v>
+      </c>
+      <c r="H208">
+        <v>0.3</v>
+      </c>
+      <c r="I208">
+        <v>0.1</v>
+      </c>
+      <c r="J208">
+        <v>4</v>
+      </c>
+      <c r="K208">
+        <v>4</v>
+      </c>
+      <c r="L208">
+        <v>2</v>
+      </c>
+      <c r="M208">
+        <v>0.36</v>
+      </c>
+      <c r="N208">
+        <v>1.5</v>
+      </c>
+      <c r="O208">
+        <v>0.46</v>
+      </c>
+      <c r="P208">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>42962.544351851851</v>
+      </c>
+      <c r="B209" t="s">
+        <v>19</v>
+      </c>
+      <c r="C209">
+        <v>1</v>
+      </c>
+      <c r="D209">
+        <v>100</v>
+      </c>
+      <c r="E209">
+        <v>6</v>
+      </c>
+      <c r="F209">
+        <v>26.86526018232394</v>
+      </c>
+      <c r="G209">
+        <v>6.4685314685314683</v>
+      </c>
+      <c r="H209">
+        <v>0.3</v>
+      </c>
+      <c r="I209">
+        <v>0.1</v>
+      </c>
+      <c r="J209">
+        <v>4</v>
+      </c>
+      <c r="K209">
+        <v>4</v>
+      </c>
+      <c r="L209">
+        <v>2</v>
+      </c>
+      <c r="M209">
+        <v>0.36</v>
+      </c>
+      <c r="N209">
+        <v>1.5</v>
+      </c>
+      <c r="O209">
+        <v>0.46</v>
+      </c>
+      <c r="P209">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
First implementation of ode45 Dormand-Prince solver
Results are reasonable but mixed.  Full runs with stats are not implemented yet.  Super symbiont introduction is not implemented.  The new functionality can easily be turned off with doDormandPrince = false.
</commit_message>
<xml_diff>
--- a/RunSummaries.xlsx
+++ b/RunSummaries.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -455,10 +455,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P211"/>
+  <dimension ref="A1:P220"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="A211" sqref="A211:P211"/>
+      <selection activeCell="A220" sqref="A220:P220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11013,6 +11013,456 @@
         <v>4.8444000000000003</v>
       </c>
     </row>
+    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>42963.427152777775</v>
+      </c>
+      <c r="B212" t="s">
+        <v>19</v>
+      </c>
+      <c r="C212">
+        <v>1</v>
+      </c>
+      <c r="D212">
+        <v>1</v>
+      </c>
+      <c r="E212">
+        <v>6</v>
+      </c>
+      <c r="F212">
+        <v>43.311756045473004</v>
+      </c>
+      <c r="G212">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H212">
+        <v>0.3</v>
+      </c>
+      <c r="I212">
+        <v>0.1</v>
+      </c>
+      <c r="J212">
+        <v>4</v>
+      </c>
+      <c r="K212">
+        <v>4</v>
+      </c>
+      <c r="L212">
+        <v>2</v>
+      </c>
+      <c r="M212">
+        <v>0.36</v>
+      </c>
+      <c r="N212">
+        <v>1.5</v>
+      </c>
+      <c r="O212">
+        <v>0.46</v>
+      </c>
+      <c r="P212">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="213" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A213" s="1">
+        <v>42963.472777777781</v>
+      </c>
+      <c r="B213" t="s">
+        <v>19</v>
+      </c>
+      <c r="C213">
+        <v>1</v>
+      </c>
+      <c r="D213">
+        <v>1</v>
+      </c>
+      <c r="E213">
+        <v>6</v>
+      </c>
+      <c r="F213">
+        <v>42.049631260625638</v>
+      </c>
+      <c r="G213">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H213">
+        <v>0.3</v>
+      </c>
+      <c r="I213">
+        <v>0.1</v>
+      </c>
+      <c r="J213">
+        <v>4</v>
+      </c>
+      <c r="K213">
+        <v>4</v>
+      </c>
+      <c r="L213">
+        <v>2</v>
+      </c>
+      <c r="M213">
+        <v>0.36</v>
+      </c>
+      <c r="N213">
+        <v>1.5</v>
+      </c>
+      <c r="O213">
+        <v>0.46</v>
+      </c>
+      <c r="P213">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="214" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
+        <v>42963.473807870374</v>
+      </c>
+      <c r="B214" t="s">
+        <v>19</v>
+      </c>
+      <c r="C214">
+        <v>1</v>
+      </c>
+      <c r="D214">
+        <v>1</v>
+      </c>
+      <c r="E214">
+        <v>11</v>
+      </c>
+      <c r="F214">
+        <v>39.755159423341347</v>
+      </c>
+      <c r="G214">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H214">
+        <v>0.3</v>
+      </c>
+      <c r="I214">
+        <v>0.1</v>
+      </c>
+      <c r="J214">
+        <v>4</v>
+      </c>
+      <c r="K214">
+        <v>4</v>
+      </c>
+      <c r="L214">
+        <v>2</v>
+      </c>
+      <c r="M214">
+        <v>0.36</v>
+      </c>
+      <c r="N214">
+        <v>1.5</v>
+      </c>
+      <c r="O214">
+        <v>0.46</v>
+      </c>
+      <c r="P214">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
+        <v>42963.474479166667</v>
+      </c>
+      <c r="B215" t="s">
+        <v>19</v>
+      </c>
+      <c r="C215">
+        <v>1</v>
+      </c>
+      <c r="D215">
+        <v>1</v>
+      </c>
+      <c r="E215">
+        <v>6</v>
+      </c>
+      <c r="F215">
+        <v>35.52102600006976</v>
+      </c>
+      <c r="G215">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H215">
+        <v>0.3</v>
+      </c>
+      <c r="I215">
+        <v>0.1</v>
+      </c>
+      <c r="J215">
+        <v>4</v>
+      </c>
+      <c r="K215">
+        <v>4</v>
+      </c>
+      <c r="L215">
+        <v>2</v>
+      </c>
+      <c r="M215">
+        <v>0.36</v>
+      </c>
+      <c r="N215">
+        <v>1.5</v>
+      </c>
+      <c r="O215">
+        <v>0.46</v>
+      </c>
+      <c r="P215">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A216" s="1">
+        <v>42963.692175925928</v>
+      </c>
+      <c r="B216" t="s">
+        <v>19</v>
+      </c>
+      <c r="C216">
+        <v>1</v>
+      </c>
+      <c r="D216">
+        <v>10000</v>
+      </c>
+      <c r="E216">
+        <v>1</v>
+      </c>
+      <c r="F216">
+        <v>14.547541572176568</v>
+      </c>
+      <c r="G216">
+        <v>0</v>
+      </c>
+      <c r="H216">
+        <v>0.3</v>
+      </c>
+      <c r="I216">
+        <v>0.1</v>
+      </c>
+      <c r="J216">
+        <v>4</v>
+      </c>
+      <c r="K216">
+        <v>4</v>
+      </c>
+      <c r="L216">
+        <v>2</v>
+      </c>
+      <c r="M216">
+        <v>0.36</v>
+      </c>
+      <c r="N216">
+        <v>1.5</v>
+      </c>
+      <c r="O216">
+        <v>0.46</v>
+      </c>
+      <c r="P216">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A217" s="1">
+        <v>42963.696458333332</v>
+      </c>
+      <c r="B217" t="s">
+        <v>19</v>
+      </c>
+      <c r="C217">
+        <v>1</v>
+      </c>
+      <c r="D217">
+        <v>10000</v>
+      </c>
+      <c r="E217">
+        <v>1</v>
+      </c>
+      <c r="F217">
+        <v>13.107532958071516</v>
+      </c>
+      <c r="G217">
+        <v>0</v>
+      </c>
+      <c r="H217">
+        <v>0.3</v>
+      </c>
+      <c r="I217">
+        <v>0.1</v>
+      </c>
+      <c r="J217">
+        <v>4</v>
+      </c>
+      <c r="K217">
+        <v>4</v>
+      </c>
+      <c r="L217">
+        <v>2</v>
+      </c>
+      <c r="M217">
+        <v>0.36</v>
+      </c>
+      <c r="N217">
+        <v>1.5</v>
+      </c>
+      <c r="O217">
+        <v>0.46</v>
+      </c>
+      <c r="P217">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A218" s="1">
+        <v>42963.711736111109</v>
+      </c>
+      <c r="B218" t="s">
+        <v>19</v>
+      </c>
+      <c r="C218">
+        <v>1</v>
+      </c>
+      <c r="D218">
+        <v>10000</v>
+      </c>
+      <c r="E218">
+        <v>1</v>
+      </c>
+      <c r="F218">
+        <v>14.766424637620409</v>
+      </c>
+      <c r="G218">
+        <v>0</v>
+      </c>
+      <c r="H218">
+        <v>0.3</v>
+      </c>
+      <c r="I218">
+        <v>0.1</v>
+      </c>
+      <c r="J218">
+        <v>4</v>
+      </c>
+      <c r="K218">
+        <v>4</v>
+      </c>
+      <c r="L218">
+        <v>2</v>
+      </c>
+      <c r="M218">
+        <v>0.36</v>
+      </c>
+      <c r="N218">
+        <v>1.5</v>
+      </c>
+      <c r="O218">
+        <v>0.46</v>
+      </c>
+      <c r="P218">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A219" s="1">
+        <v>42963.712789351855</v>
+      </c>
+      <c r="B219" t="s">
+        <v>19</v>
+      </c>
+      <c r="C219">
+        <v>1</v>
+      </c>
+      <c r="D219">
+        <v>10000</v>
+      </c>
+      <c r="E219">
+        <v>1</v>
+      </c>
+      <c r="F219">
+        <v>13.574009145926844</v>
+      </c>
+      <c r="G219">
+        <v>0</v>
+      </c>
+      <c r="H219">
+        <v>0.3</v>
+      </c>
+      <c r="I219">
+        <v>0.1</v>
+      </c>
+      <c r="J219">
+        <v>4</v>
+      </c>
+      <c r="K219">
+        <v>4</v>
+      </c>
+      <c r="L219">
+        <v>2</v>
+      </c>
+      <c r="M219">
+        <v>0.36</v>
+      </c>
+      <c r="N219">
+        <v>1.5</v>
+      </c>
+      <c r="O219">
+        <v>0.46</v>
+      </c>
+      <c r="P219">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A220" s="1">
+        <v>42963.743738425925</v>
+      </c>
+      <c r="B220" t="s">
+        <v>19</v>
+      </c>
+      <c r="C220">
+        <v>1</v>
+      </c>
+      <c r="D220">
+        <v>10000</v>
+      </c>
+      <c r="E220">
+        <v>1</v>
+      </c>
+      <c r="F220">
+        <v>14.438064040687246</v>
+      </c>
+      <c r="G220">
+        <v>0</v>
+      </c>
+      <c r="H220">
+        <v>0.3</v>
+      </c>
+      <c r="I220">
+        <v>0.1</v>
+      </c>
+      <c r="J220">
+        <v>4</v>
+      </c>
+      <c r="K220">
+        <v>4</v>
+      </c>
+      <c r="L220">
+        <v>2</v>
+      </c>
+      <c r="M220">
+        <v>0.36</v>
+      </c>
+      <c r="N220">
+        <v>1.5</v>
+      </c>
+      <c r="O220">
+        <v>0.46</v>
+      </c>
+      <c r="P220">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Move independent input calculations out of ODE function
Removed ri, gi and vgi computations from the ode function since they are independent of the solution.  Now the solver has fewer variables to deal with.  Also replaced "interp1" which turned out to be the biggest time-sink with "interp1q".  Results are the same for linear 1D interpolation.

This is still not iterating over multiple reefs or including OA and super symbionts.  It's all possible, but I want to check accuracy on one reef first.

Now only 2.2 times slower - the ratio may change after compilation.
</commit_message>
<xml_diff>
--- a/RunSummaries.xlsx
+++ b/RunSummaries.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -455,10 +455,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P220"/>
+  <dimension ref="A1:P223"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="A220" sqref="A220:P220"/>
+      <selection activeCell="A223" sqref="A223:P223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11463,6 +11463,156 @@
         <v>4.8444000000000003</v>
       </c>
     </row>
+    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>42964.457928240743</v>
+      </c>
+      <c r="B221" t="s">
+        <v>19</v>
+      </c>
+      <c r="C221">
+        <v>1</v>
+      </c>
+      <c r="D221">
+        <v>10000</v>
+      </c>
+      <c r="E221">
+        <v>1</v>
+      </c>
+      <c r="F221">
+        <v>31.701007680721592</v>
+      </c>
+      <c r="G221">
+        <v>0</v>
+      </c>
+      <c r="H221">
+        <v>0.3</v>
+      </c>
+      <c r="I221">
+        <v>0.1</v>
+      </c>
+      <c r="J221">
+        <v>4</v>
+      </c>
+      <c r="K221">
+        <v>4</v>
+      </c>
+      <c r="L221">
+        <v>2</v>
+      </c>
+      <c r="M221">
+        <v>0.36</v>
+      </c>
+      <c r="N221">
+        <v>1.5</v>
+      </c>
+      <c r="O221">
+        <v>0.46</v>
+      </c>
+      <c r="P221">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A222" s="1">
+        <v>42964.458611111113</v>
+      </c>
+      <c r="B222" t="s">
+        <v>19</v>
+      </c>
+      <c r="C222">
+        <v>1</v>
+      </c>
+      <c r="D222">
+        <v>10000</v>
+      </c>
+      <c r="E222">
+        <v>1</v>
+      </c>
+      <c r="F222">
+        <v>17.358420554625983</v>
+      </c>
+      <c r="G222">
+        <v>0</v>
+      </c>
+      <c r="H222">
+        <v>0.3</v>
+      </c>
+      <c r="I222">
+        <v>0.1</v>
+      </c>
+      <c r="J222">
+        <v>4</v>
+      </c>
+      <c r="K222">
+        <v>4</v>
+      </c>
+      <c r="L222">
+        <v>2</v>
+      </c>
+      <c r="M222">
+        <v>0.36</v>
+      </c>
+      <c r="N222">
+        <v>1.5</v>
+      </c>
+      <c r="O222">
+        <v>0.46</v>
+      </c>
+      <c r="P222">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
+    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>42964.460914351854</v>
+      </c>
+      <c r="B223" t="s">
+        <v>19</v>
+      </c>
+      <c r="C223">
+        <v>1</v>
+      </c>
+      <c r="D223">
+        <v>10000</v>
+      </c>
+      <c r="E223">
+        <v>1</v>
+      </c>
+      <c r="F223">
+        <v>109.01754249548094</v>
+      </c>
+      <c r="G223">
+        <v>0</v>
+      </c>
+      <c r="H223">
+        <v>0.3</v>
+      </c>
+      <c r="I223">
+        <v>0.1</v>
+      </c>
+      <c r="J223">
+        <v>4</v>
+      </c>
+      <c r="K223">
+        <v>4</v>
+      </c>
+      <c r="L223">
+        <v>2</v>
+      </c>
+      <c r="M223">
+        <v>0.36</v>
+      </c>
+      <c r="N223">
+        <v>1.5</v>
+      </c>
+      <c r="O223">
+        <v>0.46</v>
+      </c>
+      <c r="P223">
+        <v>4.8444000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimization and psw2 updates, and Dormand-Prince minutia
Main program: A few changes to more easily turn stats for the stress plots on and off.  Put Dormand-Prince on hold fro now.  Add title option to 4-panel stress plot.  Change getPropTest to use switch/case instead of if/elseif and update with new options for 3% and 10% bleaching targets.   Optimize_psw2.mat now has the new values.  The ones we were using recently (20-27) are still in place with the same indexes, but the new values are now in slots 2-17.  OptimizePropCalc now verifies that the RCP specified matches the model runs and the SST loading.  Stats_Tables no longer needs to be edited when changing the table columns for plotting or optimization.  It's all controlled by arguments detailStats and optimizerMode.   tryDormandPrince now has the simple code to allow setting the accuracy level.
</commit_message>
<xml_diff>
--- a/RunSummaries.xlsx
+++ b/RunSummaries.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -455,10 +455,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P223"/>
+  <dimension ref="A1:P309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="A223" sqref="A223:P223"/>
+    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
+      <selection activeCell="A309" sqref="A309:P309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11613,6 +11613,4306 @@
         <v>4.8444000000000003</v>
       </c>
     </row>
+    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A224" s="1">
+        <v>42965.394548611112</v>
+      </c>
+      <c r="B224" t="s">
+        <v>18</v>
+      </c>
+      <c r="C224">
+        <v>0</v>
+      </c>
+      <c r="D224">
+        <v>1</v>
+      </c>
+      <c r="E224">
+        <v>6</v>
+      </c>
+      <c r="F224">
+        <v>16.581075844520381</v>
+      </c>
+      <c r="G224">
+        <v>9.0489510489510501</v>
+      </c>
+      <c r="H224">
+        <v>0.3</v>
+      </c>
+      <c r="I224">
+        <v>0.1</v>
+      </c>
+      <c r="J224">
+        <v>4</v>
+      </c>
+      <c r="K224">
+        <v>4</v>
+      </c>
+      <c r="L224">
+        <v>2</v>
+      </c>
+      <c r="M224">
+        <v>0.36670000000000003</v>
+      </c>
+      <c r="N224">
+        <v>1.3</v>
+      </c>
+      <c r="O224">
+        <v>0.375</v>
+      </c>
+      <c r="P224">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A225" s="1">
+        <v>42965.394918981481</v>
+      </c>
+      <c r="B225" t="s">
+        <v>17</v>
+      </c>
+      <c r="C225">
+        <v>0</v>
+      </c>
+      <c r="D225">
+        <v>1</v>
+      </c>
+      <c r="E225">
+        <v>6</v>
+      </c>
+      <c r="F225">
+        <v>17.248627811374742</v>
+      </c>
+      <c r="G225">
+        <v>8.965034965034965</v>
+      </c>
+      <c r="H225">
+        <v>0.3</v>
+      </c>
+      <c r="I225">
+        <v>0.1</v>
+      </c>
+      <c r="J225">
+        <v>4</v>
+      </c>
+      <c r="K225">
+        <v>4</v>
+      </c>
+      <c r="L225">
+        <v>2</v>
+      </c>
+      <c r="M225">
+        <v>0.42220000000000002</v>
+      </c>
+      <c r="N225">
+        <v>1.2222</v>
+      </c>
+      <c r="O225">
+        <v>0.4556</v>
+      </c>
+      <c r="P225">
+        <v>5.1111000000000004</v>
+      </c>
+    </row>
+    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A226" s="1">
+        <v>42965.395127314812</v>
+      </c>
+      <c r="B226" t="s">
+        <v>18</v>
+      </c>
+      <c r="C226">
+        <v>1</v>
+      </c>
+      <c r="D226">
+        <v>1</v>
+      </c>
+      <c r="E226">
+        <v>6</v>
+      </c>
+      <c r="F226">
+        <v>16.381399800391474</v>
+      </c>
+      <c r="G226">
+        <v>8.9370629370629366</v>
+      </c>
+      <c r="H226">
+        <v>0.3</v>
+      </c>
+      <c r="I226">
+        <v>0.1</v>
+      </c>
+      <c r="J226">
+        <v>4</v>
+      </c>
+      <c r="K226">
+        <v>4</v>
+      </c>
+      <c r="L226">
+        <v>2</v>
+      </c>
+      <c r="M226">
+        <v>0.36</v>
+      </c>
+      <c r="N226">
+        <v>1.2</v>
+      </c>
+      <c r="O226">
+        <v>0.41670000000000001</v>
+      </c>
+      <c r="P226">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A227" s="1">
+        <v>42965.395335648151</v>
+      </c>
+      <c r="B227" t="s">
+        <v>17</v>
+      </c>
+      <c r="C227">
+        <v>1</v>
+      </c>
+      <c r="D227">
+        <v>1</v>
+      </c>
+      <c r="E227">
+        <v>6</v>
+      </c>
+      <c r="F227">
+        <v>16.339915913548197</v>
+      </c>
+      <c r="G227">
+        <v>9.6203796203796212</v>
+      </c>
+      <c r="H227">
+        <v>0.3</v>
+      </c>
+      <c r="I227">
+        <v>0.1</v>
+      </c>
+      <c r="J227">
+        <v>4</v>
+      </c>
+      <c r="K227">
+        <v>4</v>
+      </c>
+      <c r="L227">
+        <v>2</v>
+      </c>
+      <c r="M227">
+        <v>0.36</v>
+      </c>
+      <c r="N227">
+        <v>1.2222</v>
+      </c>
+      <c r="O227">
+        <v>0.4778</v>
+      </c>
+      <c r="P227">
+        <v>6.3333000000000004</v>
+      </c>
+    </row>
+    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A228" s="1">
+        <v>42965.395543981482</v>
+      </c>
+      <c r="B228" t="s">
+        <v>18</v>
+      </c>
+      <c r="C228">
+        <v>0</v>
+      </c>
+      <c r="D228">
+        <v>1</v>
+      </c>
+      <c r="E228">
+        <v>6</v>
+      </c>
+      <c r="F228">
+        <v>16.283409229158462</v>
+      </c>
+      <c r="G228">
+        <v>9.044955044955044</v>
+      </c>
+      <c r="H228">
+        <v>0.3</v>
+      </c>
+      <c r="I228">
+        <v>0.1</v>
+      </c>
+      <c r="J228">
+        <v>4</v>
+      </c>
+      <c r="K228">
+        <v>4</v>
+      </c>
+      <c r="L228">
+        <v>2</v>
+      </c>
+      <c r="M228">
+        <v>0.36670000000000003</v>
+      </c>
+      <c r="N228">
+        <v>1.3</v>
+      </c>
+      <c r="O228">
+        <v>0.375</v>
+      </c>
+      <c r="P228">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A229" s="1">
+        <v>42965.395752314813</v>
+      </c>
+      <c r="B229" t="s">
+        <v>17</v>
+      </c>
+      <c r="C229">
+        <v>0</v>
+      </c>
+      <c r="D229">
+        <v>1</v>
+      </c>
+      <c r="E229">
+        <v>6</v>
+      </c>
+      <c r="F229">
+        <v>16.711085056975467</v>
+      </c>
+      <c r="G229">
+        <v>8.965034965034965</v>
+      </c>
+      <c r="H229">
+        <v>0.3</v>
+      </c>
+      <c r="I229">
+        <v>0.1</v>
+      </c>
+      <c r="J229">
+        <v>4</v>
+      </c>
+      <c r="K229">
+        <v>4</v>
+      </c>
+      <c r="L229">
+        <v>2</v>
+      </c>
+      <c r="M229">
+        <v>0.42220000000000002</v>
+      </c>
+      <c r="N229">
+        <v>1.2222</v>
+      </c>
+      <c r="O229">
+        <v>0.4556</v>
+      </c>
+      <c r="P229">
+        <v>5.1111000000000004</v>
+      </c>
+    </row>
+    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A230" s="1">
+        <v>42965.395960648151</v>
+      </c>
+      <c r="B230" t="s">
+        <v>18</v>
+      </c>
+      <c r="C230">
+        <v>1</v>
+      </c>
+      <c r="D230">
+        <v>1</v>
+      </c>
+      <c r="E230">
+        <v>6</v>
+      </c>
+      <c r="F230">
+        <v>16.460291566683743</v>
+      </c>
+      <c r="G230">
+        <v>8.9370629370629366</v>
+      </c>
+      <c r="H230">
+        <v>0.3</v>
+      </c>
+      <c r="I230">
+        <v>0.1</v>
+      </c>
+      <c r="J230">
+        <v>4</v>
+      </c>
+      <c r="K230">
+        <v>4</v>
+      </c>
+      <c r="L230">
+        <v>2</v>
+      </c>
+      <c r="M230">
+        <v>0.36</v>
+      </c>
+      <c r="N230">
+        <v>1.2</v>
+      </c>
+      <c r="O230">
+        <v>0.41670000000000001</v>
+      </c>
+      <c r="P230">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A231" s="1">
+        <v>42965.396168981482</v>
+      </c>
+      <c r="B231" t="s">
+        <v>17</v>
+      </c>
+      <c r="C231">
+        <v>1</v>
+      </c>
+      <c r="D231">
+        <v>1</v>
+      </c>
+      <c r="E231">
+        <v>6</v>
+      </c>
+      <c r="F231">
+        <v>16.612273396484035</v>
+      </c>
+      <c r="G231">
+        <v>9.594405594405595</v>
+      </c>
+      <c r="H231">
+        <v>0.3</v>
+      </c>
+      <c r="I231">
+        <v>0.1</v>
+      </c>
+      <c r="J231">
+        <v>4</v>
+      </c>
+      <c r="K231">
+        <v>4</v>
+      </c>
+      <c r="L231">
+        <v>2</v>
+      </c>
+      <c r="M231">
+        <v>0.36</v>
+      </c>
+      <c r="N231">
+        <v>1.2222</v>
+      </c>
+      <c r="O231">
+        <v>0.4778</v>
+      </c>
+      <c r="P231">
+        <v>6.3333000000000004</v>
+      </c>
+    </row>
+    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A232" s="1">
+        <v>42965.471886574072</v>
+      </c>
+      <c r="B232" t="s">
+        <v>19</v>
+      </c>
+      <c r="C232">
+        <v>1</v>
+      </c>
+      <c r="D232">
+        <v>5</v>
+      </c>
+      <c r="E232">
+        <v>6</v>
+      </c>
+      <c r="F232">
+        <v>7.7281183392493782</v>
+      </c>
+      <c r="G232">
+        <v>9.5404595404595405</v>
+      </c>
+      <c r="H232">
+        <v>0.3</v>
+      </c>
+      <c r="I232">
+        <v>0.1</v>
+      </c>
+      <c r="J232">
+        <v>4</v>
+      </c>
+      <c r="K232">
+        <v>4</v>
+      </c>
+      <c r="L232">
+        <v>2</v>
+      </c>
+      <c r="M232">
+        <v>0.36</v>
+      </c>
+      <c r="N232">
+        <v>1.2</v>
+      </c>
+      <c r="O232">
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="P232">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A233" s="1">
+        <v>42965.489050925928</v>
+      </c>
+      <c r="B233" t="s">
+        <v>19</v>
+      </c>
+      <c r="C233">
+        <v>1</v>
+      </c>
+      <c r="D233">
+        <v>5</v>
+      </c>
+      <c r="E233">
+        <v>6</v>
+      </c>
+      <c r="F233">
+        <v>7.8454093078755127</v>
+      </c>
+      <c r="G233">
+        <v>10</v>
+      </c>
+      <c r="H233">
+        <v>0.3</v>
+      </c>
+      <c r="I233">
+        <v>0.1</v>
+      </c>
+      <c r="J233">
+        <v>4</v>
+      </c>
+      <c r="K233">
+        <v>4</v>
+      </c>
+      <c r="L233">
+        <v>2</v>
+      </c>
+      <c r="M233">
+        <v>0.36</v>
+      </c>
+      <c r="N233">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="O233">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="P233">
+        <v>4.3888888888888893</v>
+      </c>
+    </row>
+    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A234" s="1">
+        <v>42965.528611111113</v>
+      </c>
+      <c r="B234" t="s">
+        <v>19</v>
+      </c>
+      <c r="C234">
+        <v>1</v>
+      </c>
+      <c r="D234">
+        <v>1</v>
+      </c>
+      <c r="E234">
+        <v>6</v>
+      </c>
+      <c r="F234">
+        <v>16.30352975584594</v>
+      </c>
+      <c r="G234">
+        <v>10.005994005994005</v>
+      </c>
+      <c r="H234">
+        <v>0.3</v>
+      </c>
+      <c r="I234">
+        <v>0.1</v>
+      </c>
+      <c r="J234">
+        <v>4</v>
+      </c>
+      <c r="K234">
+        <v>4</v>
+      </c>
+      <c r="L234">
+        <v>2</v>
+      </c>
+      <c r="M234">
+        <v>0.36</v>
+      </c>
+      <c r="N234">
+        <v>1.25</v>
+      </c>
+      <c r="O234">
+        <v>0.35833333333333334</v>
+      </c>
+      <c r="P234">
+        <v>4.4444444444444446</v>
+      </c>
+    </row>
+    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A235" s="1">
+        <v>42965.541388888887</v>
+      </c>
+      <c r="B235" t="s">
+        <v>19</v>
+      </c>
+      <c r="C235">
+        <v>0</v>
+      </c>
+      <c r="D235">
+        <v>5</v>
+      </c>
+      <c r="E235">
+        <v>6</v>
+      </c>
+      <c r="F235">
+        <v>7.7390702492098695</v>
+      </c>
+      <c r="G235">
+        <v>10.109890109890109</v>
+      </c>
+      <c r="H235">
+        <v>0.3</v>
+      </c>
+      <c r="I235">
+        <v>0.1</v>
+      </c>
+      <c r="J235">
+        <v>4</v>
+      </c>
+      <c r="K235">
+        <v>4</v>
+      </c>
+      <c r="L235">
+        <v>2</v>
+      </c>
+      <c r="M235">
+        <v>0.36</v>
+      </c>
+      <c r="N235">
+        <v>1.4</v>
+      </c>
+      <c r="O235">
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="P235">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A236" s="1">
+        <v>42965.551192129627</v>
+      </c>
+      <c r="B236" t="s">
+        <v>19</v>
+      </c>
+      <c r="C236">
+        <v>0</v>
+      </c>
+      <c r="D236">
+        <v>5</v>
+      </c>
+      <c r="E236">
+        <v>6</v>
+      </c>
+      <c r="F236">
+        <v>5.6406940924131801</v>
+      </c>
+      <c r="G236">
+        <v>10.01998001998002</v>
+      </c>
+      <c r="H236">
+        <v>0.3</v>
+      </c>
+      <c r="I236">
+        <v>0.1</v>
+      </c>
+      <c r="J236">
+        <v>4</v>
+      </c>
+      <c r="K236">
+        <v>4</v>
+      </c>
+      <c r="L236">
+        <v>2</v>
+      </c>
+      <c r="M236">
+        <v>0.36</v>
+      </c>
+      <c r="N236">
+        <v>1.5</v>
+      </c>
+      <c r="O236">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="P236">
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A237" s="1">
+        <v>42965.579201388886</v>
+      </c>
+      <c r="B237" t="s">
+        <v>19</v>
+      </c>
+      <c r="C237">
+        <v>0</v>
+      </c>
+      <c r="D237">
+        <v>1</v>
+      </c>
+      <c r="E237">
+        <v>6</v>
+      </c>
+      <c r="F237">
+        <v>21.442338638841363</v>
+      </c>
+      <c r="G237">
+        <v>9.9820179820179824</v>
+      </c>
+      <c r="H237">
+        <v>0.3</v>
+      </c>
+      <c r="I237">
+        <v>0.1</v>
+      </c>
+      <c r="J237">
+        <v>4</v>
+      </c>
+      <c r="K237">
+        <v>4</v>
+      </c>
+      <c r="L237">
+        <v>2</v>
+      </c>
+      <c r="M237">
+        <v>0.36</v>
+      </c>
+      <c r="N237">
+        <v>1.4</v>
+      </c>
+      <c r="O237">
+        <v>0.34166666666666667</v>
+      </c>
+      <c r="P237">
+        <v>3.8333333333333335</v>
+      </c>
+    </row>
+    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A238" s="1">
+        <v>42965.590057870373</v>
+      </c>
+      <c r="B238" t="s">
+        <v>19</v>
+      </c>
+      <c r="C238">
+        <v>0</v>
+      </c>
+      <c r="D238">
+        <v>1</v>
+      </c>
+      <c r="E238">
+        <v>6</v>
+      </c>
+      <c r="F238">
+        <v>22.229905312345107</v>
+      </c>
+      <c r="G238">
+        <v>9.9700299700299695</v>
+      </c>
+      <c r="H238">
+        <v>0.3</v>
+      </c>
+      <c r="I238">
+        <v>0.1</v>
+      </c>
+      <c r="J238">
+        <v>4</v>
+      </c>
+      <c r="K238">
+        <v>4</v>
+      </c>
+      <c r="L238">
+        <v>2</v>
+      </c>
+      <c r="M238">
+        <v>0.36</v>
+      </c>
+      <c r="N238">
+        <v>1.35</v>
+      </c>
+      <c r="O238">
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="P238">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A239" s="1">
+        <v>42965.608148148145</v>
+      </c>
+      <c r="B239" t="s">
+        <v>19</v>
+      </c>
+      <c r="C239">
+        <v>0</v>
+      </c>
+      <c r="D239">
+        <v>1</v>
+      </c>
+      <c r="E239">
+        <v>5</v>
+      </c>
+      <c r="F239">
+        <v>18.898207331117522</v>
+      </c>
+      <c r="G239">
+        <v>10.009990009990011</v>
+      </c>
+      <c r="H239">
+        <v>0.3</v>
+      </c>
+      <c r="I239">
+        <v>0.1</v>
+      </c>
+      <c r="J239">
+        <v>4</v>
+      </c>
+      <c r="K239">
+        <v>4</v>
+      </c>
+      <c r="L239">
+        <v>2</v>
+      </c>
+      <c r="M239">
+        <v>0.36</v>
+      </c>
+      <c r="N239">
+        <v>1.3055555555555556</v>
+      </c>
+      <c r="O239">
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="P239">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A240" s="1">
+        <v>42965.619409722225</v>
+      </c>
+      <c r="B240" t="s">
+        <v>18</v>
+      </c>
+      <c r="C240">
+        <v>1</v>
+      </c>
+      <c r="D240">
+        <v>5</v>
+      </c>
+      <c r="E240">
+        <v>5</v>
+      </c>
+      <c r="F240">
+        <v>6.6507365964218303</v>
+      </c>
+      <c r="G240">
+        <v>9.8301698301698295</v>
+      </c>
+      <c r="H240">
+        <v>0.3</v>
+      </c>
+      <c r="I240">
+        <v>0.1</v>
+      </c>
+      <c r="J240">
+        <v>4</v>
+      </c>
+      <c r="K240">
+        <v>4</v>
+      </c>
+      <c r="L240">
+        <v>2</v>
+      </c>
+      <c r="M240">
+        <v>0.36</v>
+      </c>
+      <c r="N240">
+        <v>1.2</v>
+      </c>
+      <c r="O240">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="P240">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
+        <v>42965.640231481484</v>
+      </c>
+      <c r="B241" t="s">
+        <v>18</v>
+      </c>
+      <c r="C241">
+        <v>1</v>
+      </c>
+      <c r="D241">
+        <v>5</v>
+      </c>
+      <c r="E241">
+        <v>5</v>
+      </c>
+      <c r="F241">
+        <v>5.845965127065643</v>
+      </c>
+      <c r="G241">
+        <v>10.04995004995005</v>
+      </c>
+      <c r="H241">
+        <v>0.3</v>
+      </c>
+      <c r="I241">
+        <v>0.1</v>
+      </c>
+      <c r="J241">
+        <v>4</v>
+      </c>
+      <c r="K241">
+        <v>4</v>
+      </c>
+      <c r="L241">
+        <v>2</v>
+      </c>
+      <c r="M241">
+        <v>0.36</v>
+      </c>
+      <c r="N241">
+        <v>1.35</v>
+      </c>
+      <c r="O241">
+        <v>0.35833333333333334</v>
+      </c>
+      <c r="P241">
+        <v>4.4444444444444446</v>
+      </c>
+    </row>
+    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
+        <v>42965.700231481482</v>
+      </c>
+      <c r="B242" t="s">
+        <v>18</v>
+      </c>
+      <c r="C242">
+        <v>1</v>
+      </c>
+      <c r="D242">
+        <v>1</v>
+      </c>
+      <c r="E242">
+        <v>5</v>
+      </c>
+      <c r="F242">
+        <v>19.824858397301604</v>
+      </c>
+      <c r="G242">
+        <v>9.9940059940059953</v>
+      </c>
+      <c r="H242">
+        <v>0.3</v>
+      </c>
+      <c r="I242">
+        <v>0.1</v>
+      </c>
+      <c r="J242">
+        <v>4</v>
+      </c>
+      <c r="K242">
+        <v>4</v>
+      </c>
+      <c r="L242">
+        <v>2</v>
+      </c>
+      <c r="M242">
+        <v>0.36</v>
+      </c>
+      <c r="N242">
+        <v>1.3555555555555556</v>
+      </c>
+      <c r="O242">
+        <v>0.38133333333333336</v>
+      </c>
+      <c r="P242">
+        <v>4.7407499999999994</v>
+      </c>
+    </row>
+    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
+        <v>42965.70689814815</v>
+      </c>
+      <c r="B243" t="s">
+        <v>17</v>
+      </c>
+      <c r="C243">
+        <v>0</v>
+      </c>
+      <c r="D243">
+        <v>5</v>
+      </c>
+      <c r="E243">
+        <v>5</v>
+      </c>
+      <c r="F243">
+        <v>5.8894489390317224</v>
+      </c>
+      <c r="G243">
+        <v>12.427572427572427</v>
+      </c>
+      <c r="H243">
+        <v>0.3</v>
+      </c>
+      <c r="I243">
+        <v>0.1</v>
+      </c>
+      <c r="J243">
+        <v>4</v>
+      </c>
+      <c r="K243">
+        <v>4</v>
+      </c>
+      <c r="L243">
+        <v>2</v>
+      </c>
+      <c r="M243">
+        <v>0.36</v>
+      </c>
+      <c r="N243">
+        <v>1.3</v>
+      </c>
+      <c r="O243">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="P243">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A244" s="1">
+        <v>42965.709340277775</v>
+      </c>
+      <c r="B244" t="s">
+        <v>17</v>
+      </c>
+      <c r="C244">
+        <v>0</v>
+      </c>
+      <c r="D244">
+        <v>5</v>
+      </c>
+      <c r="E244">
+        <v>5</v>
+      </c>
+      <c r="F244">
+        <v>5.8334535954973843</v>
+      </c>
+      <c r="G244">
+        <v>10</v>
+      </c>
+      <c r="H244">
+        <v>0.3</v>
+      </c>
+      <c r="I244">
+        <v>0.1</v>
+      </c>
+      <c r="J244">
+        <v>4</v>
+      </c>
+      <c r="K244">
+        <v>4</v>
+      </c>
+      <c r="L244">
+        <v>2</v>
+      </c>
+      <c r="M244">
+        <v>0.36</v>
+      </c>
+      <c r="N244">
+        <v>1.25</v>
+      </c>
+      <c r="O244">
+        <v>0.4</v>
+      </c>
+      <c r="P244">
+        <v>4.5555555555555554</v>
+      </c>
+    </row>
+    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A245" s="1">
+        <v>42965.71266203704</v>
+      </c>
+      <c r="B245" t="s">
+        <v>17</v>
+      </c>
+      <c r="C245">
+        <v>0</v>
+      </c>
+      <c r="D245">
+        <v>1</v>
+      </c>
+      <c r="E245">
+        <v>5</v>
+      </c>
+      <c r="F245">
+        <v>17.772770107487176</v>
+      </c>
+      <c r="G245">
+        <v>10.063936063936065</v>
+      </c>
+      <c r="H245">
+        <v>0.3</v>
+      </c>
+      <c r="I245">
+        <v>0.1</v>
+      </c>
+      <c r="J245">
+        <v>4</v>
+      </c>
+      <c r="K245">
+        <v>4</v>
+      </c>
+      <c r="L245">
+        <v>2</v>
+      </c>
+      <c r="M245">
+        <v>0.36</v>
+      </c>
+      <c r="N245">
+        <v>1.25</v>
+      </c>
+      <c r="O245">
+        <v>0.4</v>
+      </c>
+      <c r="P245">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
+        <v>42965.715567129628</v>
+      </c>
+      <c r="B246" t="s">
+        <v>17</v>
+      </c>
+      <c r="C246">
+        <v>0</v>
+      </c>
+      <c r="D246">
+        <v>1</v>
+      </c>
+      <c r="E246">
+        <v>5</v>
+      </c>
+      <c r="F246">
+        <v>17.714467330343151</v>
+      </c>
+      <c r="G246">
+        <v>10.005994005994005</v>
+      </c>
+      <c r="H246">
+        <v>0.3</v>
+      </c>
+      <c r="I246">
+        <v>0.1</v>
+      </c>
+      <c r="J246">
+        <v>4</v>
+      </c>
+      <c r="K246">
+        <v>4</v>
+      </c>
+      <c r="L246">
+        <v>2</v>
+      </c>
+      <c r="M246">
+        <v>0.36</v>
+      </c>
+      <c r="N246">
+        <v>1.25</v>
+      </c>
+      <c r="O246">
+        <v>0.4</v>
+      </c>
+      <c r="P246">
+        <v>4.5388888888888888</v>
+      </c>
+    </row>
+    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A247" s="1">
+        <v>42965.737812500003</v>
+      </c>
+      <c r="B247" t="s">
+        <v>18</v>
+      </c>
+      <c r="C247">
+        <v>0</v>
+      </c>
+      <c r="D247">
+        <v>5</v>
+      </c>
+      <c r="E247">
+        <v>5</v>
+      </c>
+      <c r="F247">
+        <v>5.9281111715177381</v>
+      </c>
+      <c r="G247">
+        <v>9.4805194805194795</v>
+      </c>
+      <c r="H247">
+        <v>0.3</v>
+      </c>
+      <c r="I247">
+        <v>0.1</v>
+      </c>
+      <c r="J247">
+        <v>4</v>
+      </c>
+      <c r="K247">
+        <v>4</v>
+      </c>
+      <c r="L247">
+        <v>2</v>
+      </c>
+      <c r="M247">
+        <v>0.36</v>
+      </c>
+      <c r="N247">
+        <v>1.5</v>
+      </c>
+      <c r="O247">
+        <v>0.46</v>
+      </c>
+      <c r="P247">
+        <v>5.6666666666666661</v>
+      </c>
+    </row>
+    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>42965.739872685182</v>
+      </c>
+      <c r="B248" t="s">
+        <v>18</v>
+      </c>
+      <c r="C248">
+        <v>0</v>
+      </c>
+      <c r="D248">
+        <v>5</v>
+      </c>
+      <c r="E248">
+        <v>5</v>
+      </c>
+      <c r="F248">
+        <v>7.2931410248000317</v>
+      </c>
+      <c r="G248">
+        <v>10.009990009990011</v>
+      </c>
+      <c r="H248">
+        <v>0.3</v>
+      </c>
+      <c r="I248">
+        <v>0.1</v>
+      </c>
+      <c r="J248">
+        <v>4</v>
+      </c>
+      <c r="K248">
+        <v>4</v>
+      </c>
+      <c r="L248">
+        <v>2</v>
+      </c>
+      <c r="M248">
+        <v>0.36</v>
+      </c>
+      <c r="N248">
+        <v>1.5</v>
+      </c>
+      <c r="O248">
+        <v>0.46</v>
+      </c>
+      <c r="P248">
+        <v>5.7777777777777777</v>
+      </c>
+    </row>
+    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A249" s="1">
+        <v>42965.742650462962</v>
+      </c>
+      <c r="B249" t="s">
+        <v>18</v>
+      </c>
+      <c r="C249">
+        <v>0</v>
+      </c>
+      <c r="D249">
+        <v>1</v>
+      </c>
+      <c r="E249">
+        <v>5</v>
+      </c>
+      <c r="F249">
+        <v>24.631383401005465</v>
+      </c>
+      <c r="G249">
+        <v>10.04995004995005</v>
+      </c>
+      <c r="H249">
+        <v>0.3</v>
+      </c>
+      <c r="I249">
+        <v>0.1</v>
+      </c>
+      <c r="J249">
+        <v>4</v>
+      </c>
+      <c r="K249">
+        <v>4</v>
+      </c>
+      <c r="L249">
+        <v>2</v>
+      </c>
+      <c r="M249">
+        <v>0.36</v>
+      </c>
+      <c r="N249">
+        <v>1.5</v>
+      </c>
+      <c r="O249">
+        <v>0.46</v>
+      </c>
+      <c r="P249">
+        <v>5.6888888888888891</v>
+      </c>
+    </row>
+    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A250" s="1">
+        <v>42965.744004629632</v>
+      </c>
+      <c r="B250" t="s">
+        <v>18</v>
+      </c>
+      <c r="C250">
+        <v>1</v>
+      </c>
+      <c r="D250">
+        <v>5</v>
+      </c>
+      <c r="E250">
+        <v>5</v>
+      </c>
+      <c r="F250">
+        <v>5.9754073207499108</v>
+      </c>
+      <c r="G250">
+        <v>8.8411588411588404</v>
+      </c>
+      <c r="H250">
+        <v>0.3</v>
+      </c>
+      <c r="I250">
+        <v>0.1</v>
+      </c>
+      <c r="J250">
+        <v>4</v>
+      </c>
+      <c r="K250">
+        <v>4</v>
+      </c>
+      <c r="L250">
+        <v>2</v>
+      </c>
+      <c r="M250">
+        <v>0.36</v>
+      </c>
+      <c r="N250">
+        <v>1.5</v>
+      </c>
+      <c r="O250">
+        <v>0.46</v>
+      </c>
+      <c r="P250">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A251" s="1">
+        <v>42965.74596064815</v>
+      </c>
+      <c r="B251" t="s">
+        <v>18</v>
+      </c>
+      <c r="C251">
+        <v>1</v>
+      </c>
+      <c r="D251">
+        <v>5</v>
+      </c>
+      <c r="E251">
+        <v>5</v>
+      </c>
+      <c r="F251">
+        <v>5.9679407202994321</v>
+      </c>
+      <c r="G251">
+        <v>10</v>
+      </c>
+      <c r="H251">
+        <v>0.3</v>
+      </c>
+      <c r="I251">
+        <v>0.1</v>
+      </c>
+      <c r="J251">
+        <v>4</v>
+      </c>
+      <c r="K251">
+        <v>4</v>
+      </c>
+      <c r="L251">
+        <v>2</v>
+      </c>
+      <c r="M251">
+        <v>0.36</v>
+      </c>
+      <c r="N251">
+        <v>1.5</v>
+      </c>
+      <c r="O251">
+        <v>0.46</v>
+      </c>
+      <c r="P251">
+        <v>6.333333333333333</v>
+      </c>
+    </row>
+    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A252" s="1">
+        <v>42965.749421296299</v>
+      </c>
+      <c r="B252" t="s">
+        <v>18</v>
+      </c>
+      <c r="C252">
+        <v>1</v>
+      </c>
+      <c r="D252">
+        <v>1</v>
+      </c>
+      <c r="E252">
+        <v>5</v>
+      </c>
+      <c r="F252">
+        <v>21.223786501433388</v>
+      </c>
+      <c r="G252">
+        <v>10.057942057942057</v>
+      </c>
+      <c r="H252">
+        <v>0.3</v>
+      </c>
+      <c r="I252">
+        <v>0.1</v>
+      </c>
+      <c r="J252">
+        <v>4</v>
+      </c>
+      <c r="K252">
+        <v>4</v>
+      </c>
+      <c r="L252">
+        <v>2</v>
+      </c>
+      <c r="M252">
+        <v>0.36</v>
+      </c>
+      <c r="N252">
+        <v>1.5</v>
+      </c>
+      <c r="O252">
+        <v>0.46</v>
+      </c>
+      <c r="P252">
+        <v>6.2592722222222221</v>
+      </c>
+    </row>
+    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A253" s="1">
+        <v>42965.751793981479</v>
+      </c>
+      <c r="B253" t="s">
+        <v>19</v>
+      </c>
+      <c r="C253">
+        <v>0</v>
+      </c>
+      <c r="D253">
+        <v>5</v>
+      </c>
+      <c r="E253">
+        <v>5</v>
+      </c>
+      <c r="F253">
+        <v>5.9606609928524277</v>
+      </c>
+      <c r="G253">
+        <v>9.8401598401598402</v>
+      </c>
+      <c r="H253">
+        <v>0.3</v>
+      </c>
+      <c r="I253">
+        <v>0.1</v>
+      </c>
+      <c r="J253">
+        <v>4</v>
+      </c>
+      <c r="K253">
+        <v>4</v>
+      </c>
+      <c r="L253">
+        <v>2</v>
+      </c>
+      <c r="M253">
+        <v>0.36</v>
+      </c>
+      <c r="N253">
+        <v>1.5</v>
+      </c>
+      <c r="O253">
+        <v>0.46</v>
+      </c>
+      <c r="P253">
+        <v>5.7777777777777777</v>
+      </c>
+    </row>
+    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A254" s="1">
+        <v>42965.784918981481</v>
+      </c>
+      <c r="B254" t="s">
+        <v>19</v>
+      </c>
+      <c r="C254">
+        <v>0</v>
+      </c>
+      <c r="D254">
+        <v>1</v>
+      </c>
+      <c r="E254">
+        <v>5</v>
+      </c>
+      <c r="F254">
+        <v>24.141487182719878</v>
+      </c>
+      <c r="G254">
+        <v>10.039960039960039</v>
+      </c>
+      <c r="H254">
+        <v>0.3</v>
+      </c>
+      <c r="I254">
+        <v>0.1</v>
+      </c>
+      <c r="J254">
+        <v>4</v>
+      </c>
+      <c r="K254">
+        <v>4</v>
+      </c>
+      <c r="L254">
+        <v>2</v>
+      </c>
+      <c r="M254">
+        <v>0.36</v>
+      </c>
+      <c r="N254">
+        <v>1.5</v>
+      </c>
+      <c r="O254">
+        <v>0.46</v>
+      </c>
+      <c r="P254">
+        <v>5.7444666666666668</v>
+      </c>
+    </row>
+    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
+        <v>42965.798541666663</v>
+      </c>
+      <c r="B255" t="s">
+        <v>19</v>
+      </c>
+      <c r="C255">
+        <v>1</v>
+      </c>
+      <c r="D255">
+        <v>5</v>
+      </c>
+      <c r="E255">
+        <v>5</v>
+      </c>
+      <c r="F255">
+        <v>5.7881432919151505</v>
+      </c>
+      <c r="G255">
+        <v>8.6513486513486519</v>
+      </c>
+      <c r="H255">
+        <v>0.3</v>
+      </c>
+      <c r="I255">
+        <v>0.1</v>
+      </c>
+      <c r="J255">
+        <v>4</v>
+      </c>
+      <c r="K255">
+        <v>4</v>
+      </c>
+      <c r="L255">
+        <v>2</v>
+      </c>
+      <c r="M255">
+        <v>0.36</v>
+      </c>
+      <c r="N255">
+        <v>1.5</v>
+      </c>
+      <c r="O255">
+        <v>0.46</v>
+      </c>
+      <c r="P255">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A256" s="1">
+        <v>42965.800729166665</v>
+      </c>
+      <c r="B256" t="s">
+        <v>19</v>
+      </c>
+      <c r="C256">
+        <v>1</v>
+      </c>
+      <c r="D256">
+        <v>5</v>
+      </c>
+      <c r="E256">
+        <v>5</v>
+      </c>
+      <c r="F256">
+        <v>5.6982180187173794</v>
+      </c>
+      <c r="G256">
+        <v>9.870129870129869</v>
+      </c>
+      <c r="H256">
+        <v>0.3</v>
+      </c>
+      <c r="I256">
+        <v>0.1</v>
+      </c>
+      <c r="J256">
+        <v>4</v>
+      </c>
+      <c r="K256">
+        <v>4</v>
+      </c>
+      <c r="L256">
+        <v>2</v>
+      </c>
+      <c r="M256">
+        <v>0.36</v>
+      </c>
+      <c r="N256">
+        <v>1.5</v>
+      </c>
+      <c r="O256">
+        <v>0.46</v>
+      </c>
+      <c r="P256">
+        <v>6.333333333333333</v>
+      </c>
+    </row>
+    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A257" s="1">
+        <v>42965.803854166668</v>
+      </c>
+      <c r="B257" t="s">
+        <v>19</v>
+      </c>
+      <c r="C257">
+        <v>1</v>
+      </c>
+      <c r="D257">
+        <v>1</v>
+      </c>
+      <c r="E257">
+        <v>5</v>
+      </c>
+      <c r="F257">
+        <v>17.818703107755645</v>
+      </c>
+      <c r="G257">
+        <v>10.053946053946053</v>
+      </c>
+      <c r="H257">
+        <v>0.3</v>
+      </c>
+      <c r="I257">
+        <v>0.1</v>
+      </c>
+      <c r="J257">
+        <v>4</v>
+      </c>
+      <c r="K257">
+        <v>4</v>
+      </c>
+      <c r="L257">
+        <v>2</v>
+      </c>
+      <c r="M257">
+        <v>0.36</v>
+      </c>
+      <c r="N257">
+        <v>1.5</v>
+      </c>
+      <c r="O257">
+        <v>0.46</v>
+      </c>
+      <c r="P257">
+        <v>6.3332999999999995</v>
+      </c>
+    </row>
+    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A258" s="1">
+        <v>42965.818391203706</v>
+      </c>
+      <c r="B258" t="s">
+        <v>17</v>
+      </c>
+      <c r="C258">
+        <v>0</v>
+      </c>
+      <c r="D258">
+        <v>5</v>
+      </c>
+      <c r="E258">
+        <v>5</v>
+      </c>
+      <c r="F258">
+        <v>7.1812940123521773</v>
+      </c>
+      <c r="G258">
+        <v>5.0249750249750251</v>
+      </c>
+      <c r="H258">
+        <v>0.3</v>
+      </c>
+      <c r="I258">
+        <v>0.1</v>
+      </c>
+      <c r="J258">
+        <v>4</v>
+      </c>
+      <c r="K258">
+        <v>4</v>
+      </c>
+      <c r="L258">
+        <v>2</v>
+      </c>
+      <c r="M258">
+        <v>0.36</v>
+      </c>
+      <c r="N258">
+        <v>1.5</v>
+      </c>
+      <c r="O258">
+        <v>0.46</v>
+      </c>
+      <c r="P258">
+        <v>4.333333333333333</v>
+      </c>
+    </row>
+    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A259" s="1">
+        <v>42965.820219907408</v>
+      </c>
+      <c r="B259" t="s">
+        <v>17</v>
+      </c>
+      <c r="C259">
+        <v>0</v>
+      </c>
+      <c r="D259">
+        <v>5</v>
+      </c>
+      <c r="E259">
+        <v>5</v>
+      </c>
+      <c r="F259">
+        <v>5.5983574374975404</v>
+      </c>
+      <c r="G259">
+        <v>5.0249750249750251</v>
+      </c>
+      <c r="H259">
+        <v>0.3</v>
+      </c>
+      <c r="I259">
+        <v>0.1</v>
+      </c>
+      <c r="J259">
+        <v>4</v>
+      </c>
+      <c r="K259">
+        <v>4</v>
+      </c>
+      <c r="L259">
+        <v>2</v>
+      </c>
+      <c r="M259">
+        <v>0.36</v>
+      </c>
+      <c r="N259">
+        <v>1.5</v>
+      </c>
+      <c r="O259">
+        <v>0.46</v>
+      </c>
+      <c r="P259">
+        <v>4.3333333333333339</v>
+      </c>
+    </row>
+    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A260" s="1">
+        <v>42965.822928240741</v>
+      </c>
+      <c r="B260" t="s">
+        <v>17</v>
+      </c>
+      <c r="C260">
+        <v>0</v>
+      </c>
+      <c r="D260">
+        <v>5</v>
+      </c>
+      <c r="E260">
+        <v>5</v>
+      </c>
+      <c r="F260">
+        <v>5.7169033991367364</v>
+      </c>
+      <c r="G260">
+        <v>5.0249750249750251</v>
+      </c>
+      <c r="H260">
+        <v>0.3</v>
+      </c>
+      <c r="I260">
+        <v>0.1</v>
+      </c>
+      <c r="J260">
+        <v>4</v>
+      </c>
+      <c r="K260">
+        <v>4</v>
+      </c>
+      <c r="L260">
+        <v>2</v>
+      </c>
+      <c r="M260">
+        <v>0.36</v>
+      </c>
+      <c r="N260">
+        <v>1.5</v>
+      </c>
+      <c r="O260">
+        <v>0.46</v>
+      </c>
+      <c r="P260">
+        <v>4.3333333333333339</v>
+      </c>
+    </row>
+    <row r="261" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A261" s="1">
+        <v>42965.826481481483</v>
+      </c>
+      <c r="B261" t="s">
+        <v>17</v>
+      </c>
+      <c r="C261">
+        <v>0</v>
+      </c>
+      <c r="D261">
+        <v>1</v>
+      </c>
+      <c r="E261">
+        <v>5</v>
+      </c>
+      <c r="F261">
+        <v>17.852430485002643</v>
+      </c>
+      <c r="G261">
+        <v>4.9930069930069925</v>
+      </c>
+      <c r="H261">
+        <v>0.3</v>
+      </c>
+      <c r="I261">
+        <v>0.1</v>
+      </c>
+      <c r="J261">
+        <v>4</v>
+      </c>
+      <c r="K261">
+        <v>4</v>
+      </c>
+      <c r="L261">
+        <v>2</v>
+      </c>
+      <c r="M261">
+        <v>0.36</v>
+      </c>
+      <c r="N261">
+        <v>1.5</v>
+      </c>
+      <c r="O261">
+        <v>0.46</v>
+      </c>
+      <c r="P261">
+        <v>4.2555555555555555</v>
+      </c>
+    </row>
+    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A262" s="1">
+        <v>42965.829583333332</v>
+      </c>
+      <c r="B262" t="s">
+        <v>17</v>
+      </c>
+      <c r="C262">
+        <v>1</v>
+      </c>
+      <c r="D262">
+        <v>5</v>
+      </c>
+      <c r="E262">
+        <v>5</v>
+      </c>
+      <c r="F262">
+        <v>5.64541007584676</v>
+      </c>
+      <c r="G262">
+        <v>5.0549450549450547</v>
+      </c>
+      <c r="H262">
+        <v>0.3</v>
+      </c>
+      <c r="I262">
+        <v>0.1</v>
+      </c>
+      <c r="J262">
+        <v>4</v>
+      </c>
+      <c r="K262">
+        <v>4</v>
+      </c>
+      <c r="L262">
+        <v>2</v>
+      </c>
+      <c r="M262">
+        <v>0.36</v>
+      </c>
+      <c r="N262">
+        <v>1.5</v>
+      </c>
+      <c r="O262">
+        <v>0.46</v>
+      </c>
+      <c r="P262">
+        <v>4.791666666666667</v>
+      </c>
+    </row>
+    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A263" s="1">
+        <v>42965.833194444444</v>
+      </c>
+      <c r="B263" t="s">
+        <v>17</v>
+      </c>
+      <c r="C263">
+        <v>1</v>
+      </c>
+      <c r="D263">
+        <v>1</v>
+      </c>
+      <c r="E263">
+        <v>5</v>
+      </c>
+      <c r="F263">
+        <v>21.372518212918109</v>
+      </c>
+      <c r="G263">
+        <v>5.0269730269730264</v>
+      </c>
+      <c r="H263">
+        <v>0.3</v>
+      </c>
+      <c r="I263">
+        <v>0.1</v>
+      </c>
+      <c r="J263">
+        <v>4</v>
+      </c>
+      <c r="K263">
+        <v>4</v>
+      </c>
+      <c r="L263">
+        <v>2</v>
+      </c>
+      <c r="M263">
+        <v>0.36</v>
+      </c>
+      <c r="N263">
+        <v>1.5</v>
+      </c>
+      <c r="O263">
+        <v>0.46</v>
+      </c>
+      <c r="P263">
+        <v>4.7250333333333332</v>
+      </c>
+    </row>
+    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A264" s="1">
+        <v>42965.839675925927</v>
+      </c>
+      <c r="B264" t="s">
+        <v>16</v>
+      </c>
+      <c r="C264">
+        <v>0</v>
+      </c>
+      <c r="D264">
+        <v>1</v>
+      </c>
+      <c r="E264">
+        <v>5</v>
+      </c>
+      <c r="F264">
+        <v>17.630244883631558</v>
+      </c>
+      <c r="G264">
+        <v>4.9830169830169826</v>
+      </c>
+      <c r="H264">
+        <v>0.3</v>
+      </c>
+      <c r="I264">
+        <v>0.1</v>
+      </c>
+      <c r="J264">
+        <v>4</v>
+      </c>
+      <c r="K264">
+        <v>4</v>
+      </c>
+      <c r="L264">
+        <v>2</v>
+      </c>
+      <c r="M264">
+        <v>0.36</v>
+      </c>
+      <c r="N264">
+        <v>1.5</v>
+      </c>
+      <c r="O264">
+        <v>0.46</v>
+      </c>
+      <c r="P264">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A265" s="1">
+        <v>42965.843055555553</v>
+      </c>
+      <c r="B265" t="s">
+        <v>16</v>
+      </c>
+      <c r="C265">
+        <v>1</v>
+      </c>
+      <c r="D265">
+        <v>1</v>
+      </c>
+      <c r="E265">
+        <v>5</v>
+      </c>
+      <c r="F265">
+        <v>21.380464795398062</v>
+      </c>
+      <c r="G265">
+        <v>5.0249750249750251</v>
+      </c>
+      <c r="H265">
+        <v>0.3</v>
+      </c>
+      <c r="I265">
+        <v>0.1</v>
+      </c>
+      <c r="J265">
+        <v>4</v>
+      </c>
+      <c r="K265">
+        <v>4</v>
+      </c>
+      <c r="L265">
+        <v>2</v>
+      </c>
+      <c r="M265">
+        <v>0.36</v>
+      </c>
+      <c r="N265">
+        <v>1.5</v>
+      </c>
+      <c r="O265">
+        <v>0.46</v>
+      </c>
+      <c r="P265">
+        <v>4.7222222222222223</v>
+      </c>
+    </row>
+    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A266" s="1">
+        <v>42965.852025462962</v>
+      </c>
+      <c r="B266" t="s">
+        <v>17</v>
+      </c>
+      <c r="C266">
+        <v>0</v>
+      </c>
+      <c r="D266">
+        <v>5</v>
+      </c>
+      <c r="E266">
+        <v>5</v>
+      </c>
+      <c r="F266">
+        <v>5.640835527117865</v>
+      </c>
+      <c r="G266">
+        <v>2.5674325674325678</v>
+      </c>
+      <c r="H266">
+        <v>0.3</v>
+      </c>
+      <c r="I266">
+        <v>0.1</v>
+      </c>
+      <c r="J266">
+        <v>4</v>
+      </c>
+      <c r="K266">
+        <v>4</v>
+      </c>
+      <c r="L266">
+        <v>2</v>
+      </c>
+      <c r="M266">
+        <v>0.36</v>
+      </c>
+      <c r="N266">
+        <v>1.5</v>
+      </c>
+      <c r="O266">
+        <v>0.46</v>
+      </c>
+      <c r="P266">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A267" s="1">
+        <v>42965.857743055552</v>
+      </c>
+      <c r="B267" t="s">
+        <v>17</v>
+      </c>
+      <c r="C267">
+        <v>0</v>
+      </c>
+      <c r="D267">
+        <v>5</v>
+      </c>
+      <c r="E267">
+        <v>5</v>
+      </c>
+      <c r="F267">
+        <v>7.4004915655957841</v>
+      </c>
+      <c r="G267">
+        <v>2.5674325674325678</v>
+      </c>
+      <c r="H267">
+        <v>0.3</v>
+      </c>
+      <c r="I267">
+        <v>0.1</v>
+      </c>
+      <c r="J267">
+        <v>4</v>
+      </c>
+      <c r="K267">
+        <v>4</v>
+      </c>
+      <c r="L267">
+        <v>2</v>
+      </c>
+      <c r="M267">
+        <v>0.36</v>
+      </c>
+      <c r="N267">
+        <v>1.5</v>
+      </c>
+      <c r="O267">
+        <v>0.46</v>
+      </c>
+      <c r="P267">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A268" s="1">
+        <v>42965.865405092591</v>
+      </c>
+      <c r="B268" t="s">
+        <v>17</v>
+      </c>
+      <c r="C268">
+        <v>0</v>
+      </c>
+      <c r="D268">
+        <v>1</v>
+      </c>
+      <c r="E268">
+        <v>5</v>
+      </c>
+      <c r="F268">
+        <v>17.662202087153858</v>
+      </c>
+      <c r="G268">
+        <v>2.8231768231768233</v>
+      </c>
+      <c r="H268">
+        <v>0.3</v>
+      </c>
+      <c r="I268">
+        <v>0.1</v>
+      </c>
+      <c r="J268">
+        <v>4</v>
+      </c>
+      <c r="K268">
+        <v>4</v>
+      </c>
+      <c r="L268">
+        <v>2</v>
+      </c>
+      <c r="M268">
+        <v>0.36</v>
+      </c>
+      <c r="N268">
+        <v>1.5</v>
+      </c>
+      <c r="O268">
+        <v>0.46</v>
+      </c>
+      <c r="P268">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A269" s="1">
+        <v>42965.874479166669</v>
+      </c>
+      <c r="B269" t="s">
+        <v>17</v>
+      </c>
+      <c r="C269">
+        <v>0</v>
+      </c>
+      <c r="D269">
+        <v>1</v>
+      </c>
+      <c r="E269">
+        <v>5</v>
+      </c>
+      <c r="F269">
+        <v>22.430454923767655</v>
+      </c>
+      <c r="G269">
+        <v>2.8691308691308688</v>
+      </c>
+      <c r="H269">
+        <v>0.3</v>
+      </c>
+      <c r="I269">
+        <v>0.1</v>
+      </c>
+      <c r="J269">
+        <v>4</v>
+      </c>
+      <c r="K269">
+        <v>4</v>
+      </c>
+      <c r="L269">
+        <v>2</v>
+      </c>
+      <c r="M269">
+        <v>0.36</v>
+      </c>
+      <c r="N269">
+        <v>1.5</v>
+      </c>
+      <c r="O269">
+        <v>0.46</v>
+      </c>
+      <c r="P269">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A270" s="1">
+        <v>42965.877905092595</v>
+      </c>
+      <c r="B270" t="s">
+        <v>17</v>
+      </c>
+      <c r="C270">
+        <v>0</v>
+      </c>
+      <c r="D270">
+        <v>1</v>
+      </c>
+      <c r="E270">
+        <v>5</v>
+      </c>
+      <c r="F270">
+        <v>17.493182495247378</v>
+      </c>
+      <c r="G270">
+        <v>3.0009990009990011</v>
+      </c>
+      <c r="H270">
+        <v>0.3</v>
+      </c>
+      <c r="I270">
+        <v>0.1</v>
+      </c>
+      <c r="J270">
+        <v>4</v>
+      </c>
+      <c r="K270">
+        <v>4</v>
+      </c>
+      <c r="L270">
+        <v>2</v>
+      </c>
+      <c r="M270">
+        <v>0.36</v>
+      </c>
+      <c r="N270">
+        <v>1.5</v>
+      </c>
+      <c r="O270">
+        <v>0.46</v>
+      </c>
+      <c r="P270">
+        <v>2.8888888888888888</v>
+      </c>
+    </row>
+    <row r="271" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A271" s="1">
+        <v>42965.889432870368</v>
+      </c>
+      <c r="B271" t="s">
+        <v>17</v>
+      </c>
+      <c r="C271">
+        <v>0</v>
+      </c>
+      <c r="D271">
+        <v>1</v>
+      </c>
+      <c r="E271">
+        <v>5</v>
+      </c>
+      <c r="F271">
+        <v>24.729763077670373</v>
+      </c>
+      <c r="G271">
+        <v>2.9990009990009989</v>
+      </c>
+      <c r="H271">
+        <v>0.3</v>
+      </c>
+      <c r="I271">
+        <v>0.1</v>
+      </c>
+      <c r="J271">
+        <v>4</v>
+      </c>
+      <c r="K271">
+        <v>4</v>
+      </c>
+      <c r="L271">
+        <v>2</v>
+      </c>
+      <c r="M271">
+        <v>0.36</v>
+      </c>
+      <c r="N271">
+        <v>1.5</v>
+      </c>
+      <c r="O271">
+        <v>0.46</v>
+      </c>
+      <c r="P271">
+        <v>2.8666777777777779</v>
+      </c>
+    </row>
+    <row r="272" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A272" s="1">
+        <v>42965.893136574072</v>
+      </c>
+      <c r="B272" t="s">
+        <v>17</v>
+      </c>
+      <c r="C272">
+        <v>1</v>
+      </c>
+      <c r="D272">
+        <v>1</v>
+      </c>
+      <c r="E272">
+        <v>5</v>
+      </c>
+      <c r="F272">
+        <v>20.468380543832438</v>
+      </c>
+      <c r="G272">
+        <v>2.7052947052947052</v>
+      </c>
+      <c r="H272">
+        <v>0.3</v>
+      </c>
+      <c r="I272">
+        <v>0.1</v>
+      </c>
+      <c r="J272">
+        <v>4</v>
+      </c>
+      <c r="K272">
+        <v>4</v>
+      </c>
+      <c r="L272">
+        <v>2</v>
+      </c>
+      <c r="M272">
+        <v>0.36</v>
+      </c>
+      <c r="N272">
+        <v>1.5</v>
+      </c>
+      <c r="O272">
+        <v>0.46</v>
+      </c>
+      <c r="P272">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A273" s="1">
+        <v>42965.897256944445</v>
+      </c>
+      <c r="B273" t="s">
+        <v>17</v>
+      </c>
+      <c r="C273">
+        <v>1</v>
+      </c>
+      <c r="D273">
+        <v>1</v>
+      </c>
+      <c r="E273">
+        <v>5</v>
+      </c>
+      <c r="F273">
+        <v>23.99596591103629</v>
+      </c>
+      <c r="G273">
+        <v>3.0389610389610389</v>
+      </c>
+      <c r="H273">
+        <v>0.3</v>
+      </c>
+      <c r="I273">
+        <v>0.1</v>
+      </c>
+      <c r="J273">
+        <v>4</v>
+      </c>
+      <c r="K273">
+        <v>4</v>
+      </c>
+      <c r="L273">
+        <v>2</v>
+      </c>
+      <c r="M273">
+        <v>0.36</v>
+      </c>
+      <c r="N273">
+        <v>1.5</v>
+      </c>
+      <c r="O273">
+        <v>0.46</v>
+      </c>
+      <c r="P273">
+        <v>3.7777777777777777</v>
+      </c>
+    </row>
+    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A274" s="1">
+        <v>42965.900081018517</v>
+      </c>
+      <c r="B274" t="s">
+        <v>17</v>
+      </c>
+      <c r="C274">
+        <v>1</v>
+      </c>
+      <c r="D274">
+        <v>1</v>
+      </c>
+      <c r="E274">
+        <v>5</v>
+      </c>
+      <c r="F274">
+        <v>25.029356980874635</v>
+      </c>
+      <c r="G274">
+        <v>3.0089910089910088</v>
+      </c>
+      <c r="H274">
+        <v>0.3</v>
+      </c>
+      <c r="I274">
+        <v>0.1</v>
+      </c>
+      <c r="J274">
+        <v>4</v>
+      </c>
+      <c r="K274">
+        <v>4</v>
+      </c>
+      <c r="L274">
+        <v>2</v>
+      </c>
+      <c r="M274">
+        <v>0.36</v>
+      </c>
+      <c r="N274">
+        <v>1.5</v>
+      </c>
+      <c r="O274">
+        <v>0.46</v>
+      </c>
+      <c r="P274">
+        <v>3.7555777777777775</v>
+      </c>
+    </row>
+    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A275" s="1">
+        <v>42965.90353009259</v>
+      </c>
+      <c r="B275" t="s">
+        <v>16</v>
+      </c>
+      <c r="C275">
+        <v>0</v>
+      </c>
+      <c r="D275">
+        <v>1</v>
+      </c>
+      <c r="E275">
+        <v>5</v>
+      </c>
+      <c r="F275">
+        <v>18.756539355166542</v>
+      </c>
+      <c r="G275">
+        <v>2.9930069930069929</v>
+      </c>
+      <c r="H275">
+        <v>0.3</v>
+      </c>
+      <c r="I275">
+        <v>0.1</v>
+      </c>
+      <c r="J275">
+        <v>4</v>
+      </c>
+      <c r="K275">
+        <v>4</v>
+      </c>
+      <c r="L275">
+        <v>2</v>
+      </c>
+      <c r="M275">
+        <v>0.36</v>
+      </c>
+      <c r="N275">
+        <v>1.5</v>
+      </c>
+      <c r="O275">
+        <v>0.46</v>
+      </c>
+      <c r="P275">
+        <v>2.7333333333333334</v>
+      </c>
+    </row>
+    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A276" s="1">
+        <v>42965.906099537038</v>
+      </c>
+      <c r="B276" t="s">
+        <v>16</v>
+      </c>
+      <c r="C276">
+        <v>0</v>
+      </c>
+      <c r="D276">
+        <v>1</v>
+      </c>
+      <c r="E276">
+        <v>5</v>
+      </c>
+      <c r="F276">
+        <v>17.572044822641839</v>
+      </c>
+      <c r="G276">
+        <v>3.0069930069930071</v>
+      </c>
+      <c r="H276">
+        <v>0.3</v>
+      </c>
+      <c r="I276">
+        <v>0.1</v>
+      </c>
+      <c r="J276">
+        <v>4</v>
+      </c>
+      <c r="K276">
+        <v>4</v>
+      </c>
+      <c r="L276">
+        <v>2</v>
+      </c>
+      <c r="M276">
+        <v>0.36</v>
+      </c>
+      <c r="N276">
+        <v>1.5</v>
+      </c>
+      <c r="O276">
+        <v>0.46</v>
+      </c>
+      <c r="P276">
+        <v>2.7555222222222224</v>
+      </c>
+    </row>
+    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A277" s="1">
+        <v>42965.909189814818</v>
+      </c>
+      <c r="B277" t="s">
+        <v>16</v>
+      </c>
+      <c r="C277">
+        <v>1</v>
+      </c>
+      <c r="D277">
+        <v>1</v>
+      </c>
+      <c r="E277">
+        <v>5</v>
+      </c>
+      <c r="F277">
+        <v>24.115578712732994</v>
+      </c>
+      <c r="G277">
+        <v>3.0109890109890114</v>
+      </c>
+      <c r="H277">
+        <v>0.3</v>
+      </c>
+      <c r="I277">
+        <v>0.1</v>
+      </c>
+      <c r="J277">
+        <v>4</v>
+      </c>
+      <c r="K277">
+        <v>4</v>
+      </c>
+      <c r="L277">
+        <v>2</v>
+      </c>
+      <c r="M277">
+        <v>0.36</v>
+      </c>
+      <c r="N277">
+        <v>1.5</v>
+      </c>
+      <c r="O277">
+        <v>0.46</v>
+      </c>
+      <c r="P277">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A278" s="1">
+        <v>42965.914571759262</v>
+      </c>
+      <c r="B278" t="s">
+        <v>16</v>
+      </c>
+      <c r="C278">
+        <v>1</v>
+      </c>
+      <c r="D278">
+        <v>1</v>
+      </c>
+      <c r="E278">
+        <v>5</v>
+      </c>
+      <c r="F278">
+        <v>17.710802827542135</v>
+      </c>
+      <c r="G278">
+        <v>2.9870129870129869</v>
+      </c>
+      <c r="H278">
+        <v>0.3</v>
+      </c>
+      <c r="I278">
+        <v>0.1</v>
+      </c>
+      <c r="J278">
+        <v>4</v>
+      </c>
+      <c r="K278">
+        <v>4</v>
+      </c>
+      <c r="L278">
+        <v>2</v>
+      </c>
+      <c r="M278">
+        <v>0.36</v>
+      </c>
+      <c r="N278">
+        <v>1.5</v>
+      </c>
+      <c r="O278">
+        <v>0.46</v>
+      </c>
+      <c r="P278">
+        <v>3.6833333333333336</v>
+      </c>
+    </row>
+    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A279" s="1">
+        <v>42965.943784722222</v>
+      </c>
+      <c r="B279" t="s">
+        <v>18</v>
+      </c>
+      <c r="C279">
+        <v>1</v>
+      </c>
+      <c r="D279">
+        <v>1</v>
+      </c>
+      <c r="E279">
+        <v>5</v>
+      </c>
+      <c r="F279">
+        <v>17.768846414390246</v>
+      </c>
+      <c r="G279">
+        <v>3.0009990009990011</v>
+      </c>
+      <c r="H279">
+        <v>0.3</v>
+      </c>
+      <c r="I279">
+        <v>0.1</v>
+      </c>
+      <c r="J279">
+        <v>4</v>
+      </c>
+      <c r="K279">
+        <v>4</v>
+      </c>
+      <c r="L279">
+        <v>2</v>
+      </c>
+      <c r="M279">
+        <v>0.36</v>
+      </c>
+      <c r="N279">
+        <v>1.5</v>
+      </c>
+      <c r="O279">
+        <v>0.46</v>
+      </c>
+      <c r="P279">
+        <v>3.6555555555555554</v>
+      </c>
+    </row>
+    <row r="280" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A280" s="1">
+        <v>42965.949050925927</v>
+      </c>
+      <c r="B280" t="s">
+        <v>18</v>
+      </c>
+      <c r="C280">
+        <v>0</v>
+      </c>
+      <c r="D280">
+        <v>1</v>
+      </c>
+      <c r="E280">
+        <v>5</v>
+      </c>
+      <c r="F280">
+        <v>18.210004937415142</v>
+      </c>
+      <c r="G280">
+        <v>3.0009990009990011</v>
+      </c>
+      <c r="H280">
+        <v>0.3</v>
+      </c>
+      <c r="I280">
+        <v>0.1</v>
+      </c>
+      <c r="J280">
+        <v>4</v>
+      </c>
+      <c r="K280">
+        <v>4</v>
+      </c>
+      <c r="L280">
+        <v>2</v>
+      </c>
+      <c r="M280">
+        <v>0.36</v>
+      </c>
+      <c r="N280">
+        <v>1.5</v>
+      </c>
+      <c r="O280">
+        <v>0.46</v>
+      </c>
+      <c r="P280">
+        <v>2.6527777777777777</v>
+      </c>
+    </row>
+    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A281" s="1">
+        <v>42965.954085648147</v>
+      </c>
+      <c r="B281" t="s">
+        <v>18</v>
+      </c>
+      <c r="C281">
+        <v>0</v>
+      </c>
+      <c r="D281">
+        <v>1</v>
+      </c>
+      <c r="E281">
+        <v>5</v>
+      </c>
+      <c r="F281">
+        <v>17.628824776800357</v>
+      </c>
+      <c r="G281">
+        <v>3.0009990009990011</v>
+      </c>
+      <c r="H281">
+        <v>0.3</v>
+      </c>
+      <c r="I281">
+        <v>0.1</v>
+      </c>
+      <c r="J281">
+        <v>4</v>
+      </c>
+      <c r="K281">
+        <v>4</v>
+      </c>
+      <c r="L281">
+        <v>2</v>
+      </c>
+      <c r="M281">
+        <v>0.36</v>
+      </c>
+      <c r="N281">
+        <v>1.5</v>
+      </c>
+      <c r="O281">
+        <v>0.46</v>
+      </c>
+      <c r="P281">
+        <v>2.6527777777777777</v>
+      </c>
+    </row>
+    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A282" s="1">
+        <v>42965.958136574074</v>
+      </c>
+      <c r="B282" t="s">
+        <v>19</v>
+      </c>
+      <c r="C282">
+        <v>1</v>
+      </c>
+      <c r="D282">
+        <v>1</v>
+      </c>
+      <c r="E282">
+        <v>5</v>
+      </c>
+      <c r="F282">
+        <v>17.726492480121543</v>
+      </c>
+      <c r="G282">
+        <v>3.0009990009990011</v>
+      </c>
+      <c r="H282">
+        <v>0.3</v>
+      </c>
+      <c r="I282">
+        <v>0.1</v>
+      </c>
+      <c r="J282">
+        <v>4</v>
+      </c>
+      <c r="K282">
+        <v>4</v>
+      </c>
+      <c r="L282">
+        <v>2</v>
+      </c>
+      <c r="M282">
+        <v>0.36</v>
+      </c>
+      <c r="N282">
+        <v>1.5</v>
+      </c>
+      <c r="O282">
+        <v>0.46</v>
+      </c>
+      <c r="P282">
+        <v>3.8221999999999996</v>
+      </c>
+    </row>
+    <row r="283" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A283" s="1">
+        <v>42965.961863425924</v>
+      </c>
+      <c r="B283" t="s">
+        <v>19</v>
+      </c>
+      <c r="C283">
+        <v>0</v>
+      </c>
+      <c r="D283">
+        <v>1</v>
+      </c>
+      <c r="E283">
+        <v>5</v>
+      </c>
+      <c r="F283">
+        <v>17.618587720075759</v>
+      </c>
+      <c r="G283">
+        <v>3.0009990009990011</v>
+      </c>
+      <c r="H283">
+        <v>0.3</v>
+      </c>
+      <c r="I283">
+        <v>0.1</v>
+      </c>
+      <c r="J283">
+        <v>4</v>
+      </c>
+      <c r="K283">
+        <v>4</v>
+      </c>
+      <c r="L283">
+        <v>2</v>
+      </c>
+      <c r="M283">
+        <v>0.36</v>
+      </c>
+      <c r="N283">
+        <v>1.5</v>
+      </c>
+      <c r="O283">
+        <v>0.46</v>
+      </c>
+      <c r="P283">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A284" s="1">
+        <v>42965.981724537036</v>
+      </c>
+      <c r="B284" t="s">
+        <v>19</v>
+      </c>
+      <c r="C284">
+        <v>0</v>
+      </c>
+      <c r="D284">
+        <v>1</v>
+      </c>
+      <c r="E284">
+        <v>5</v>
+      </c>
+      <c r="F284">
+        <v>18.705996287498998</v>
+      </c>
+      <c r="G284">
+        <v>3.1188811188811192</v>
+      </c>
+      <c r="H284">
+        <v>0.3</v>
+      </c>
+      <c r="I284">
+        <v>0.1</v>
+      </c>
+      <c r="J284">
+        <v>4</v>
+      </c>
+      <c r="K284">
+        <v>4</v>
+      </c>
+      <c r="L284">
+        <v>2</v>
+      </c>
+      <c r="M284">
+        <v>0.36</v>
+      </c>
+      <c r="N284">
+        <v>1.5</v>
+      </c>
+      <c r="O284">
+        <v>0.46</v>
+      </c>
+      <c r="P284">
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A285" s="1">
+        <v>42965.982222222221</v>
+      </c>
+      <c r="B285" t="s">
+        <v>17</v>
+      </c>
+      <c r="C285">
+        <v>1</v>
+      </c>
+      <c r="D285">
+        <v>1</v>
+      </c>
+      <c r="E285">
+        <v>5</v>
+      </c>
+      <c r="F285">
+        <v>18.159072444327684</v>
+      </c>
+      <c r="G285">
+        <v>10.001998001998002</v>
+      </c>
+      <c r="H285">
+        <v>0.3</v>
+      </c>
+      <c r="I285">
+        <v>0.1</v>
+      </c>
+      <c r="J285">
+        <v>4</v>
+      </c>
+      <c r="K285">
+        <v>4</v>
+      </c>
+      <c r="L285">
+        <v>2</v>
+      </c>
+      <c r="M285">
+        <v>0.36</v>
+      </c>
+      <c r="N285">
+        <v>1.5</v>
+      </c>
+      <c r="O285">
+        <v>0.46</v>
+      </c>
+      <c r="P285">
+        <v>6.2222</v>
+      </c>
+    </row>
+    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A286" s="1">
+        <v>42965.983946759261</v>
+      </c>
+      <c r="B286" t="s">
+        <v>18</v>
+      </c>
+      <c r="C286">
+        <v>0</v>
+      </c>
+      <c r="D286">
+        <v>1</v>
+      </c>
+      <c r="E286">
+        <v>5</v>
+      </c>
+      <c r="F286">
+        <v>17.822325052150049</v>
+      </c>
+      <c r="G286">
+        <v>2.9930069930069929</v>
+      </c>
+      <c r="H286">
+        <v>0.3</v>
+      </c>
+      <c r="I286">
+        <v>0.1</v>
+      </c>
+      <c r="J286">
+        <v>4</v>
+      </c>
+      <c r="K286">
+        <v>4</v>
+      </c>
+      <c r="L286">
+        <v>2</v>
+      </c>
+      <c r="M286">
+        <v>0.36</v>
+      </c>
+      <c r="N286">
+        <v>1.5</v>
+      </c>
+      <c r="O286">
+        <v>0.46</v>
+      </c>
+      <c r="P286">
+        <v>2.629</v>
+      </c>
+    </row>
+    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A287" s="1">
+        <v>42965.984189814815</v>
+      </c>
+      <c r="B287" t="s">
+        <v>19</v>
+      </c>
+      <c r="C287">
+        <v>0</v>
+      </c>
+      <c r="D287">
+        <v>1</v>
+      </c>
+      <c r="E287">
+        <v>5</v>
+      </c>
+      <c r="F287">
+        <v>19.639815085323207</v>
+      </c>
+      <c r="G287">
+        <v>3.0029970029970032</v>
+      </c>
+      <c r="H287">
+        <v>0.3</v>
+      </c>
+      <c r="I287">
+        <v>0.1</v>
+      </c>
+      <c r="J287">
+        <v>4</v>
+      </c>
+      <c r="K287">
+        <v>4</v>
+      </c>
+      <c r="L287">
+        <v>2</v>
+      </c>
+      <c r="M287">
+        <v>0.36</v>
+      </c>
+      <c r="N287">
+        <v>1.5</v>
+      </c>
+      <c r="O287">
+        <v>0.46</v>
+      </c>
+      <c r="P287">
+        <v>2.9056000000000002</v>
+      </c>
+    </row>
+    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A288" s="1">
+        <v>42965.984490740739</v>
+      </c>
+      <c r="B288" t="s">
+        <v>16</v>
+      </c>
+      <c r="C288">
+        <v>0</v>
+      </c>
+      <c r="D288">
+        <v>1</v>
+      </c>
+      <c r="E288">
+        <v>5</v>
+      </c>
+      <c r="F288">
+        <v>23.750183433132264</v>
+      </c>
+      <c r="G288">
+        <v>3.0069930069930071</v>
+      </c>
+      <c r="H288">
+        <v>0.3</v>
+      </c>
+      <c r="I288">
+        <v>0.1</v>
+      </c>
+      <c r="J288">
+        <v>4</v>
+      </c>
+      <c r="K288">
+        <v>4</v>
+      </c>
+      <c r="L288">
+        <v>2</v>
+      </c>
+      <c r="M288">
+        <v>0.36</v>
+      </c>
+      <c r="N288">
+        <v>1.5</v>
+      </c>
+      <c r="O288">
+        <v>0.46</v>
+      </c>
+      <c r="P288">
+        <v>2.7555000000000001</v>
+      </c>
+    </row>
+    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A289" s="1">
+        <v>42965.984780092593</v>
+      </c>
+      <c r="B289" t="s">
+        <v>17</v>
+      </c>
+      <c r="C289">
+        <v>0</v>
+      </c>
+      <c r="D289">
+        <v>1</v>
+      </c>
+      <c r="E289">
+        <v>5</v>
+      </c>
+      <c r="F289">
+        <v>23.612647462479003</v>
+      </c>
+      <c r="G289">
+        <v>2.9990009990009989</v>
+      </c>
+      <c r="H289">
+        <v>0.3</v>
+      </c>
+      <c r="I289">
+        <v>0.1</v>
+      </c>
+      <c r="J289">
+        <v>4</v>
+      </c>
+      <c r="K289">
+        <v>4</v>
+      </c>
+      <c r="L289">
+        <v>2</v>
+      </c>
+      <c r="M289">
+        <v>0.36</v>
+      </c>
+      <c r="N289">
+        <v>1.5</v>
+      </c>
+      <c r="O289">
+        <v>0.46</v>
+      </c>
+      <c r="P289">
+        <v>2.8666999999999998</v>
+      </c>
+    </row>
+    <row r="290" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A290" s="1">
+        <v>42965.985081018516</v>
+      </c>
+      <c r="B290" t="s">
+        <v>18</v>
+      </c>
+      <c r="C290">
+        <v>1</v>
+      </c>
+      <c r="D290">
+        <v>1</v>
+      </c>
+      <c r="E290">
+        <v>5</v>
+      </c>
+      <c r="F290">
+        <v>23.876882049536064</v>
+      </c>
+      <c r="G290">
+        <v>3.0009990009990011</v>
+      </c>
+      <c r="H290">
+        <v>0.3</v>
+      </c>
+      <c r="I290">
+        <v>0.1</v>
+      </c>
+      <c r="J290">
+        <v>4</v>
+      </c>
+      <c r="K290">
+        <v>4</v>
+      </c>
+      <c r="L290">
+        <v>2</v>
+      </c>
+      <c r="M290">
+        <v>0.36</v>
+      </c>
+      <c r="N290">
+        <v>1.5</v>
+      </c>
+      <c r="O290">
+        <v>0.46</v>
+      </c>
+      <c r="P290">
+        <v>3.6556000000000002</v>
+      </c>
+    </row>
+    <row r="291" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A291" s="1">
+        <v>42965.985381944447</v>
+      </c>
+      <c r="B291" t="s">
+        <v>19</v>
+      </c>
+      <c r="C291">
+        <v>1</v>
+      </c>
+      <c r="D291">
+        <v>1</v>
+      </c>
+      <c r="E291">
+        <v>5</v>
+      </c>
+      <c r="F291">
+        <v>23.820402884116017</v>
+      </c>
+      <c r="G291">
+        <v>3.0009990009990011</v>
+      </c>
+      <c r="H291">
+        <v>0.3</v>
+      </c>
+      <c r="I291">
+        <v>0.1</v>
+      </c>
+      <c r="J291">
+        <v>4</v>
+      </c>
+      <c r="K291">
+        <v>4</v>
+      </c>
+      <c r="L291">
+        <v>2</v>
+      </c>
+      <c r="M291">
+        <v>0.36</v>
+      </c>
+      <c r="N291">
+        <v>1.5</v>
+      </c>
+      <c r="O291">
+        <v>0.46</v>
+      </c>
+      <c r="P291">
+        <v>3.8222</v>
+      </c>
+    </row>
+    <row r="292" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A292" s="1">
+        <v>42965.985682870371</v>
+      </c>
+      <c r="B292" t="s">
+        <v>16</v>
+      </c>
+      <c r="C292">
+        <v>1</v>
+      </c>
+      <c r="D292">
+        <v>1</v>
+      </c>
+      <c r="E292">
+        <v>5</v>
+      </c>
+      <c r="F292">
+        <v>23.858484978322412</v>
+      </c>
+      <c r="G292">
+        <v>2.9950049950049951</v>
+      </c>
+      <c r="H292">
+        <v>0.3</v>
+      </c>
+      <c r="I292">
+        <v>0.1</v>
+      </c>
+      <c r="J292">
+        <v>4</v>
+      </c>
+      <c r="K292">
+        <v>4</v>
+      </c>
+      <c r="L292">
+        <v>2</v>
+      </c>
+      <c r="M292">
+        <v>0.36</v>
+      </c>
+      <c r="N292">
+        <v>1.5</v>
+      </c>
+      <c r="O292">
+        <v>0.46</v>
+      </c>
+      <c r="P292">
+        <v>3.6917</v>
+      </c>
+    </row>
+    <row r="293" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A293" s="1">
+        <v>42965.985983796294</v>
+      </c>
+      <c r="B293" t="s">
+        <v>17</v>
+      </c>
+      <c r="C293">
+        <v>1</v>
+      </c>
+      <c r="D293">
+        <v>1</v>
+      </c>
+      <c r="E293">
+        <v>5</v>
+      </c>
+      <c r="F293">
+        <v>23.838623321942826</v>
+      </c>
+      <c r="G293">
+        <v>3.0089910089910088</v>
+      </c>
+      <c r="H293">
+        <v>0.3</v>
+      </c>
+      <c r="I293">
+        <v>0.1</v>
+      </c>
+      <c r="J293">
+        <v>4</v>
+      </c>
+      <c r="K293">
+        <v>4</v>
+      </c>
+      <c r="L293">
+        <v>2</v>
+      </c>
+      <c r="M293">
+        <v>0.36</v>
+      </c>
+      <c r="N293">
+        <v>1.5</v>
+      </c>
+      <c r="O293">
+        <v>0.46</v>
+      </c>
+      <c r="P293">
+        <v>3.7555999999999998</v>
+      </c>
+    </row>
+    <row r="294" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A294" s="1">
+        <v>42965.986273148148</v>
+      </c>
+      <c r="B294" t="s">
+        <v>18</v>
+      </c>
+      <c r="C294">
+        <v>0</v>
+      </c>
+      <c r="D294">
+        <v>1</v>
+      </c>
+      <c r="E294">
+        <v>5</v>
+      </c>
+      <c r="F294">
+        <v>23.614624988440433</v>
+      </c>
+      <c r="G294">
+        <v>3.0049950049950049</v>
+      </c>
+      <c r="H294">
+        <v>0.3</v>
+      </c>
+      <c r="I294">
+        <v>0.1</v>
+      </c>
+      <c r="J294">
+        <v>4</v>
+      </c>
+      <c r="K294">
+        <v>4</v>
+      </c>
+      <c r="L294">
+        <v>2</v>
+      </c>
+      <c r="M294">
+        <v>0.36</v>
+      </c>
+      <c r="N294">
+        <v>1.5</v>
+      </c>
+      <c r="O294">
+        <v>0.46</v>
+      </c>
+      <c r="P294">
+        <v>2.629</v>
+      </c>
+    </row>
+    <row r="295" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A295" s="1">
+        <v>42965.986574074072</v>
+      </c>
+      <c r="B295" t="s">
+        <v>19</v>
+      </c>
+      <c r="C295">
+        <v>0</v>
+      </c>
+      <c r="D295">
+        <v>1</v>
+      </c>
+      <c r="E295">
+        <v>5</v>
+      </c>
+      <c r="F295">
+        <v>23.670726248009274</v>
+      </c>
+      <c r="G295">
+        <v>3.0149850149850153</v>
+      </c>
+      <c r="H295">
+        <v>0.3</v>
+      </c>
+      <c r="I295">
+        <v>0.1</v>
+      </c>
+      <c r="J295">
+        <v>4</v>
+      </c>
+      <c r="K295">
+        <v>4</v>
+      </c>
+      <c r="L295">
+        <v>2</v>
+      </c>
+      <c r="M295">
+        <v>0.36</v>
+      </c>
+      <c r="N295">
+        <v>1.5</v>
+      </c>
+      <c r="O295">
+        <v>0.46</v>
+      </c>
+      <c r="P295">
+        <v>2.9056000000000002</v>
+      </c>
+    </row>
+    <row r="296" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A296" s="1">
+        <v>42965.986863425926</v>
+      </c>
+      <c r="B296" t="s">
+        <v>16</v>
+      </c>
+      <c r="C296">
+        <v>0</v>
+      </c>
+      <c r="D296">
+        <v>1</v>
+      </c>
+      <c r="E296">
+        <v>5</v>
+      </c>
+      <c r="F296">
+        <v>23.503288996859958</v>
+      </c>
+      <c r="G296">
+        <v>3.0189810189810187</v>
+      </c>
+      <c r="H296">
+        <v>0.3</v>
+      </c>
+      <c r="I296">
+        <v>0.1</v>
+      </c>
+      <c r="J296">
+        <v>4</v>
+      </c>
+      <c r="K296">
+        <v>4</v>
+      </c>
+      <c r="L296">
+        <v>2</v>
+      </c>
+      <c r="M296">
+        <v>0.36</v>
+      </c>
+      <c r="N296">
+        <v>1.5</v>
+      </c>
+      <c r="O296">
+        <v>0.46</v>
+      </c>
+      <c r="P296">
+        <v>2.7555000000000001</v>
+      </c>
+    </row>
+    <row r="297" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A297" s="1">
+        <v>42965.987175925926</v>
+      </c>
+      <c r="B297" t="s">
+        <v>17</v>
+      </c>
+      <c r="C297">
+        <v>0</v>
+      </c>
+      <c r="D297">
+        <v>1</v>
+      </c>
+      <c r="E297">
+        <v>5</v>
+      </c>
+      <c r="F297">
+        <v>24.519888695367246</v>
+      </c>
+      <c r="G297">
+        <v>3.0029970029970032</v>
+      </c>
+      <c r="H297">
+        <v>0.3</v>
+      </c>
+      <c r="I297">
+        <v>0.1</v>
+      </c>
+      <c r="J297">
+        <v>4</v>
+      </c>
+      <c r="K297">
+        <v>4</v>
+      </c>
+      <c r="L297">
+        <v>2</v>
+      </c>
+      <c r="M297">
+        <v>0.36</v>
+      </c>
+      <c r="N297">
+        <v>1.5</v>
+      </c>
+      <c r="O297">
+        <v>0.46</v>
+      </c>
+      <c r="P297">
+        <v>2.8666999999999998</v>
+      </c>
+    </row>
+    <row r="298" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A298" s="1">
+        <v>42965.987476851849</v>
+      </c>
+      <c r="B298" t="s">
+        <v>18</v>
+      </c>
+      <c r="C298">
+        <v>1</v>
+      </c>
+      <c r="D298">
+        <v>1</v>
+      </c>
+      <c r="E298">
+        <v>5</v>
+      </c>
+      <c r="F298">
+        <v>24.424107641409904</v>
+      </c>
+      <c r="G298">
+        <v>3.0269730269730268</v>
+      </c>
+      <c r="H298">
+        <v>0.3</v>
+      </c>
+      <c r="I298">
+        <v>0.1</v>
+      </c>
+      <c r="J298">
+        <v>4</v>
+      </c>
+      <c r="K298">
+        <v>4</v>
+      </c>
+      <c r="L298">
+        <v>2</v>
+      </c>
+      <c r="M298">
+        <v>0.36</v>
+      </c>
+      <c r="N298">
+        <v>1.5</v>
+      </c>
+      <c r="O298">
+        <v>0.46</v>
+      </c>
+      <c r="P298">
+        <v>3.6556000000000002</v>
+      </c>
+    </row>
+    <row r="299" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A299" s="1">
+        <v>42965.98777777778</v>
+      </c>
+      <c r="B299" t="s">
+        <v>19</v>
+      </c>
+      <c r="C299">
+        <v>1</v>
+      </c>
+      <c r="D299">
+        <v>1</v>
+      </c>
+      <c r="E299">
+        <v>5</v>
+      </c>
+      <c r="F299">
+        <v>24.873157708975377</v>
+      </c>
+      <c r="G299">
+        <v>3.0189810189810187</v>
+      </c>
+      <c r="H299">
+        <v>0.3</v>
+      </c>
+      <c r="I299">
+        <v>0.1</v>
+      </c>
+      <c r="J299">
+        <v>4</v>
+      </c>
+      <c r="K299">
+        <v>4</v>
+      </c>
+      <c r="L299">
+        <v>2</v>
+      </c>
+      <c r="M299">
+        <v>0.36</v>
+      </c>
+      <c r="N299">
+        <v>1.5</v>
+      </c>
+      <c r="O299">
+        <v>0.46</v>
+      </c>
+      <c r="P299">
+        <v>3.8222</v>
+      </c>
+    </row>
+    <row r="300" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A300" s="1">
+        <v>42965.98809027778</v>
+      </c>
+      <c r="B300" t="s">
+        <v>16</v>
+      </c>
+      <c r="C300">
+        <v>1</v>
+      </c>
+      <c r="D300">
+        <v>1</v>
+      </c>
+      <c r="E300">
+        <v>5</v>
+      </c>
+      <c r="F300">
+        <v>24.956452190429989</v>
+      </c>
+      <c r="G300">
+        <v>3.034965034965035</v>
+      </c>
+      <c r="H300">
+        <v>0.3</v>
+      </c>
+      <c r="I300">
+        <v>0.1</v>
+      </c>
+      <c r="J300">
+        <v>4</v>
+      </c>
+      <c r="K300">
+        <v>4</v>
+      </c>
+      <c r="L300">
+        <v>2</v>
+      </c>
+      <c r="M300">
+        <v>0.36</v>
+      </c>
+      <c r="N300">
+        <v>1.5</v>
+      </c>
+      <c r="O300">
+        <v>0.46</v>
+      </c>
+      <c r="P300">
+        <v>3.6917</v>
+      </c>
+    </row>
+    <row r="301" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A301" s="1">
+        <v>42965.988391203704</v>
+      </c>
+      <c r="B301" t="s">
+        <v>17</v>
+      </c>
+      <c r="C301">
+        <v>1</v>
+      </c>
+      <c r="D301">
+        <v>1</v>
+      </c>
+      <c r="E301">
+        <v>5</v>
+      </c>
+      <c r="F301">
+        <v>24.874819726749429</v>
+      </c>
+      <c r="G301">
+        <v>3.0329670329670333</v>
+      </c>
+      <c r="H301">
+        <v>0.3</v>
+      </c>
+      <c r="I301">
+        <v>0.1</v>
+      </c>
+      <c r="J301">
+        <v>4</v>
+      </c>
+      <c r="K301">
+        <v>4</v>
+      </c>
+      <c r="L301">
+        <v>2</v>
+      </c>
+      <c r="M301">
+        <v>0.36</v>
+      </c>
+      <c r="N301">
+        <v>1.5</v>
+      </c>
+      <c r="O301">
+        <v>0.46</v>
+      </c>
+      <c r="P301">
+        <v>3.7555999999999998</v>
+      </c>
+    </row>
+    <row r="302" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A302" s="1">
+        <v>42966.384293981479</v>
+      </c>
+      <c r="B302" t="s">
+        <v>17</v>
+      </c>
+      <c r="C302">
+        <v>1</v>
+      </c>
+      <c r="D302">
+        <v>1</v>
+      </c>
+      <c r="E302">
+        <v>5</v>
+      </c>
+      <c r="F302">
+        <v>20.270601388684007</v>
+      </c>
+      <c r="G302">
+        <v>10.001998001998002</v>
+      </c>
+      <c r="H302">
+        <v>0.3</v>
+      </c>
+      <c r="I302">
+        <v>0.1</v>
+      </c>
+      <c r="J302">
+        <v>4</v>
+      </c>
+      <c r="K302">
+        <v>4</v>
+      </c>
+      <c r="L302">
+        <v>2</v>
+      </c>
+      <c r="M302">
+        <v>0.36</v>
+      </c>
+      <c r="N302">
+        <v>1.5</v>
+      </c>
+      <c r="O302">
+        <v>0.46</v>
+      </c>
+      <c r="P302">
+        <v>6.2222000000000008</v>
+      </c>
+    </row>
+    <row r="303" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A303" s="1">
+        <v>42966.387361111112</v>
+      </c>
+      <c r="B303" t="s">
+        <v>18</v>
+      </c>
+      <c r="C303">
+        <v>0</v>
+      </c>
+      <c r="D303">
+        <v>1</v>
+      </c>
+      <c r="E303">
+        <v>5</v>
+      </c>
+      <c r="F303">
+        <v>21.007846746217822</v>
+      </c>
+      <c r="G303">
+        <v>2.9970029970029968</v>
+      </c>
+      <c r="H303">
+        <v>0.3</v>
+      </c>
+      <c r="I303">
+        <v>0.1</v>
+      </c>
+      <c r="J303">
+        <v>4</v>
+      </c>
+      <c r="K303">
+        <v>4</v>
+      </c>
+      <c r="L303">
+        <v>2</v>
+      </c>
+      <c r="M303">
+        <v>0.36</v>
+      </c>
+      <c r="N303">
+        <v>1.5</v>
+      </c>
+      <c r="O303">
+        <v>0.46</v>
+      </c>
+      <c r="P303">
+        <v>2.6501111111111113</v>
+      </c>
+    </row>
+    <row r="304" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A304" s="1">
+        <v>42966.390115740738</v>
+      </c>
+      <c r="B304" t="s">
+        <v>17</v>
+      </c>
+      <c r="C304">
+        <v>0</v>
+      </c>
+      <c r="D304">
+        <v>1</v>
+      </c>
+      <c r="E304">
+        <v>5</v>
+      </c>
+      <c r="F304">
+        <v>19.48318286963336</v>
+      </c>
+      <c r="G304">
+        <v>2.8231768231768233</v>
+      </c>
+      <c r="H304">
+        <v>0.3</v>
+      </c>
+      <c r="I304">
+        <v>0.1</v>
+      </c>
+      <c r="J304">
+        <v>4</v>
+      </c>
+      <c r="K304">
+        <v>4</v>
+      </c>
+      <c r="L304">
+        <v>2</v>
+      </c>
+      <c r="M304">
+        <v>0.36</v>
+      </c>
+      <c r="N304">
+        <v>1.5</v>
+      </c>
+      <c r="O304">
+        <v>0.46</v>
+      </c>
+      <c r="P304">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="305" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A305" s="1">
+        <v>42966.392916666664</v>
+      </c>
+      <c r="B305" t="s">
+        <v>17</v>
+      </c>
+      <c r="C305">
+        <v>0</v>
+      </c>
+      <c r="D305">
+        <v>1</v>
+      </c>
+      <c r="E305">
+        <v>5</v>
+      </c>
+      <c r="F305">
+        <v>21.616883463883113</v>
+      </c>
+      <c r="G305">
+        <v>2.8231768231768233</v>
+      </c>
+      <c r="H305">
+        <v>0.3</v>
+      </c>
+      <c r="I305">
+        <v>0.1</v>
+      </c>
+      <c r="J305">
+        <v>4</v>
+      </c>
+      <c r="K305">
+        <v>4</v>
+      </c>
+      <c r="L305">
+        <v>2</v>
+      </c>
+      <c r="M305">
+        <v>0.36</v>
+      </c>
+      <c r="N305">
+        <v>1.5</v>
+      </c>
+      <c r="O305">
+        <v>0.46</v>
+      </c>
+      <c r="P305">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="306" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A306" s="1">
+        <v>42966.398981481485</v>
+      </c>
+      <c r="B306" t="s">
+        <v>17</v>
+      </c>
+      <c r="C306">
+        <v>0</v>
+      </c>
+      <c r="D306">
+        <v>1</v>
+      </c>
+      <c r="E306">
+        <v>7</v>
+      </c>
+      <c r="F306">
+        <v>17.07692415995945</v>
+      </c>
+      <c r="G306">
+        <v>1.8161838161838162</v>
+      </c>
+      <c r="H306">
+        <v>0.3</v>
+      </c>
+      <c r="I306">
+        <v>0.1</v>
+      </c>
+      <c r="J306">
+        <v>4</v>
+      </c>
+      <c r="K306">
+        <v>4</v>
+      </c>
+      <c r="L306">
+        <v>2</v>
+      </c>
+      <c r="M306">
+        <v>0.36</v>
+      </c>
+      <c r="N306">
+        <v>1.75</v>
+      </c>
+      <c r="O306">
+        <v>0.46</v>
+      </c>
+      <c r="P306">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="307" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A307" s="1">
+        <v>42966.401076388887</v>
+      </c>
+      <c r="B307" t="s">
+        <v>17</v>
+      </c>
+      <c r="C307">
+        <v>0</v>
+      </c>
+      <c r="D307">
+        <v>1</v>
+      </c>
+      <c r="E307">
+        <v>7</v>
+      </c>
+      <c r="F307">
+        <v>16.788356723924256</v>
+      </c>
+      <c r="G307">
+        <v>1.8601398601398602</v>
+      </c>
+      <c r="H307">
+        <v>0.3</v>
+      </c>
+      <c r="I307">
+        <v>0.1</v>
+      </c>
+      <c r="J307">
+        <v>4</v>
+      </c>
+      <c r="K307">
+        <v>4</v>
+      </c>
+      <c r="L307">
+        <v>2</v>
+      </c>
+      <c r="M307">
+        <v>0.36</v>
+      </c>
+      <c r="N307">
+        <v>1.9</v>
+      </c>
+      <c r="O307">
+        <v>0.46</v>
+      </c>
+      <c r="P307">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="308" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A308" s="1">
+        <v>42966.405532407407</v>
+      </c>
+      <c r="B308" t="s">
+        <v>17</v>
+      </c>
+      <c r="C308">
+        <v>0</v>
+      </c>
+      <c r="D308">
+        <v>1</v>
+      </c>
+      <c r="E308">
+        <v>7</v>
+      </c>
+      <c r="F308">
+        <v>16.200172345547383</v>
+      </c>
+      <c r="G308">
+        <v>1.9540459540459538</v>
+      </c>
+      <c r="H308">
+        <v>0.3</v>
+      </c>
+      <c r="I308">
+        <v>0.1</v>
+      </c>
+      <c r="J308">
+        <v>4</v>
+      </c>
+      <c r="K308">
+        <v>4</v>
+      </c>
+      <c r="L308">
+        <v>2</v>
+      </c>
+      <c r="M308">
+        <v>0.36</v>
+      </c>
+      <c r="N308">
+        <v>1.8499999999999999</v>
+      </c>
+      <c r="O308">
+        <v>0.46</v>
+      </c>
+      <c r="P308">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="309" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A309" s="1">
+        <v>42966.418564814812</v>
+      </c>
+      <c r="B309" t="s">
+        <v>17</v>
+      </c>
+      <c r="C309">
+        <v>0</v>
+      </c>
+      <c r="D309">
+        <v>1</v>
+      </c>
+      <c r="E309">
+        <v>7</v>
+      </c>
+      <c r="F309">
+        <v>17.097721781296507</v>
+      </c>
+      <c r="G309">
+        <v>1.9980019980019981</v>
+      </c>
+      <c r="H309">
+        <v>0.3</v>
+      </c>
+      <c r="I309">
+        <v>0.1</v>
+      </c>
+      <c r="J309">
+        <v>4</v>
+      </c>
+      <c r="K309">
+        <v>4</v>
+      </c>
+      <c r="L309">
+        <v>2</v>
+      </c>
+      <c r="M309">
+        <v>0.36</v>
+      </c>
+      <c r="N309">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="O309">
+        <v>0.5</v>
+      </c>
+      <c r="P309">
+        <v>3.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update psw calculations for new seed values
This updates constants for 3, 5, and 10% targets.  15% was NOT reachable without mix-and-match pMin values, which we decided to avoid.
</commit_message>
<xml_diff>
--- a/RunSummaries.xlsx
+++ b/RunSummaries.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -497,10 +497,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P511"/>
+  <dimension ref="A1:P552"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A481" workbookViewId="0">
-      <selection activeCell="A511" sqref="A511:P511"/>
+    <sheetView tabSelected="1" topLeftCell="A512" workbookViewId="0">
+      <selection activeCell="A552" sqref="A552:P552"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26055,6 +26055,2056 @@
         <v>4.7156000000000002</v>
       </c>
     </row>
+    <row r="512" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A512" s="1">
+        <v>42997.821562500001</v>
+      </c>
+      <c r="B512" t="s">
+        <v>17</v>
+      </c>
+      <c r="C512">
+        <v>1</v>
+      </c>
+      <c r="D512">
+        <v>1</v>
+      </c>
+      <c r="E512">
+        <v>6</v>
+      </c>
+      <c r="F512">
+        <v>23.25437290426505</v>
+      </c>
+      <c r="G512">
+        <v>4.0199800199800197</v>
+      </c>
+      <c r="H512">
+        <v>0.3</v>
+      </c>
+      <c r="I512">
+        <v>0.1</v>
+      </c>
+      <c r="J512">
+        <v>4</v>
+      </c>
+      <c r="K512">
+        <v>4</v>
+      </c>
+      <c r="L512">
+        <v>2</v>
+      </c>
+      <c r="M512">
+        <v>0.36</v>
+      </c>
+      <c r="N512">
+        <v>1.5</v>
+      </c>
+      <c r="O512">
+        <v>0.46</v>
+      </c>
+      <c r="P512">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="513" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A513" s="1">
+        <v>42997.827303240738</v>
+      </c>
+      <c r="B513" t="s">
+        <v>17</v>
+      </c>
+      <c r="C513">
+        <v>1</v>
+      </c>
+      <c r="D513">
+        <v>1</v>
+      </c>
+      <c r="E513">
+        <v>6</v>
+      </c>
+      <c r="F513">
+        <v>23.671478357311788</v>
+      </c>
+      <c r="G513">
+        <v>4.9350649350649345</v>
+      </c>
+      <c r="H513">
+        <v>0.3</v>
+      </c>
+      <c r="I513">
+        <v>0.1</v>
+      </c>
+      <c r="J513">
+        <v>4</v>
+      </c>
+      <c r="K513">
+        <v>4</v>
+      </c>
+      <c r="L513">
+        <v>2</v>
+      </c>
+      <c r="M513">
+        <v>0.36</v>
+      </c>
+      <c r="N513">
+        <v>1.5</v>
+      </c>
+      <c r="O513">
+        <v>0.46</v>
+      </c>
+      <c r="P513">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="514" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A514" s="1">
+        <v>42997.830787037034</v>
+      </c>
+      <c r="B514" t="s">
+        <v>17</v>
+      </c>
+      <c r="C514">
+        <v>1</v>
+      </c>
+      <c r="D514">
+        <v>1</v>
+      </c>
+      <c r="E514">
+        <v>6</v>
+      </c>
+      <c r="F514">
+        <v>23.359930587754555</v>
+      </c>
+      <c r="G514">
+        <v>5.0209790209790208</v>
+      </c>
+      <c r="H514">
+        <v>0.3</v>
+      </c>
+      <c r="I514">
+        <v>0.1</v>
+      </c>
+      <c r="J514">
+        <v>4</v>
+      </c>
+      <c r="K514">
+        <v>4</v>
+      </c>
+      <c r="L514">
+        <v>2</v>
+      </c>
+      <c r="M514">
+        <v>0.36</v>
+      </c>
+      <c r="N514">
+        <v>1.5</v>
+      </c>
+      <c r="O514">
+        <v>0.46</v>
+      </c>
+      <c r="P514">
+        <v>5.3277777777777775</v>
+      </c>
+    </row>
+    <row r="515" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A515" s="1">
+        <v>42997.834016203706</v>
+      </c>
+      <c r="B515" t="s">
+        <v>17</v>
+      </c>
+      <c r="C515">
+        <v>1</v>
+      </c>
+      <c r="D515">
+        <v>1</v>
+      </c>
+      <c r="E515">
+        <v>6</v>
+      </c>
+      <c r="F515">
+        <v>23.723335307672048</v>
+      </c>
+      <c r="G515">
+        <v>4.9970029970029977</v>
+      </c>
+      <c r="H515">
+        <v>0.3</v>
+      </c>
+      <c r="I515">
+        <v>0.1</v>
+      </c>
+      <c r="J515">
+        <v>4</v>
+      </c>
+      <c r="K515">
+        <v>4</v>
+      </c>
+      <c r="L515">
+        <v>2</v>
+      </c>
+      <c r="M515">
+        <v>0.36</v>
+      </c>
+      <c r="N515">
+        <v>1.5</v>
+      </c>
+      <c r="O515">
+        <v>0.46</v>
+      </c>
+      <c r="P515">
+        <v>5.322222222222222</v>
+      </c>
+    </row>
+    <row r="516" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A516" s="1">
+        <v>42997.837025462963</v>
+      </c>
+      <c r="B516" t="s">
+        <v>16</v>
+      </c>
+      <c r="C516">
+        <v>1</v>
+      </c>
+      <c r="D516">
+        <v>1</v>
+      </c>
+      <c r="E516">
+        <v>6</v>
+      </c>
+      <c r="F516">
+        <v>20.828367567470707</v>
+      </c>
+      <c r="G516">
+        <v>4.9730269730269736</v>
+      </c>
+      <c r="H516">
+        <v>0.3</v>
+      </c>
+      <c r="I516">
+        <v>0.1</v>
+      </c>
+      <c r="J516">
+        <v>4</v>
+      </c>
+      <c r="K516">
+        <v>4</v>
+      </c>
+      <c r="L516">
+        <v>2</v>
+      </c>
+      <c r="M516">
+        <v>0.36</v>
+      </c>
+      <c r="N516">
+        <v>1.5</v>
+      </c>
+      <c r="O516">
+        <v>0.46</v>
+      </c>
+      <c r="P516">
+        <v>5.3666666666666663</v>
+      </c>
+    </row>
+    <row r="517" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A517" s="1">
+        <v>42997.840497685182</v>
+      </c>
+      <c r="B517" t="s">
+        <v>16</v>
+      </c>
+      <c r="C517">
+        <v>1</v>
+      </c>
+      <c r="D517">
+        <v>1</v>
+      </c>
+      <c r="E517">
+        <v>6</v>
+      </c>
+      <c r="F517">
+        <v>17.513752373126337</v>
+      </c>
+      <c r="G517">
+        <v>4.9850149850149847</v>
+      </c>
+      <c r="H517">
+        <v>0.3</v>
+      </c>
+      <c r="I517">
+        <v>0.1</v>
+      </c>
+      <c r="J517">
+        <v>4</v>
+      </c>
+      <c r="K517">
+        <v>4</v>
+      </c>
+      <c r="L517">
+        <v>2</v>
+      </c>
+      <c r="M517">
+        <v>0.36</v>
+      </c>
+      <c r="N517">
+        <v>1.5</v>
+      </c>
+      <c r="O517">
+        <v>0.46</v>
+      </c>
+      <c r="P517">
+        <v>5.3699999999999992</v>
+      </c>
+    </row>
+    <row r="518" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A518" s="1">
+        <v>42997.844918981478</v>
+      </c>
+      <c r="B518" t="s">
+        <v>16</v>
+      </c>
+      <c r="C518">
+        <v>1</v>
+      </c>
+      <c r="D518">
+        <v>1</v>
+      </c>
+      <c r="E518">
+        <v>6</v>
+      </c>
+      <c r="F518">
+        <v>23.380630425231601</v>
+      </c>
+      <c r="G518">
+        <v>5.0029970029970023</v>
+      </c>
+      <c r="H518">
+        <v>0.3</v>
+      </c>
+      <c r="I518">
+        <v>0.1</v>
+      </c>
+      <c r="J518">
+        <v>4</v>
+      </c>
+      <c r="K518">
+        <v>4</v>
+      </c>
+      <c r="L518">
+        <v>2</v>
+      </c>
+      <c r="M518">
+        <v>0.36</v>
+      </c>
+      <c r="N518">
+        <v>1.5</v>
+      </c>
+      <c r="O518">
+        <v>0.46</v>
+      </c>
+      <c r="P518">
+        <v>5.3733333333333331</v>
+      </c>
+    </row>
+    <row r="519" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A519" s="1">
+        <v>42997.848749999997</v>
+      </c>
+      <c r="B519" t="s">
+        <v>19</v>
+      </c>
+      <c r="C519">
+        <v>1</v>
+      </c>
+      <c r="D519">
+        <v>1</v>
+      </c>
+      <c r="E519">
+        <v>6</v>
+      </c>
+      <c r="F519">
+        <v>23.855911672501687</v>
+      </c>
+      <c r="G519">
+        <v>4.977022977022977</v>
+      </c>
+      <c r="H519">
+        <v>0.3</v>
+      </c>
+      <c r="I519">
+        <v>0.1</v>
+      </c>
+      <c r="J519">
+        <v>4</v>
+      </c>
+      <c r="K519">
+        <v>4</v>
+      </c>
+      <c r="L519">
+        <v>2</v>
+      </c>
+      <c r="M519">
+        <v>0.36</v>
+      </c>
+      <c r="N519">
+        <v>1.5</v>
+      </c>
+      <c r="O519">
+        <v>0.46</v>
+      </c>
+      <c r="P519">
+        <v>5.427777777777778</v>
+      </c>
+    </row>
+    <row r="520" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A520" s="1">
+        <v>42997.851307870369</v>
+      </c>
+      <c r="B520" t="s">
+        <v>19</v>
+      </c>
+      <c r="C520">
+        <v>1</v>
+      </c>
+      <c r="D520">
+        <v>1</v>
+      </c>
+      <c r="E520">
+        <v>6</v>
+      </c>
+      <c r="F520">
+        <v>22.926220530114744</v>
+      </c>
+      <c r="G520">
+        <v>5.0069930069930075</v>
+      </c>
+      <c r="H520">
+        <v>0.3</v>
+      </c>
+      <c r="I520">
+        <v>0.1</v>
+      </c>
+      <c r="J520">
+        <v>4</v>
+      </c>
+      <c r="K520">
+        <v>4</v>
+      </c>
+      <c r="L520">
+        <v>2</v>
+      </c>
+      <c r="M520">
+        <v>0.36</v>
+      </c>
+      <c r="N520">
+        <v>1.5</v>
+      </c>
+      <c r="O520">
+        <v>0.46</v>
+      </c>
+      <c r="P520">
+        <v>5.4411111111111117</v>
+      </c>
+    </row>
+    <row r="521" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A521" s="1">
+        <v>42997.854027777779</v>
+      </c>
+      <c r="B521" t="s">
+        <v>18</v>
+      </c>
+      <c r="C521">
+        <v>1</v>
+      </c>
+      <c r="D521">
+        <v>1</v>
+      </c>
+      <c r="E521">
+        <v>6</v>
+      </c>
+      <c r="F521">
+        <v>17.07247679032043</v>
+      </c>
+      <c r="G521">
+        <v>5.0309690309690316</v>
+      </c>
+      <c r="H521">
+        <v>0.3</v>
+      </c>
+      <c r="I521">
+        <v>0.1</v>
+      </c>
+      <c r="J521">
+        <v>4</v>
+      </c>
+      <c r="K521">
+        <v>4</v>
+      </c>
+      <c r="L521">
+        <v>2</v>
+      </c>
+      <c r="M521">
+        <v>0.36</v>
+      </c>
+      <c r="N521">
+        <v>1.5</v>
+      </c>
+      <c r="O521">
+        <v>0.46</v>
+      </c>
+      <c r="P521">
+        <v>5.3422222222222224</v>
+      </c>
+    </row>
+    <row r="522" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A522" s="1">
+        <v>42997.858310185184</v>
+      </c>
+      <c r="B522" t="s">
+        <v>18</v>
+      </c>
+      <c r="C522">
+        <v>1</v>
+      </c>
+      <c r="D522">
+        <v>1</v>
+      </c>
+      <c r="E522">
+        <v>6</v>
+      </c>
+      <c r="F522">
+        <v>17.305446198949983</v>
+      </c>
+      <c r="G522">
+        <v>4.9890109890109891</v>
+      </c>
+      <c r="H522">
+        <v>0.3</v>
+      </c>
+      <c r="I522">
+        <v>0.1</v>
+      </c>
+      <c r="J522">
+        <v>4</v>
+      </c>
+      <c r="K522">
+        <v>4</v>
+      </c>
+      <c r="L522">
+        <v>2</v>
+      </c>
+      <c r="M522">
+        <v>0.36</v>
+      </c>
+      <c r="N522">
+        <v>1.5</v>
+      </c>
+      <c r="O522">
+        <v>0.46</v>
+      </c>
+      <c r="P522">
+        <v>5.3288888888888888</v>
+      </c>
+    </row>
+    <row r="523" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A523" s="1">
+        <v>42997.862314814818</v>
+      </c>
+      <c r="B523" t="s">
+        <v>16</v>
+      </c>
+      <c r="C523">
+        <v>1</v>
+      </c>
+      <c r="D523">
+        <v>1</v>
+      </c>
+      <c r="E523">
+        <v>6</v>
+      </c>
+      <c r="F523">
+        <v>16.961575912683671</v>
+      </c>
+      <c r="G523">
+        <v>5.0149850149850153</v>
+      </c>
+      <c r="H523">
+        <v>0.3</v>
+      </c>
+      <c r="I523">
+        <v>0.1</v>
+      </c>
+      <c r="J523">
+        <v>4</v>
+      </c>
+      <c r="K523">
+        <v>4</v>
+      </c>
+      <c r="L523">
+        <v>2</v>
+      </c>
+      <c r="M523">
+        <v>0.36</v>
+      </c>
+      <c r="N523">
+        <v>1.5</v>
+      </c>
+      <c r="O523">
+        <v>0.46</v>
+      </c>
+      <c r="P523">
+        <v>5.3755555555555556</v>
+      </c>
+    </row>
+    <row r="524" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A524" s="1">
+        <v>42997.884953703702</v>
+      </c>
+      <c r="B524" t="s">
+        <v>17</v>
+      </c>
+      <c r="C524">
+        <v>1</v>
+      </c>
+      <c r="D524">
+        <v>1</v>
+      </c>
+      <c r="E524">
+        <v>6</v>
+      </c>
+      <c r="F524">
+        <v>23.723781373826156</v>
+      </c>
+      <c r="G524">
+        <v>2.9970029970029968</v>
+      </c>
+      <c r="H524">
+        <v>0.3</v>
+      </c>
+      <c r="I524">
+        <v>0.1</v>
+      </c>
+      <c r="J524">
+        <v>4</v>
+      </c>
+      <c r="K524">
+        <v>4</v>
+      </c>
+      <c r="L524">
+        <v>2</v>
+      </c>
+      <c r="M524">
+        <v>0.36</v>
+      </c>
+      <c r="N524">
+        <v>1.5</v>
+      </c>
+      <c r="O524">
+        <v>0.46</v>
+      </c>
+      <c r="P524">
+        <v>4.293333333333333</v>
+      </c>
+    </row>
+    <row r="525" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A525" s="1">
+        <v>42997.887650462966</v>
+      </c>
+      <c r="B525" t="s">
+        <v>16</v>
+      </c>
+      <c r="C525">
+        <v>1</v>
+      </c>
+      <c r="D525">
+        <v>1</v>
+      </c>
+      <c r="E525">
+        <v>6</v>
+      </c>
+      <c r="F525">
+        <v>17.985750842293854</v>
+      </c>
+      <c r="G525">
+        <v>2.2837162837162839</v>
+      </c>
+      <c r="H525">
+        <v>0.3</v>
+      </c>
+      <c r="I525">
+        <v>0.1</v>
+      </c>
+      <c r="J525">
+        <v>4</v>
+      </c>
+      <c r="K525">
+        <v>4</v>
+      </c>
+      <c r="L525">
+        <v>2</v>
+      </c>
+      <c r="M525">
+        <v>0.36</v>
+      </c>
+      <c r="N525">
+        <v>1.5</v>
+      </c>
+      <c r="O525">
+        <v>0.46</v>
+      </c>
+      <c r="P525">
+        <v>3.6917</v>
+      </c>
+    </row>
+    <row r="526" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A526" s="1">
+        <v>42997.890590277777</v>
+      </c>
+      <c r="B526" t="s">
+        <v>16</v>
+      </c>
+      <c r="C526">
+        <v>1</v>
+      </c>
+      <c r="D526">
+        <v>1</v>
+      </c>
+      <c r="E526">
+        <v>6</v>
+      </c>
+      <c r="F526">
+        <v>18.37119263818051</v>
+      </c>
+      <c r="G526">
+        <v>3.0009990009990011</v>
+      </c>
+      <c r="H526">
+        <v>0.3</v>
+      </c>
+      <c r="I526">
+        <v>0.1</v>
+      </c>
+      <c r="J526">
+        <v>4</v>
+      </c>
+      <c r="K526">
+        <v>4</v>
+      </c>
+      <c r="L526">
+        <v>2</v>
+      </c>
+      <c r="M526">
+        <v>0.36</v>
+      </c>
+      <c r="N526">
+        <v>1.5</v>
+      </c>
+      <c r="O526">
+        <v>0.46</v>
+      </c>
+      <c r="P526">
+        <v>4.3533333333333335</v>
+      </c>
+    </row>
+    <row r="527" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A527" s="1">
+        <v>42997.89439814815</v>
+      </c>
+      <c r="B527" t="s">
+        <v>19</v>
+      </c>
+      <c r="C527">
+        <v>1</v>
+      </c>
+      <c r="D527">
+        <v>1</v>
+      </c>
+      <c r="E527">
+        <v>6</v>
+      </c>
+      <c r="F527">
+        <v>23.835267513296387</v>
+      </c>
+      <c r="G527">
+        <v>2.9930069930069929</v>
+      </c>
+      <c r="H527">
+        <v>0.3</v>
+      </c>
+      <c r="I527">
+        <v>0.1</v>
+      </c>
+      <c r="J527">
+        <v>4</v>
+      </c>
+      <c r="K527">
+        <v>4</v>
+      </c>
+      <c r="L527">
+        <v>2</v>
+      </c>
+      <c r="M527">
+        <v>0.36</v>
+      </c>
+      <c r="N527">
+        <v>1.5</v>
+      </c>
+      <c r="O527">
+        <v>0.46</v>
+      </c>
+      <c r="P527">
+        <v>4.4422222222222221</v>
+      </c>
+    </row>
+    <row r="528" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A528" s="1">
+        <v>42997.897407407407</v>
+      </c>
+      <c r="B528" t="s">
+        <v>18</v>
+      </c>
+      <c r="C528">
+        <v>1</v>
+      </c>
+      <c r="D528">
+        <v>1</v>
+      </c>
+      <c r="E528">
+        <v>6</v>
+      </c>
+      <c r="F528">
+        <v>23.794490219023601</v>
+      </c>
+      <c r="G528">
+        <v>3.0129870129870131</v>
+      </c>
+      <c r="H528">
+        <v>0.3</v>
+      </c>
+      <c r="I528">
+        <v>0.1</v>
+      </c>
+      <c r="J528">
+        <v>4</v>
+      </c>
+      <c r="K528">
+        <v>4</v>
+      </c>
+      <c r="L528">
+        <v>2</v>
+      </c>
+      <c r="M528">
+        <v>0.36</v>
+      </c>
+      <c r="N528">
+        <v>1.5</v>
+      </c>
+      <c r="O528">
+        <v>0.46</v>
+      </c>
+      <c r="P528">
+        <v>4.2822222222222219</v>
+      </c>
+    </row>
+    <row r="529" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A529" s="1">
+        <v>42997.901122685187</v>
+      </c>
+      <c r="B529" t="s">
+        <v>18</v>
+      </c>
+      <c r="C529">
+        <v>1</v>
+      </c>
+      <c r="D529">
+        <v>1</v>
+      </c>
+      <c r="E529">
+        <v>6</v>
+      </c>
+      <c r="F529">
+        <v>17.842280095625831</v>
+      </c>
+      <c r="G529">
+        <v>2.9930069930069929</v>
+      </c>
+      <c r="H529">
+        <v>0.3</v>
+      </c>
+      <c r="I529">
+        <v>0.1</v>
+      </c>
+      <c r="J529">
+        <v>4</v>
+      </c>
+      <c r="K529">
+        <v>4</v>
+      </c>
+      <c r="L529">
+        <v>2</v>
+      </c>
+      <c r="M529">
+        <v>0.36</v>
+      </c>
+      <c r="N529">
+        <v>1.5</v>
+      </c>
+      <c r="O529">
+        <v>0.46</v>
+      </c>
+      <c r="P529">
+        <v>4.2711111111111117</v>
+      </c>
+    </row>
+    <row r="530" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A530" s="1">
+        <v>42997.908854166664</v>
+      </c>
+      <c r="B530" t="s">
+        <v>17</v>
+      </c>
+      <c r="C530">
+        <v>1</v>
+      </c>
+      <c r="D530">
+        <v>1</v>
+      </c>
+      <c r="E530">
+        <v>6</v>
+      </c>
+      <c r="F530">
+        <v>17.31121018003601</v>
+      </c>
+      <c r="G530">
+        <v>13.416583416583418</v>
+      </c>
+      <c r="H530">
+        <v>0.3</v>
+      </c>
+      <c r="I530">
+        <v>0.1</v>
+      </c>
+      <c r="J530">
+        <v>4</v>
+      </c>
+      <c r="K530">
+        <v>4</v>
+      </c>
+      <c r="L530">
+        <v>2</v>
+      </c>
+      <c r="M530">
+        <v>0.36</v>
+      </c>
+      <c r="N530">
+        <v>1.5</v>
+      </c>
+      <c r="O530">
+        <v>0.46</v>
+      </c>
+      <c r="P530">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="531" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A531" s="1">
+        <v>42997.913240740738</v>
+      </c>
+      <c r="B531" t="s">
+        <v>17</v>
+      </c>
+      <c r="C531">
+        <v>1</v>
+      </c>
+      <c r="D531">
+        <v>1</v>
+      </c>
+      <c r="E531">
+        <v>6</v>
+      </c>
+      <c r="F531">
+        <v>25.21320970197085</v>
+      </c>
+      <c r="G531">
+        <v>14.035964035964035</v>
+      </c>
+      <c r="H531">
+        <v>0.3</v>
+      </c>
+      <c r="I531">
+        <v>0.1</v>
+      </c>
+      <c r="J531">
+        <v>4</v>
+      </c>
+      <c r="K531">
+        <v>4</v>
+      </c>
+      <c r="L531">
+        <v>2</v>
+      </c>
+      <c r="M531">
+        <v>0.36</v>
+      </c>
+      <c r="N531">
+        <v>1.5</v>
+      </c>
+      <c r="O531">
+        <v>0.46</v>
+      </c>
+      <c r="P531">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="532" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A532" s="1">
+        <v>42997.916041666664</v>
+      </c>
+      <c r="B532" t="s">
+        <v>17</v>
+      </c>
+      <c r="C532">
+        <v>1</v>
+      </c>
+      <c r="D532">
+        <v>1</v>
+      </c>
+      <c r="E532">
+        <v>6</v>
+      </c>
+      <c r="F532">
+        <v>25.936665005918215</v>
+      </c>
+      <c r="G532">
+        <v>14.705294705294705</v>
+      </c>
+      <c r="H532">
+        <v>0.3</v>
+      </c>
+      <c r="I532">
+        <v>0.1</v>
+      </c>
+      <c r="J532">
+        <v>4</v>
+      </c>
+      <c r="K532">
+        <v>4</v>
+      </c>
+      <c r="L532">
+        <v>2</v>
+      </c>
+      <c r="M532">
+        <v>0.36</v>
+      </c>
+      <c r="N532">
+        <v>1.5</v>
+      </c>
+      <c r="O532">
+        <v>0.46</v>
+      </c>
+      <c r="P532">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="533" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A533" s="1">
+        <v>42997.919699074075</v>
+      </c>
+      <c r="B533" t="s">
+        <v>17</v>
+      </c>
+      <c r="C533">
+        <v>1</v>
+      </c>
+      <c r="D533">
+        <v>1</v>
+      </c>
+      <c r="E533">
+        <v>6</v>
+      </c>
+      <c r="F533">
+        <v>17.392404459765569</v>
+      </c>
+      <c r="G533">
+        <v>14.853146853146853</v>
+      </c>
+      <c r="H533">
+        <v>0.3</v>
+      </c>
+      <c r="I533">
+        <v>0.1</v>
+      </c>
+      <c r="J533">
+        <v>4</v>
+      </c>
+      <c r="K533">
+        <v>4</v>
+      </c>
+      <c r="L533">
+        <v>2</v>
+      </c>
+      <c r="M533">
+        <v>0.36</v>
+      </c>
+      <c r="N533">
+        <v>1.5</v>
+      </c>
+      <c r="O533">
+        <v>0.46</v>
+      </c>
+      <c r="P533">
+        <v>10.241666666666665</v>
+      </c>
+    </row>
+    <row r="534" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A534" s="1">
+        <v>42997.93041666667</v>
+      </c>
+      <c r="B534" t="s">
+        <v>17</v>
+      </c>
+      <c r="C534">
+        <v>1</v>
+      </c>
+      <c r="D534">
+        <v>1</v>
+      </c>
+      <c r="E534">
+        <v>6</v>
+      </c>
+      <c r="F534">
+        <v>18.363106809164645</v>
+      </c>
+      <c r="G534">
+        <v>14.86113886113886</v>
+      </c>
+      <c r="H534">
+        <v>0.3</v>
+      </c>
+      <c r="I534">
+        <v>0.1</v>
+      </c>
+      <c r="J534">
+        <v>4</v>
+      </c>
+      <c r="K534">
+        <v>4</v>
+      </c>
+      <c r="L534">
+        <v>2</v>
+      </c>
+      <c r="M534">
+        <v>0.36</v>
+      </c>
+      <c r="N534">
+        <v>1.5</v>
+      </c>
+      <c r="O534">
+        <v>0.46</v>
+      </c>
+      <c r="P534">
+        <v>10.295555555555556</v>
+      </c>
+    </row>
+    <row r="535" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A535" s="1">
+        <v>42997.939293981479</v>
+      </c>
+      <c r="B535" t="s">
+        <v>17</v>
+      </c>
+      <c r="C535">
+        <v>1</v>
+      </c>
+      <c r="D535">
+        <v>1</v>
+      </c>
+      <c r="E535">
+        <v>6</v>
+      </c>
+      <c r="F535">
+        <v>19.223795293394094</v>
+      </c>
+      <c r="G535">
+        <v>14.837162837162838</v>
+      </c>
+      <c r="H535">
+        <v>0.3</v>
+      </c>
+      <c r="I535">
+        <v>0.1</v>
+      </c>
+      <c r="J535">
+        <v>4</v>
+      </c>
+      <c r="K535">
+        <v>4</v>
+      </c>
+      <c r="L535">
+        <v>2</v>
+      </c>
+      <c r="M535">
+        <v>0.36</v>
+      </c>
+      <c r="N535">
+        <v>1.5</v>
+      </c>
+      <c r="O535">
+        <v>0.46</v>
+      </c>
+      <c r="P535">
+        <v>10.888888888888889</v>
+      </c>
+    </row>
+    <row r="536" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A536" s="1">
+        <v>42997.948009259257</v>
+      </c>
+      <c r="B536" t="s">
+        <v>17</v>
+      </c>
+      <c r="C536">
+        <v>1</v>
+      </c>
+      <c r="D536">
+        <v>1</v>
+      </c>
+      <c r="E536">
+        <v>6</v>
+      </c>
+      <c r="F536">
+        <v>17.154198733671308</v>
+      </c>
+      <c r="G536">
+        <v>15.002997002997004</v>
+      </c>
+      <c r="H536">
+        <v>0.3</v>
+      </c>
+      <c r="I536">
+        <v>0.1</v>
+      </c>
+      <c r="J536">
+        <v>4</v>
+      </c>
+      <c r="K536">
+        <v>4</v>
+      </c>
+      <c r="L536">
+        <v>2</v>
+      </c>
+      <c r="M536">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="N536">
+        <v>1.5</v>
+      </c>
+      <c r="O536">
+        <v>0.46</v>
+      </c>
+      <c r="P536">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="537" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A537" s="1">
+        <v>42997.951608796298</v>
+      </c>
+      <c r="B537" t="s">
+        <v>17</v>
+      </c>
+      <c r="C537">
+        <v>1</v>
+      </c>
+      <c r="D537">
+        <v>5</v>
+      </c>
+      <c r="E537">
+        <v>6</v>
+      </c>
+      <c r="F537">
+        <v>5.9348282629307185</v>
+      </c>
+      <c r="G537">
+        <v>14.975024975024976</v>
+      </c>
+      <c r="H537">
+        <v>0.3</v>
+      </c>
+      <c r="I537">
+        <v>0.1</v>
+      </c>
+      <c r="J537">
+        <v>4</v>
+      </c>
+      <c r="K537">
+        <v>4</v>
+      </c>
+      <c r="L537">
+        <v>2</v>
+      </c>
+      <c r="M537">
+        <v>0.45</v>
+      </c>
+      <c r="N537">
+        <v>1.5</v>
+      </c>
+      <c r="O537">
+        <v>0.46</v>
+      </c>
+      <c r="P537">
+        <v>9.8888888888888893</v>
+      </c>
+    </row>
+    <row r="538" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A538" s="1">
+        <v>42997.955358796295</v>
+      </c>
+      <c r="B538" t="s">
+        <v>18</v>
+      </c>
+      <c r="C538">
+        <v>1</v>
+      </c>
+      <c r="D538">
+        <v>5</v>
+      </c>
+      <c r="E538">
+        <v>6</v>
+      </c>
+      <c r="F538">
+        <v>5.737666382835477</v>
+      </c>
+      <c r="G538">
+        <v>14.975024975024976</v>
+      </c>
+      <c r="H538">
+        <v>0.3</v>
+      </c>
+      <c r="I538">
+        <v>0.1</v>
+      </c>
+      <c r="J538">
+        <v>4</v>
+      </c>
+      <c r="K538">
+        <v>4</v>
+      </c>
+      <c r="L538">
+        <v>2</v>
+      </c>
+      <c r="M538">
+        <v>0.36</v>
+      </c>
+      <c r="N538">
+        <v>1.5</v>
+      </c>
+      <c r="O538">
+        <v>0.46</v>
+      </c>
+      <c r="P538">
+        <v>9.8888888888888893</v>
+      </c>
+    </row>
+    <row r="539" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A539" s="1">
+        <v>42997.95815972222</v>
+      </c>
+      <c r="B539" t="s">
+        <v>18</v>
+      </c>
+      <c r="C539">
+        <v>1</v>
+      </c>
+      <c r="D539">
+        <v>5</v>
+      </c>
+      <c r="E539">
+        <v>6</v>
+      </c>
+      <c r="F539">
+        <v>5.66450097388977</v>
+      </c>
+      <c r="G539">
+        <v>14.975024975024976</v>
+      </c>
+      <c r="H539">
+        <v>0.3</v>
+      </c>
+      <c r="I539">
+        <v>0.1</v>
+      </c>
+      <c r="J539">
+        <v>4</v>
+      </c>
+      <c r="K539">
+        <v>4</v>
+      </c>
+      <c r="L539">
+        <v>2</v>
+      </c>
+      <c r="M539">
+        <v>0.36</v>
+      </c>
+      <c r="N539">
+        <v>1.5</v>
+      </c>
+      <c r="O539">
+        <v>0.46</v>
+      </c>
+      <c r="P539">
+        <v>10.011111111111111</v>
+      </c>
+    </row>
+    <row r="540" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A540" s="1">
+        <v>42997.961145833331</v>
+      </c>
+      <c r="B540" t="s">
+        <v>18</v>
+      </c>
+      <c r="C540">
+        <v>1</v>
+      </c>
+      <c r="D540">
+        <v>5</v>
+      </c>
+      <c r="E540">
+        <v>6</v>
+      </c>
+      <c r="F540">
+        <v>5.7565355571363064</v>
+      </c>
+      <c r="G540">
+        <v>14.995004995004994</v>
+      </c>
+      <c r="H540">
+        <v>0.3</v>
+      </c>
+      <c r="I540">
+        <v>0.1</v>
+      </c>
+      <c r="J540">
+        <v>4</v>
+      </c>
+      <c r="K540">
+        <v>4</v>
+      </c>
+      <c r="L540">
+        <v>2</v>
+      </c>
+      <c r="M540">
+        <v>0.36333333333333334</v>
+      </c>
+      <c r="N540">
+        <v>1.5</v>
+      </c>
+      <c r="O540">
+        <v>0.46</v>
+      </c>
+      <c r="P540">
+        <v>10.011111111111111</v>
+      </c>
+    </row>
+    <row r="541" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A541" s="1">
+        <v>42997.966747685183</v>
+      </c>
+      <c r="B541" t="s">
+        <v>18</v>
+      </c>
+      <c r="C541">
+        <v>1</v>
+      </c>
+      <c r="D541">
+        <v>5</v>
+      </c>
+      <c r="E541">
+        <v>6</v>
+      </c>
+      <c r="F541">
+        <v>5.5943377117574267</v>
+      </c>
+      <c r="G541">
+        <v>15.284715284715285</v>
+      </c>
+      <c r="H541">
+        <v>0.3</v>
+      </c>
+      <c r="I541">
+        <v>0.1</v>
+      </c>
+      <c r="J541">
+        <v>4</v>
+      </c>
+      <c r="K541">
+        <v>4</v>
+      </c>
+      <c r="L541">
+        <v>2</v>
+      </c>
+      <c r="M541">
+        <v>0.39</v>
+      </c>
+      <c r="N541">
+        <v>1.5</v>
+      </c>
+      <c r="O541">
+        <v>0.46</v>
+      </c>
+      <c r="P541">
+        <v>9.5111111111111111</v>
+      </c>
+    </row>
+    <row r="542" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A542" s="1">
+        <v>42997.971921296295</v>
+      </c>
+      <c r="B542" t="s">
+        <v>17</v>
+      </c>
+      <c r="C542">
+        <v>1</v>
+      </c>
+      <c r="D542">
+        <v>5</v>
+      </c>
+      <c r="E542">
+        <v>6</v>
+      </c>
+      <c r="F542">
+        <v>5.5840276317823099</v>
+      </c>
+      <c r="G542">
+        <v>9.1208791208791204</v>
+      </c>
+      <c r="H542">
+        <v>0.3</v>
+      </c>
+      <c r="I542">
+        <v>0.1</v>
+      </c>
+      <c r="J542">
+        <v>4</v>
+      </c>
+      <c r="K542">
+        <v>4</v>
+      </c>
+      <c r="L542">
+        <v>2</v>
+      </c>
+      <c r="M542">
+        <v>0.36</v>
+      </c>
+      <c r="N542">
+        <v>1.5</v>
+      </c>
+      <c r="O542">
+        <v>0.46</v>
+      </c>
+      <c r="P542">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="543" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A543" s="1">
+        <v>42997.973900462966</v>
+      </c>
+      <c r="B543" t="s">
+        <v>17</v>
+      </c>
+      <c r="C543">
+        <v>1</v>
+      </c>
+      <c r="D543">
+        <v>5</v>
+      </c>
+      <c r="E543">
+        <v>6</v>
+      </c>
+      <c r="F543">
+        <v>7.4379464061435536</v>
+      </c>
+      <c r="G543">
+        <v>10.04995004995005</v>
+      </c>
+      <c r="H543">
+        <v>0.3</v>
+      </c>
+      <c r="I543">
+        <v>0.1</v>
+      </c>
+      <c r="J543">
+        <v>4</v>
+      </c>
+      <c r="K543">
+        <v>4</v>
+      </c>
+      <c r="L543">
+        <v>2</v>
+      </c>
+      <c r="M543">
+        <v>0.36</v>
+      </c>
+      <c r="N543">
+        <v>1.5</v>
+      </c>
+      <c r="O543">
+        <v>0.46</v>
+      </c>
+      <c r="P543">
+        <v>7.1333333333333337</v>
+      </c>
+    </row>
+    <row r="544" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A544" s="1">
+        <v>42997.976215277777</v>
+      </c>
+      <c r="B544" t="s">
+        <v>16</v>
+      </c>
+      <c r="C544">
+        <v>1</v>
+      </c>
+      <c r="D544">
+        <v>5</v>
+      </c>
+      <c r="E544">
+        <v>6</v>
+      </c>
+      <c r="F544">
+        <v>7.0682839604658669</v>
+      </c>
+      <c r="G544">
+        <v>10</v>
+      </c>
+      <c r="H544">
+        <v>0.3</v>
+      </c>
+      <c r="I544">
+        <v>0.1</v>
+      </c>
+      <c r="J544">
+        <v>4</v>
+      </c>
+      <c r="K544">
+        <v>4</v>
+      </c>
+      <c r="L544">
+        <v>2</v>
+      </c>
+      <c r="M544">
+        <v>0.36</v>
+      </c>
+      <c r="N544">
+        <v>1.5</v>
+      </c>
+      <c r="O544">
+        <v>0.46</v>
+      </c>
+      <c r="P544">
+        <v>7.1477777777777778</v>
+      </c>
+    </row>
+    <row r="545" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A545" s="1">
+        <v>42997.977881944447</v>
+      </c>
+      <c r="B545" t="s">
+        <v>19</v>
+      </c>
+      <c r="C545">
+        <v>1</v>
+      </c>
+      <c r="D545">
+        <v>5</v>
+      </c>
+      <c r="E545">
+        <v>6</v>
+      </c>
+      <c r="F545">
+        <v>5.8498117018447751</v>
+      </c>
+      <c r="G545">
+        <v>9.9900099900099892</v>
+      </c>
+      <c r="H545">
+        <v>0.3</v>
+      </c>
+      <c r="I545">
+        <v>0.1</v>
+      </c>
+      <c r="J545">
+        <v>4</v>
+      </c>
+      <c r="K545">
+        <v>4</v>
+      </c>
+      <c r="L545">
+        <v>2</v>
+      </c>
+      <c r="M545">
+        <v>0.36</v>
+      </c>
+      <c r="N545">
+        <v>1.5</v>
+      </c>
+      <c r="O545">
+        <v>0.46</v>
+      </c>
+      <c r="P545">
+        <v>7.1555555555555559</v>
+      </c>
+    </row>
+    <row r="546" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A546" s="1">
+        <v>42997.979803240742</v>
+      </c>
+      <c r="B546" t="s">
+        <v>18</v>
+      </c>
+      <c r="C546">
+        <v>1</v>
+      </c>
+      <c r="D546">
+        <v>5</v>
+      </c>
+      <c r="E546">
+        <v>6</v>
+      </c>
+      <c r="F546">
+        <v>5.4847459134868455</v>
+      </c>
+      <c r="G546">
+        <v>9.9600399600399605</v>
+      </c>
+      <c r="H546">
+        <v>0.3</v>
+      </c>
+      <c r="I546">
+        <v>0.1</v>
+      </c>
+      <c r="J546">
+        <v>4</v>
+      </c>
+      <c r="K546">
+        <v>4</v>
+      </c>
+      <c r="L546">
+        <v>2</v>
+      </c>
+      <c r="M546">
+        <v>0.36</v>
+      </c>
+      <c r="N546">
+        <v>1.5</v>
+      </c>
+      <c r="O546">
+        <v>0.46</v>
+      </c>
+      <c r="P546">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="547" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A547" s="1">
+        <v>42997.984467592592</v>
+      </c>
+      <c r="B547" t="s">
+        <v>18</v>
+      </c>
+      <c r="C547">
+        <v>1</v>
+      </c>
+      <c r="D547">
+        <v>1</v>
+      </c>
+      <c r="E547">
+        <v>6</v>
+      </c>
+      <c r="F547">
+        <v>23.688048082987503</v>
+      </c>
+      <c r="G547">
+        <v>10.415584415584416</v>
+      </c>
+      <c r="H547">
+        <v>0.3</v>
+      </c>
+      <c r="I547">
+        <v>0.1</v>
+      </c>
+      <c r="J547">
+        <v>4</v>
+      </c>
+      <c r="K547">
+        <v>4</v>
+      </c>
+      <c r="L547">
+        <v>2</v>
+      </c>
+      <c r="M547">
+        <v>0.36</v>
+      </c>
+      <c r="N547">
+        <v>1.5</v>
+      </c>
+      <c r="O547">
+        <v>0.46</v>
+      </c>
+      <c r="P547">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="548" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A548" s="1">
+        <v>42997.986921296295</v>
+      </c>
+      <c r="B548" t="s">
+        <v>18</v>
+      </c>
+      <c r="C548">
+        <v>1</v>
+      </c>
+      <c r="D548">
+        <v>1</v>
+      </c>
+      <c r="E548">
+        <v>6</v>
+      </c>
+      <c r="F548">
+        <v>24.699746919855606</v>
+      </c>
+      <c r="G548">
+        <v>10.08991008991009</v>
+      </c>
+      <c r="H548">
+        <v>0.3</v>
+      </c>
+      <c r="I548">
+        <v>0.1</v>
+      </c>
+      <c r="J548">
+        <v>4</v>
+      </c>
+      <c r="K548">
+        <v>4</v>
+      </c>
+      <c r="L548">
+        <v>2</v>
+      </c>
+      <c r="M548">
+        <v>0.36</v>
+      </c>
+      <c r="N548">
+        <v>1.5</v>
+      </c>
+      <c r="O548">
+        <v>0.46</v>
+      </c>
+      <c r="P548">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="549" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A549" s="1">
+        <v>42997.990937499999</v>
+      </c>
+      <c r="B549" t="s">
+        <v>18</v>
+      </c>
+      <c r="C549">
+        <v>1</v>
+      </c>
+      <c r="D549">
+        <v>1</v>
+      </c>
+      <c r="E549">
+        <v>6</v>
+      </c>
+      <c r="F549">
+        <v>23.855003220700031</v>
+      </c>
+      <c r="G549">
+        <v>10.007992007992007</v>
+      </c>
+      <c r="H549">
+        <v>0.3</v>
+      </c>
+      <c r="I549">
+        <v>0.1</v>
+      </c>
+      <c r="J549">
+        <v>4</v>
+      </c>
+      <c r="K549">
+        <v>4</v>
+      </c>
+      <c r="L549">
+        <v>2</v>
+      </c>
+      <c r="M549">
+        <v>0.36</v>
+      </c>
+      <c r="N549">
+        <v>1.5</v>
+      </c>
+      <c r="O549">
+        <v>0.46</v>
+      </c>
+      <c r="P549">
+        <v>7.0777777777777775</v>
+      </c>
+    </row>
+    <row r="550" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A550" s="1">
+        <v>42997.994710648149</v>
+      </c>
+      <c r="B550" t="s">
+        <v>19</v>
+      </c>
+      <c r="C550">
+        <v>1</v>
+      </c>
+      <c r="D550">
+        <v>1</v>
+      </c>
+      <c r="E550">
+        <v>6</v>
+      </c>
+      <c r="F550">
+        <v>26.103752299528622</v>
+      </c>
+      <c r="G550">
+        <v>10.029970029970031</v>
+      </c>
+      <c r="H550">
+        <v>0.3</v>
+      </c>
+      <c r="I550">
+        <v>0.1</v>
+      </c>
+      <c r="J550">
+        <v>4</v>
+      </c>
+      <c r="K550">
+        <v>4</v>
+      </c>
+      <c r="L550">
+        <v>2</v>
+      </c>
+      <c r="M550">
+        <v>0.36</v>
+      </c>
+      <c r="N550">
+        <v>1.5</v>
+      </c>
+      <c r="O550">
+        <v>0.46</v>
+      </c>
+      <c r="P550">
+        <v>7.16</v>
+      </c>
+    </row>
+    <row r="551" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A551" s="1">
+        <v>42997.997731481482</v>
+      </c>
+      <c r="B551" t="s">
+        <v>16</v>
+      </c>
+      <c r="C551">
+        <v>1</v>
+      </c>
+      <c r="D551">
+        <v>1</v>
+      </c>
+      <c r="E551">
+        <v>6</v>
+      </c>
+      <c r="F551">
+        <v>26.989697599786503</v>
+      </c>
+      <c r="G551">
+        <v>9.9960039960039957</v>
+      </c>
+      <c r="H551">
+        <v>0.3</v>
+      </c>
+      <c r="I551">
+        <v>0.1</v>
+      </c>
+      <c r="J551">
+        <v>4</v>
+      </c>
+      <c r="K551">
+        <v>4</v>
+      </c>
+      <c r="L551">
+        <v>2</v>
+      </c>
+      <c r="M551">
+        <v>0.36</v>
+      </c>
+      <c r="N551">
+        <v>1.5</v>
+      </c>
+      <c r="O551">
+        <v>0.46</v>
+      </c>
+      <c r="P551">
+        <v>7.1388888888888884</v>
+      </c>
+    </row>
+    <row r="552" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A552" s="1">
+        <v>42998.000416666669</v>
+      </c>
+      <c r="B552" t="s">
+        <v>17</v>
+      </c>
+      <c r="C552">
+        <v>1</v>
+      </c>
+      <c r="D552">
+        <v>1</v>
+      </c>
+      <c r="E552">
+        <v>6</v>
+      </c>
+      <c r="F552">
+        <v>28.408314685912149</v>
+      </c>
+      <c r="G552">
+        <v>9.9980019980019978</v>
+      </c>
+      <c r="H552">
+        <v>0.3</v>
+      </c>
+      <c r="I552">
+        <v>0.1</v>
+      </c>
+      <c r="J552">
+        <v>4</v>
+      </c>
+      <c r="K552">
+        <v>4</v>
+      </c>
+      <c r="L552">
+        <v>2</v>
+      </c>
+      <c r="M552">
+        <v>0.36</v>
+      </c>
+      <c r="N552">
+        <v>1.5</v>
+      </c>
+      <c r="O552">
+        <v>0.46</v>
+      </c>
+      <c r="P552">
+        <v>7.1188888888888888</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Small type and updated run list
</commit_message>
<xml_diff>
--- a/RunSummaries.xlsx
+++ b/RunSummaries.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -506,10 +506,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P894"/>
+  <dimension ref="A1:P895"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A863" workbookViewId="0">
-      <selection activeCell="A894" sqref="A894:P894"/>
+      <selection activeCell="A895" sqref="A895:P895"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45214,6 +45214,56 @@
         <v>5.4410999999999996</v>
       </c>
     </row>
+    <row r="895" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A895" s="1">
+        <v>43075.789756944447</v>
+      </c>
+      <c r="B895" t="s">
+        <v>19</v>
+      </c>
+      <c r="C895">
+        <v>1</v>
+      </c>
+      <c r="D895">
+        <v>10</v>
+      </c>
+      <c r="E895">
+        <v>5</v>
+      </c>
+      <c r="F895">
+        <v>58.157460851178477</v>
+      </c>
+      <c r="G895">
+        <v>4.8969072164948448</v>
+      </c>
+      <c r="H895">
+        <v>0.3</v>
+      </c>
+      <c r="I895">
+        <v>0.1</v>
+      </c>
+      <c r="J895">
+        <v>4</v>
+      </c>
+      <c r="K895">
+        <v>4</v>
+      </c>
+      <c r="L895">
+        <v>2</v>
+      </c>
+      <c r="M895">
+        <v>0.36</v>
+      </c>
+      <c r="N895">
+        <v>1.5</v>
+      </c>
+      <c r="O895">
+        <v>0.46</v>
+      </c>
+      <c r="P895">
+        <v>5.4410999999999996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Small type and updated run list"
This reverts commit 7901dcc82e84e6e75cf9729bd6a019c166ab2764.
</commit_message>
<xml_diff>
--- a/RunSummaries.xlsx
+++ b/RunSummaries.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -506,10 +506,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P895"/>
+  <dimension ref="A1:P894"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A863" workbookViewId="0">
-      <selection activeCell="A895" sqref="A895:P895"/>
+      <selection activeCell="A894" sqref="A894:P894"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45214,56 +45214,6 @@
         <v>5.4410999999999996</v>
       </c>
     </row>
-    <row r="895" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A895" s="1">
-        <v>43075.789756944447</v>
-      </c>
-      <c r="B895" t="s">
-        <v>19</v>
-      </c>
-      <c r="C895">
-        <v>1</v>
-      </c>
-      <c r="D895">
-        <v>10</v>
-      </c>
-      <c r="E895">
-        <v>5</v>
-      </c>
-      <c r="F895">
-        <v>58.157460851178477</v>
-      </c>
-      <c r="G895">
-        <v>4.8969072164948448</v>
-      </c>
-      <c r="H895">
-        <v>0.3</v>
-      </c>
-      <c r="I895">
-        <v>0.1</v>
-      </c>
-      <c r="J895">
-        <v>4</v>
-      </c>
-      <c r="K895">
-        <v>4</v>
-      </c>
-      <c r="L895">
-        <v>2</v>
-      </c>
-      <c r="M895">
-        <v>0.36</v>
-      </c>
-      <c r="N895">
-        <v>1.5</v>
-      </c>
-      <c r="O895">
-        <v>0.46</v>
-      </c>
-      <c r="P895">
-        <v>5.4410999999999996</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>